<commit_message>
Include walking and cycling
</commit_message>
<xml_diff>
--- a/VT_IE_SUP.xlsx
+++ b/VT_IE_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF1D956-5C0E-4A2B-B624-71EDF0FE1289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7857BC-0B38-42E8-9738-327DE3ACCC7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONVENTIONS" sheetId="20" r:id="rId1"/>
@@ -790,7 +790,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="514">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -2413,6 +2413,18 @@
   </si>
   <si>
     <t>I/E rule</t>
+  </si>
+  <si>
+    <t>CYC</t>
+  </si>
+  <si>
+    <t>WLK</t>
+  </si>
+  <si>
+    <t>Cycling</t>
+  </si>
+  <si>
+    <t>Walking</t>
   </si>
 </sst>
 </file>
@@ -5907,6 +5919,24 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5965,24 +5995,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6844,10 +6856,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E428973-03EE-47B5-B88E-68B51CDC4391}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:T92"/>
+  <dimension ref="B2:T94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7130,11 +7142,11 @@
         <v>IMPCOABIT</v>
       </c>
       <c r="F13" s="294" t="str">
-        <f t="shared" ref="F13:F44" si="1">G13 &amp; " of " &amp; VLOOKUP(H13,$B$13:$C$90,2,FALSE) &amp; IF(J13&lt;&gt;0,IF(VLOOKUP(J13,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J13,$I$4:$J$10,2,FALSE),""),"")</f>
+        <f>G13 &amp; " of " &amp; VLOOKUP(H13,$B$13:$C$91,2,FALSE) &amp; IF(J13&lt;&gt;0,IF(VLOOKUP(J13,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J13,$I$4:$J$10,2,FALSE),""),"")</f>
         <v xml:space="preserve">Import of Bituminous Coal </v>
       </c>
       <c r="G13" s="296" t="str">
-        <f t="shared" ref="G13:G44" si="2">VLOOKUP(I13,$E$4:$F$9,2,FALSE)</f>
+        <f t="shared" ref="G13:G44" si="1">VLOOKUP(I13,$E$4:$F$9,2,FALSE)</f>
         <v>Import</v>
       </c>
       <c r="H13" s="296" t="str">
@@ -7142,7 +7154,7 @@
         <v>COABIT</v>
       </c>
       <c r="I13" s="296" t="str">
-        <f t="shared" ref="I13:I43" si="3">$E$5</f>
+        <f t="shared" ref="I13:I43" si="2">$E$5</f>
         <v>IMP</v>
       </c>
       <c r="J13" s="297"/>
@@ -7168,11 +7180,11 @@
         <v>IMPCOAHAR</v>
       </c>
       <c r="F14" s="294" t="str">
+        <f t="shared" ref="F14:F77" si="3">G14 &amp; " of " &amp; VLOOKUP(H14,$B$13:$C$91,2,FALSE) &amp; IF(J14&lt;&gt;0,IF(VLOOKUP(J14,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J14,$I$4:$J$10,2,FALSE),""),"")</f>
+        <v xml:space="preserve">Import of Hard Coal / Antracite </v>
+      </c>
+      <c r="G14" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Hard Coal / Antracite </v>
-      </c>
-      <c r="G14" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H14" s="296" t="str">
@@ -7180,7 +7192,7 @@
         <v>COAHAR</v>
       </c>
       <c r="I14" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J14" s="297"/>
@@ -7206,11 +7218,11 @@
         <v>IMPCOACOK</v>
       </c>
       <c r="F15" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Coke Coal </v>
+      </c>
+      <c r="G15" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Coke Coal </v>
-      </c>
-      <c r="G15" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H15" s="296" t="str">
@@ -7218,7 +7230,7 @@
         <v>COACOK</v>
       </c>
       <c r="I15" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J15" s="297"/>
@@ -7244,11 +7256,11 @@
         <v>IMPCOALIG</v>
       </c>
       <c r="F16" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Lignite /  Brown Coal </v>
+      </c>
+      <c r="G16" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Lignite /  Brown Coal </v>
-      </c>
-      <c r="G16" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H16" s="296" t="str">
@@ -7256,7 +7268,7 @@
         <v>COALIG</v>
       </c>
       <c r="I16" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J16" s="297"/>
@@ -7286,11 +7298,11 @@
         <v>IMPOILCRD</v>
       </c>
       <c r="F17" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Crude Oil </v>
+      </c>
+      <c r="G17" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Crude Oil </v>
-      </c>
-      <c r="G17" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H17" s="296" t="str">
@@ -7324,11 +7336,11 @@
         <v>IMPOILKER</v>
       </c>
       <c r="F18" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Kerosene </v>
+      </c>
+      <c r="G18" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Kerosene </v>
-      </c>
-      <c r="G18" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H18" s="296" t="str">
@@ -7362,11 +7374,11 @@
         <v>IMPOILHFO</v>
       </c>
       <c r="F19" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Heavy Fuel Oil </v>
+      </c>
+      <c r="G19" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Heavy Fuel Oil </v>
-      </c>
-      <c r="G19" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H19" s="296" t="str">
@@ -7400,11 +7412,11 @@
         <v>IMPOILDST</v>
       </c>
       <c r="F20" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Diesel Oil </v>
+      </c>
+      <c r="G20" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Diesel Oil </v>
-      </c>
-      <c r="G20" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H20" s="296" t="str">
@@ -7438,11 +7450,11 @@
         <v>IMPOILLPG</v>
       </c>
       <c r="F21" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Liquified Petroleum Gas </v>
+      </c>
+      <c r="G21" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Liquified Petroleum Gas </v>
-      </c>
-      <c r="G21" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H21" s="296" t="str">
@@ -7476,11 +7488,11 @@
         <v>IMPOILGSL</v>
       </c>
       <c r="F22" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Gasoline </v>
+      </c>
+      <c r="G22" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Gasoline </v>
-      </c>
-      <c r="G22" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H22" s="296" t="str">
@@ -7514,11 +7526,11 @@
         <v>IMPOILCOK</v>
       </c>
       <c r="F23" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Petroleum Coke </v>
+      </c>
+      <c r="G23" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Petroleum Coke </v>
-      </c>
-      <c r="G23" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H23" s="296" t="str">
@@ -7547,11 +7559,11 @@
         <v>IMPOILNEU</v>
       </c>
       <c r="F24" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Oil for Non-Energy uses</v>
+      </c>
+      <c r="G24" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Oil for Non-Energy uses</v>
-      </c>
-      <c r="G24" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H24" s="296" t="str">
@@ -7579,11 +7591,11 @@
         <v>IMPGASNAT_UK</v>
       </c>
       <c r="F25" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Natural Gas  - UK</v>
+      </c>
+      <c r="G25" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Natural Gas  - UK</v>
-      </c>
-      <c r="G25" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H25" s="296" t="str">
@@ -7591,7 +7603,7 @@
         <v>GASNAT</v>
       </c>
       <c r="I25" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J25" s="296" t="str">
@@ -7614,11 +7626,11 @@
         <v>IMPGASLNG_GLOBAL</v>
       </c>
       <c r="F26" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Import of Liquified Natural Gas </v>
+      </c>
+      <c r="G26" s="296" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Import of Liquified Natural Gas </v>
-      </c>
-      <c r="G26" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H26" s="296" t="str">
@@ -7626,7 +7638,7 @@
         <v>GASLNG</v>
       </c>
       <c r="I26" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J26" s="296" t="str">
@@ -7649,11 +7661,11 @@
         <v>IMPNUCURM</v>
       </c>
       <c r="F27" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Uranium</v>
+      </c>
+      <c r="G27" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Uranium</v>
-      </c>
-      <c r="G27" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H27" s="296" t="str">
@@ -7661,7 +7673,7 @@
         <v>NUCURM</v>
       </c>
       <c r="I27" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J27" s="296"/>
@@ -7681,11 +7693,11 @@
         <v>IMPBIOETH1G_S1</v>
       </c>
       <c r="F28" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Ethanol 1st generation  - Step 1</v>
+      </c>
+      <c r="G28" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Ethanol 1st generation  - Step 1</v>
-      </c>
-      <c r="G28" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H28" s="296" t="str">
@@ -7693,7 +7705,7 @@
         <v>BIOETH1G</v>
       </c>
       <c r="I28" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J28" s="296" t="str">
@@ -7716,11 +7728,11 @@
         <v>IMPBIOETH1G_S2</v>
       </c>
       <c r="F29" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Ethanol 1st generation  - Step 2</v>
+      </c>
+      <c r="G29" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Ethanol 1st generation  - Step 2</v>
-      </c>
-      <c r="G29" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H29" s="296" t="str">
@@ -7728,7 +7740,7 @@
         <v>BIOETH1G</v>
       </c>
       <c r="I29" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J29" s="296" t="str">
@@ -7751,11 +7763,11 @@
         <v>IMPBIOETH1G_S3</v>
       </c>
       <c r="F30" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Ethanol 1st generation  - Step 3</v>
+      </c>
+      <c r="G30" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Ethanol 1st generation  - Step 3</v>
-      </c>
-      <c r="G30" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H30" s="296" t="str">
@@ -7763,7 +7775,7 @@
         <v>BIOETH1G</v>
       </c>
       <c r="I30" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J30" s="296" t="str">
@@ -7786,11 +7798,11 @@
         <v>IMPBIOETH1G_S4</v>
       </c>
       <c r="F31" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Ethanol 1st generation  - Step 4</v>
+      </c>
+      <c r="G31" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Ethanol 1st generation  - Step 4</v>
-      </c>
-      <c r="G31" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H31" s="296" t="str">
@@ -7798,7 +7810,7 @@
         <v>BIOETH1G</v>
       </c>
       <c r="I31" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J31" s="296" t="str">
@@ -7821,11 +7833,11 @@
         <v>IMPBIODST1G_S1</v>
       </c>
       <c r="F32" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Biodiesel 1st generation  - Step 1</v>
+      </c>
+      <c r="G32" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Biodiesel 1st generation  - Step 1</v>
-      </c>
-      <c r="G32" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H32" s="296" t="str">
@@ -7833,7 +7845,7 @@
         <v>BIODST1G</v>
       </c>
       <c r="I32" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J32" s="296" t="str">
@@ -7856,11 +7868,11 @@
         <v>IMPBIODST1G_S2</v>
       </c>
       <c r="F33" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Biodiesel 1st generation  - Step 2</v>
+      </c>
+      <c r="G33" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Biodiesel 1st generation  - Step 2</v>
-      </c>
-      <c r="G33" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H33" s="296" t="str">
@@ -7868,7 +7880,7 @@
         <v>BIODST1G</v>
       </c>
       <c r="I33" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J33" s="296" t="str">
@@ -7891,11 +7903,11 @@
         <v>IMPBIODST1G_S3</v>
       </c>
       <c r="F34" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Biodiesel 1st generation  - Step 3</v>
+      </c>
+      <c r="G34" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Biodiesel 1st generation  - Step 3</v>
-      </c>
-      <c r="G34" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H34" s="296" t="str">
@@ -7903,7 +7915,7 @@
         <v>BIODST1G</v>
       </c>
       <c r="I34" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J34" s="296" t="str">
@@ -7926,11 +7938,11 @@
         <v>IMPBIODST1G_S4</v>
       </c>
       <c r="F35" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Biodiesel 1st generation  - Step 4</v>
+      </c>
+      <c r="G35" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Biodiesel 1st generation  - Step 4</v>
-      </c>
-      <c r="G35" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H35" s="296" t="str">
@@ -7938,7 +7950,7 @@
         <v>BIODST1G</v>
       </c>
       <c r="I35" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J35" s="296" t="str">
@@ -7961,11 +7973,11 @@
         <v>IMPBIOWPE_S1</v>
       </c>
       <c r="F36" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Pellets  - Step 1</v>
+      </c>
+      <c r="G36" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Pellets  - Step 1</v>
-      </c>
-      <c r="G36" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H36" s="296" t="str">
@@ -7973,7 +7985,7 @@
         <v>BIOWPE</v>
       </c>
       <c r="I36" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J36" s="296" t="str">
@@ -7996,11 +8008,11 @@
         <v>IMPBIOWPE_S2</v>
       </c>
       <c r="F37" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Pellets  - Step 2</v>
+      </c>
+      <c r="G37" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Pellets  - Step 2</v>
-      </c>
-      <c r="G37" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H37" s="296" t="str">
@@ -8008,7 +8020,7 @@
         <v>BIOWPE</v>
       </c>
       <c r="I37" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J37" s="296" t="str">
@@ -8031,11 +8043,11 @@
         <v>IMPBIOWPE_S3</v>
       </c>
       <c r="F38" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Pellets  - Step 3</v>
+      </c>
+      <c r="G38" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Pellets  - Step 3</v>
-      </c>
-      <c r="G38" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H38" s="296" t="str">
@@ -8043,7 +8055,7 @@
         <v>BIOWPE</v>
       </c>
       <c r="I38" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J38" s="296" t="str">
@@ -8066,11 +8078,11 @@
         <v>IMPBIOWPE_S4</v>
       </c>
       <c r="F39" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Pellets  - Step 4</v>
+      </c>
+      <c r="G39" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Pellets  - Step 4</v>
-      </c>
-      <c r="G39" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H39" s="296" t="str">
@@ -8078,7 +8090,7 @@
         <v>BIOWPE</v>
       </c>
       <c r="I39" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J39" s="296" t="str">
@@ -8101,11 +8113,11 @@
         <v>IMPBIOWCH_S1</v>
       </c>
       <c r="F40" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Chip  - Step 1</v>
+      </c>
+      <c r="G40" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Chip  - Step 1</v>
-      </c>
-      <c r="G40" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H40" s="296" t="str">
@@ -8113,7 +8125,7 @@
         <v>BIOWCH</v>
       </c>
       <c r="I40" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J40" s="296" t="str">
@@ -8136,11 +8148,11 @@
         <v>IMPBIOWCH_S2</v>
       </c>
       <c r="F41" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Chip  - Step 2</v>
+      </c>
+      <c r="G41" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Chip  - Step 2</v>
-      </c>
-      <c r="G41" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H41" s="296" t="str">
@@ -8148,7 +8160,7 @@
         <v>BIOWCH</v>
       </c>
       <c r="I41" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J41" s="296" t="str">
@@ -8171,11 +8183,11 @@
         <v>IMPBIOWCH_S3</v>
       </c>
       <c r="F42" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Chip  - Step 3</v>
+      </c>
+      <c r="G42" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Chip  - Step 3</v>
-      </c>
-      <c r="G42" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H42" s="296" t="str">
@@ -8183,7 +8195,7 @@
         <v>BIOWCH</v>
       </c>
       <c r="I42" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J42" s="296" t="str">
@@ -8206,11 +8218,11 @@
         <v>IMPBIOWCH_S4</v>
       </c>
       <c r="F43" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Import of Wood Chip  - Step 4</v>
+      </c>
+      <c r="G43" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Import of Wood Chip  - Step 4</v>
-      </c>
-      <c r="G43" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Import</v>
       </c>
       <c r="H43" s="296" t="str">
@@ -8218,7 +8230,7 @@
         <v>BIOWCH</v>
       </c>
       <c r="I43" s="296" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>IMP</v>
       </c>
       <c r="J43" s="296" t="str">
@@ -8241,11 +8253,11 @@
         <v>MINGASNAT_S1</v>
       </c>
       <c r="F44" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Natural Gas  - Step 1</v>
+      </c>
+      <c r="G44" s="296" t="str">
         <f t="shared" si="1"/>
-        <v>Domestic Potential of Natural Gas  - Step 1</v>
-      </c>
-      <c r="G44" s="296" t="str">
-        <f t="shared" si="2"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H44" s="296" t="str">
@@ -8284,11 +8296,11 @@
         <v>MINGASNAT_S2</v>
       </c>
       <c r="F45" s="294" t="str">
-        <f t="shared" ref="F45:F76" si="11">G45 &amp; " of " &amp; VLOOKUP(H45,$B$13:$C$90,2,FALSE) &amp; IF(J45&lt;&gt;0,IF(VLOOKUP(J45,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J45,$I$4:$J$10,2,FALSE),""),"")</f>
+        <f t="shared" si="3"/>
         <v>Domestic Potential of Natural Gas  - Step 2</v>
       </c>
       <c r="G45" s="296" t="str">
-        <f t="shared" ref="G45:G76" si="12">VLOOKUP(I45,$E$4:$F$9,2,FALSE)</f>
+        <f t="shared" ref="G45:G76" si="11">VLOOKUP(I45,$E$4:$F$9,2,FALSE)</f>
         <v>Domestic Potential</v>
       </c>
       <c r="H45" s="296" t="str">
@@ -8327,11 +8339,11 @@
         <v>MINPEAT_S1</v>
       </c>
       <c r="F46" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Peat  - Step 1</v>
+      </c>
+      <c r="G46" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Peat  - Step 1</v>
-      </c>
-      <c r="G46" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H46" s="296" t="str">
@@ -8339,7 +8351,7 @@
         <v>PEAT</v>
       </c>
       <c r="I46" s="296" t="str">
-        <f t="shared" ref="I46:I83" si="13">$E$4</f>
+        <f t="shared" ref="I46:I85" si="12">$E$4</f>
         <v>MIN</v>
       </c>
       <c r="J46" s="296" t="str">
@@ -8370,11 +8382,11 @@
         <v>MINPEAT_S2</v>
       </c>
       <c r="F47" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Peat  - Step 2</v>
+      </c>
+      <c r="G47" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Peat  - Step 2</v>
-      </c>
-      <c r="G47" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H47" s="296" t="str">
@@ -8382,7 +8394,7 @@
         <v>PEAT</v>
       </c>
       <c r="I47" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J47" s="296" t="str">
@@ -8405,19 +8417,19 @@
         <v>MINRENHYD</v>
       </c>
       <c r="F48" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Domestic Potential of Hydro </v>
+      </c>
+      <c r="G48" s="296" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Domestic Potential of Hydro </v>
-      </c>
-      <c r="G48" s="296" t="str">
+        <v>Domestic Potential</v>
+      </c>
+      <c r="H48" s="296" t="str">
+        <f t="shared" ref="H48:H53" si="13">B64</f>
+        <v>RENHYD</v>
+      </c>
+      <c r="I48" s="296" t="str">
         <f t="shared" si="12"/>
-        <v>Domestic Potential</v>
-      </c>
-      <c r="H48" s="296" t="str">
-        <f t="shared" ref="H48:H53" si="14">B64</f>
-        <v>RENHYD</v>
-      </c>
-      <c r="I48" s="296" t="str">
-        <f t="shared" si="13"/>
         <v>MIN</v>
       </c>
       <c r="J48" s="296"/>
@@ -8433,23 +8445,23 @@
         <v>301</v>
       </c>
       <c r="E49" s="296" t="str">
-        <f t="shared" ref="E49:E54" si="15">I49&amp;H49&amp;J49</f>
+        <f t="shared" ref="E49:E54" si="14">I49&amp;H49&amp;J49</f>
         <v>MINRENWIN</v>
       </c>
       <c r="F49" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Domestic Potential of Wind </v>
+      </c>
+      <c r="G49" s="296" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Domestic Potential of Wind </v>
-      </c>
-      <c r="G49" s="296" t="str">
+        <v>Domestic Potential</v>
+      </c>
+      <c r="H49" s="296" t="str">
+        <f t="shared" si="13"/>
+        <v>RENWIN</v>
+      </c>
+      <c r="I49" s="296" t="str">
         <f t="shared" si="12"/>
-        <v>Domestic Potential</v>
-      </c>
-      <c r="H49" s="296" t="str">
-        <f t="shared" si="14"/>
-        <v>RENWIN</v>
-      </c>
-      <c r="I49" s="296" t="str">
-        <f t="shared" si="13"/>
         <v>MIN</v>
       </c>
       <c r="J49" s="296"/>
@@ -8465,23 +8477,23 @@
         <v>302</v>
       </c>
       <c r="E50" s="296" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>MINRENSOL</v>
       </c>
       <c r="F50" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Domestic Potential of Solar </v>
+      </c>
+      <c r="G50" s="296" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Domestic Potential of Solar </v>
-      </c>
-      <c r="G50" s="296" t="str">
+        <v>Domestic Potential</v>
+      </c>
+      <c r="H50" s="296" t="str">
+        <f t="shared" si="13"/>
+        <v>RENSOL</v>
+      </c>
+      <c r="I50" s="296" t="str">
         <f t="shared" si="12"/>
-        <v>Domestic Potential</v>
-      </c>
-      <c r="H50" s="296" t="str">
-        <f t="shared" si="14"/>
-        <v>RENSOL</v>
-      </c>
-      <c r="I50" s="296" t="str">
-        <f t="shared" si="13"/>
         <v>MIN</v>
       </c>
       <c r="J50" s="296"/>
@@ -8497,23 +8509,23 @@
         <v>303</v>
       </c>
       <c r="E51" s="296" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>MINMSWAS</v>
       </c>
       <c r="F51" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Domestic Potential of Municipal Solid Waste </v>
+      </c>
+      <c r="G51" s="296" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Domestic Potential of Municipal Solid Waste </v>
-      </c>
-      <c r="G51" s="296" t="str">
+        <v>Domestic Potential</v>
+      </c>
+      <c r="H51" s="296" t="str">
+        <f t="shared" si="13"/>
+        <v>MSWAS</v>
+      </c>
+      <c r="I51" s="296" t="str">
         <f t="shared" si="12"/>
-        <v>Domestic Potential</v>
-      </c>
-      <c r="H51" s="296" t="str">
-        <f t="shared" si="14"/>
-        <v>MSWAS</v>
-      </c>
-      <c r="I51" s="296" t="str">
-        <f t="shared" si="13"/>
         <v>MIN</v>
       </c>
       <c r="J51" s="296"/>
@@ -8529,23 +8541,23 @@
         <v>304</v>
       </c>
       <c r="E52" s="296" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>MINRENOCE</v>
       </c>
       <c r="F52" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Domestic Potential of Ocean </v>
+      </c>
+      <c r="G52" s="296" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Domestic Potential of Ocean </v>
-      </c>
-      <c r="G52" s="296" t="str">
+        <v>Domestic Potential</v>
+      </c>
+      <c r="H52" s="296" t="str">
+        <f t="shared" si="13"/>
+        <v>RENOCE</v>
+      </c>
+      <c r="I52" s="296" t="str">
         <f t="shared" si="12"/>
-        <v>Domestic Potential</v>
-      </c>
-      <c r="H52" s="296" t="str">
-        <f t="shared" si="14"/>
-        <v>RENOCE</v>
-      </c>
-      <c r="I52" s="296" t="str">
-        <f t="shared" si="13"/>
         <v>MIN</v>
       </c>
       <c r="J52" s="296"/>
@@ -8561,23 +8573,23 @@
         <v>305</v>
       </c>
       <c r="E53" s="296" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>MINRENGEO</v>
       </c>
       <c r="F53" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Domestic Potential of Geothermal </v>
+      </c>
+      <c r="G53" s="296" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Domestic Potential of Geothermal </v>
-      </c>
-      <c r="G53" s="296" t="str">
+        <v>Domestic Potential</v>
+      </c>
+      <c r="H53" s="296" t="str">
+        <f t="shared" si="13"/>
+        <v>RENGEO</v>
+      </c>
+      <c r="I53" s="296" t="str">
         <f t="shared" si="12"/>
-        <v>Domestic Potential</v>
-      </c>
-      <c r="H53" s="296" t="str">
-        <f t="shared" si="14"/>
-        <v>RENGEO</v>
-      </c>
-      <c r="I53" s="296" t="str">
-        <f t="shared" si="13"/>
         <v>MIN</v>
       </c>
       <c r="J53" s="296"/>
@@ -8593,15 +8605,15 @@
         <v>306</v>
       </c>
       <c r="E54" s="296" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>MINBIOWOO1_S1</v>
       </c>
       <c r="F54" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Sawmill residues - Step 1</v>
+      </c>
+      <c r="G54" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Sawmill residues - Step 1</v>
-      </c>
-      <c r="G54" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H54" s="296" t="str">
@@ -8609,7 +8621,7 @@
         <v>BIOWOO1</v>
       </c>
       <c r="I54" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J54" s="296" t="str">
@@ -8628,15 +8640,15 @@
         <v>307</v>
       </c>
       <c r="E55" s="296" t="str">
-        <f t="shared" ref="E55:E63" si="16">I55&amp;H55&amp;J55</f>
+        <f t="shared" ref="E55:E63" si="15">I55&amp;H55&amp;J55</f>
         <v>MINBIOWOO1_S2</v>
       </c>
       <c r="F55" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Sawmill residues - Step 2</v>
+      </c>
+      <c r="G55" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Sawmill residues - Step 2</v>
-      </c>
-      <c r="G55" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H55" s="296" t="str">
@@ -8644,7 +8656,7 @@
         <v>BIOWOO1</v>
       </c>
       <c r="I55" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J55" s="296" t="str">
@@ -8663,15 +8675,15 @@
         <v>308</v>
       </c>
       <c r="E56" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO1_S3</v>
       </c>
       <c r="F56" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Sawmill residues - Step 3</v>
+      </c>
+      <c r="G56" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Sawmill residues - Step 3</v>
-      </c>
-      <c r="G56" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H56" s="296" t="str">
@@ -8679,7 +8691,7 @@
         <v>BIOWOO1</v>
       </c>
       <c r="I56" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J56" s="296" t="str">
@@ -8698,15 +8710,15 @@
         <v>309</v>
       </c>
       <c r="E57" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO2_S1</v>
       </c>
       <c r="F57" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Post-Consumer Recycled Wood - Step 1</v>
+      </c>
+      <c r="G57" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Post-Consumer Recycled Wood - Step 1</v>
-      </c>
-      <c r="G57" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H57" s="296" t="str">
@@ -8714,7 +8726,7 @@
         <v>BIOWOO2</v>
       </c>
       <c r="I57" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J57" s="296" t="str">
@@ -8733,15 +8745,15 @@
         <v>310</v>
       </c>
       <c r="E58" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO2_S2</v>
       </c>
       <c r="F58" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Post-Consumer Recycled Wood - Step 2</v>
+      </c>
+      <c r="G58" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Post-Consumer Recycled Wood - Step 2</v>
-      </c>
-      <c r="G58" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H58" s="296" t="str">
@@ -8749,7 +8761,7 @@
         <v>BIOWOO2</v>
       </c>
       <c r="I58" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J58" s="296" t="str">
@@ -8776,15 +8788,15 @@
         <v>311</v>
       </c>
       <c r="E59" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO2_S3</v>
       </c>
       <c r="F59" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Post-Consumer Recycled Wood - Step 3</v>
+      </c>
+      <c r="G59" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Post-Consumer Recycled Wood - Step 3</v>
-      </c>
-      <c r="G59" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H59" s="296" t="str">
@@ -8792,7 +8804,7 @@
         <v>BIOWOO2</v>
       </c>
       <c r="I59" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J59" s="296" t="str">
@@ -8811,15 +8823,15 @@
         <v>342</v>
       </c>
       <c r="E60" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO3_S1</v>
       </c>
       <c r="F60" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Straw - Step 1</v>
+      </c>
+      <c r="G60" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Straw - Step 1</v>
-      </c>
-      <c r="G60" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H60" s="296" t="str">
@@ -8827,7 +8839,7 @@
         <v>BIOWOO3</v>
       </c>
       <c r="I60" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J60" s="296" t="str">
@@ -8846,15 +8858,15 @@
         <v>296</v>
       </c>
       <c r="E61" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO3_S2</v>
       </c>
       <c r="F61" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Straw - Step 2</v>
+      </c>
+      <c r="G61" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Straw - Step 2</v>
-      </c>
-      <c r="G61" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H61" s="296" t="str">
@@ -8862,7 +8874,7 @@
         <v>BIOWOO3</v>
       </c>
       <c r="I61" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J61" s="296" t="str">
@@ -8881,15 +8893,15 @@
         <v>297</v>
       </c>
       <c r="E62" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOWOO3_S3</v>
       </c>
       <c r="F62" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Straw - Step 3</v>
+      </c>
+      <c r="G62" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Straw - Step 3</v>
-      </c>
-      <c r="G62" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H62" s="296" t="str">
@@ -8897,7 +8909,7 @@
         <v>BIOWOO3</v>
       </c>
       <c r="I62" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J62" s="296" t="str">
@@ -8916,15 +8928,15 @@
         <v>333</v>
       </c>
       <c r="E63" s="296" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>MINBIOMSW1_S1</v>
       </c>
       <c r="F63" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Biodegradable Municipal Solid Waste potential - Solid  - Step 1</v>
+      </c>
+      <c r="G63" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Biodegradable Municipal Solid Waste potential - Solid  - Step 1</v>
-      </c>
-      <c r="G63" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H63" s="296" t="str">
@@ -8932,7 +8944,7 @@
         <v>BIOMSW1</v>
       </c>
       <c r="I63" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J63" s="296" t="str">
@@ -8951,15 +8963,15 @@
         <v>312</v>
       </c>
       <c r="E64" s="296" t="str">
-        <f t="shared" ref="E64:E83" si="17">I64&amp;H64&amp;J64</f>
+        <f t="shared" ref="E64:E83" si="16">I64&amp;H64&amp;J64</f>
         <v>MINBIOMSW1_S2</v>
       </c>
       <c r="F64" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Biodegradable Municipal Solid Waste potential - Solid  - Step 2</v>
+      </c>
+      <c r="G64" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Biodegradable Municipal Solid Waste potential - Solid  - Step 2</v>
-      </c>
-      <c r="G64" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H64" s="296" t="str">
@@ -8967,7 +8979,7 @@
         <v>BIOMSW1</v>
       </c>
       <c r="I64" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J64" s="296" t="str">
@@ -8986,15 +8998,15 @@
         <v>313</v>
       </c>
       <c r="E65" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOMSW1_S3</v>
       </c>
       <c r="F65" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Biodegradable Municipal Solid Waste potential - Solid  - Step 3</v>
+      </c>
+      <c r="G65" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Biodegradable Municipal Solid Waste potential - Solid  - Step 3</v>
-      </c>
-      <c r="G65" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H65" s="296" t="str">
@@ -9002,7 +9014,7 @@
         <v>BIOMSW1</v>
       </c>
       <c r="I65" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J65" s="296" t="str">
@@ -9021,15 +9033,15 @@
         <v>314</v>
       </c>
       <c r="E66" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOMSW2_S1</v>
       </c>
       <c r="F66" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Biodegradable Municipal Solid Waste  - Step 1</v>
+      </c>
+      <c r="G66" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Biodegradable Municipal Solid Waste  - Step 1</v>
-      </c>
-      <c r="G66" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H66" s="296" t="str">
@@ -9037,7 +9049,7 @@
         <v>BIOMSW2</v>
       </c>
       <c r="I66" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J66" s="296" t="str">
@@ -9056,15 +9068,15 @@
         <v>315</v>
       </c>
       <c r="E67" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOMSW2_S2</v>
       </c>
       <c r="F67" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Biodegradable Municipal Solid Waste  - Step 2</v>
+      </c>
+      <c r="G67" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Biodegradable Municipal Solid Waste  - Step 2</v>
-      </c>
-      <c r="G67" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H67" s="296" t="str">
@@ -9072,7 +9084,7 @@
         <v>BIOMSW2</v>
       </c>
       <c r="I67" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J67" s="296" t="str">
@@ -9091,15 +9103,15 @@
         <v>316</v>
       </c>
       <c r="E68" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOMSW2_S3</v>
       </c>
       <c r="F68" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Biodegradable Municipal Solid Waste  - Step 3</v>
+      </c>
+      <c r="G68" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Biodegradable Municipal Solid Waste  - Step 3</v>
-      </c>
-      <c r="G68" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H68" s="296" t="str">
@@ -9107,7 +9119,7 @@
         <v>BIOMSW2</v>
       </c>
       <c r="I68" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J68" s="296" t="str">
@@ -9126,15 +9138,15 @@
         <v>317</v>
       </c>
       <c r="E69" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOTLW_S1</v>
       </c>
       <c r="F69" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Tallow  - Step 1</v>
+      </c>
+      <c r="G69" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Tallow  - Step 1</v>
-      </c>
-      <c r="G69" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H69" s="296" t="str">
@@ -9142,7 +9154,7 @@
         <v>BIOTLW</v>
       </c>
       <c r="I69" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J69" s="296" t="str">
@@ -9161,15 +9173,15 @@
         <v>318</v>
       </c>
       <c r="E70" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOTLW_S2</v>
       </c>
       <c r="F70" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Tallow  - Step 2</v>
+      </c>
+      <c r="G70" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Tallow  - Step 2</v>
-      </c>
-      <c r="G70" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H70" s="296" t="str">
@@ -9177,7 +9189,7 @@
         <v>BIOTLW</v>
       </c>
       <c r="I70" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J70" s="296" t="str">
@@ -9196,15 +9208,15 @@
         <v>319</v>
       </c>
       <c r="E71" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOTLW_S3</v>
       </c>
       <c r="F71" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Tallow  - Step 3</v>
+      </c>
+      <c r="G71" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Tallow  - Step 3</v>
-      </c>
-      <c r="G71" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H71" s="296" t="str">
@@ -9212,7 +9224,7 @@
         <v>BIOTLW</v>
       </c>
       <c r="I71" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J71" s="296" t="str">
@@ -9231,15 +9243,15 @@
         <v>320</v>
       </c>
       <c r="E72" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIORVO_S1</v>
       </c>
       <c r="F72" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Recovered Vegetable Oil  - Step 1</v>
+      </c>
+      <c r="G72" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Recovered Vegetable Oil  - Step 1</v>
-      </c>
-      <c r="G72" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H72" s="296" t="str">
@@ -9247,7 +9259,7 @@
         <v>BIORVO</v>
       </c>
       <c r="I72" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J72" s="296" t="str">
@@ -9266,15 +9278,15 @@
         <v>321</v>
       </c>
       <c r="E73" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIORVO_S2</v>
       </c>
       <c r="F73" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Recovered Vegetable Oil  - Step 2</v>
+      </c>
+      <c r="G73" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Recovered Vegetable Oil  - Step 2</v>
-      </c>
-      <c r="G73" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H73" s="296" t="str">
@@ -9282,7 +9294,7 @@
         <v>BIORVO</v>
       </c>
       <c r="I73" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J73" s="296" t="str">
@@ -9301,15 +9313,15 @@
         <v>322</v>
       </c>
       <c r="E74" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIORVO_S3</v>
       </c>
       <c r="F74" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Recovered Vegetable Oil  - Step 3</v>
+      </c>
+      <c r="G74" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Recovered Vegetable Oil  - Step 3</v>
-      </c>
-      <c r="G74" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H74" s="296" t="str">
@@ -9317,7 +9329,7 @@
         <v>BIORVO</v>
       </c>
       <c r="I74" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J74" s="296" t="str">
@@ -9336,15 +9348,15 @@
         <v>323</v>
       </c>
       <c r="E75" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOCATW_S1</v>
       </c>
       <c r="F75" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Cattle Waste  - Step 1</v>
+      </c>
+      <c r="G75" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Cattle Waste  - Step 1</v>
-      </c>
-      <c r="G75" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H75" s="296" t="str">
@@ -9352,7 +9364,7 @@
         <v>BIOCATW</v>
       </c>
       <c r="I75" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J75" s="296" t="str">
@@ -9371,15 +9383,15 @@
         <v>488</v>
       </c>
       <c r="E76" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOCATW_S2</v>
       </c>
       <c r="F76" s="294" t="str">
+        <f t="shared" si="3"/>
+        <v>Domestic Potential of Cattle Waste  - Step 2</v>
+      </c>
+      <c r="G76" s="296" t="str">
         <f t="shared" si="11"/>
-        <v>Domestic Potential of Cattle Waste  - Step 2</v>
-      </c>
-      <c r="G76" s="296" t="str">
-        <f t="shared" si="12"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H76" s="296" t="str">
@@ -9387,7 +9399,7 @@
         <v>BIOCATW</v>
       </c>
       <c r="I76" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J76" s="296" t="str">
@@ -9406,15 +9418,15 @@
         <v>489</v>
       </c>
       <c r="E77" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOCATW_S3</v>
       </c>
       <c r="F77" s="294" t="str">
-        <f t="shared" ref="F77:F83" si="18">G77 &amp; " of " &amp; VLOOKUP(H77,$B$13:$C$90,2,FALSE) &amp; IF(J77&lt;&gt;0,IF(VLOOKUP(J77,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J77,$I$4:$J$10,2,FALSE),""),"")</f>
+        <f t="shared" si="3"/>
         <v>Domestic Potential of Cattle Waste  - Step 3</v>
       </c>
       <c r="G77" s="296" t="str">
-        <f t="shared" ref="G77:G83" si="19">VLOOKUP(I77,$E$4:$F$9,2,FALSE)</f>
+        <f t="shared" ref="G77:G83" si="17">VLOOKUP(I77,$E$4:$F$9,2,FALSE)</f>
         <v>Domestic Potential</v>
       </c>
       <c r="H77" s="296" t="str">
@@ -9422,7 +9434,7 @@
         <v>BIOCATW</v>
       </c>
       <c r="I77" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J77" s="296" t="str">
@@ -9441,15 +9453,15 @@
         <v>490</v>
       </c>
       <c r="E78" s="296" t="str">
+        <f t="shared" si="16"/>
+        <v>MINBIOPIGW_S1</v>
+      </c>
+      <c r="F78" s="294" t="str">
+        <f t="shared" ref="F78:F85" si="18">G78 &amp; " of " &amp; VLOOKUP(H78,$B$13:$C$91,2,FALSE) &amp; IF(J78&lt;&gt;0,IF(VLOOKUP(J78,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J78,$I$4:$J$10,2,FALSE),""),"")</f>
+        <v>Domestic Potential of Pig Waste  - Step 1</v>
+      </c>
+      <c r="G78" s="296" t="str">
         <f t="shared" si="17"/>
-        <v>MINBIOPIGW_S1</v>
-      </c>
-      <c r="F78" s="294" t="str">
-        <f t="shared" si="18"/>
-        <v>Domestic Potential of Pig Waste  - Step 1</v>
-      </c>
-      <c r="G78" s="296" t="str">
-        <f t="shared" si="19"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H78" s="296" t="str">
@@ -9457,7 +9469,7 @@
         <v>BIOPIGW</v>
       </c>
       <c r="I78" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J78" s="296" t="str">
@@ -9476,7 +9488,7 @@
         <v>491</v>
       </c>
       <c r="E79" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOPIGW_S2</v>
       </c>
       <c r="F79" s="294" t="str">
@@ -9484,7 +9496,7 @@
         <v>Domestic Potential of Pig Waste  - Step 2</v>
       </c>
       <c r="G79" s="296" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H79" s="296" t="str">
@@ -9492,7 +9504,7 @@
         <v>BIOPIGW</v>
       </c>
       <c r="I79" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J79" s="296" t="str">
@@ -9511,7 +9523,7 @@
         <v>324</v>
       </c>
       <c r="E80" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOPIGW_S3</v>
       </c>
       <c r="F80" s="294" t="str">
@@ -9519,7 +9531,7 @@
         <v>Domestic Potential of Pig Waste  - Step 3</v>
       </c>
       <c r="G80" s="296" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H80" s="296" t="str">
@@ -9527,7 +9539,7 @@
         <v>BIOPIGW</v>
       </c>
       <c r="I80" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J80" s="296" t="str">
@@ -9546,7 +9558,7 @@
         <v>325</v>
       </c>
       <c r="E81" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOINDF_S1</v>
       </c>
       <c r="F81" s="294" t="str">
@@ -9554,7 +9566,7 @@
         <v>Domestic Potential of Industrial Food Waste  - Step 1</v>
       </c>
       <c r="G81" s="296" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H81" s="296" t="str">
@@ -9562,7 +9574,7 @@
         <v>BIOINDF</v>
       </c>
       <c r="I81" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J81" s="296" t="str">
@@ -9581,7 +9593,7 @@
         <v>326</v>
       </c>
       <c r="E82" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOINDF_S2</v>
       </c>
       <c r="F82" s="294" t="str">
@@ -9589,7 +9601,7 @@
         <v>Domestic Potential of Industrial Food Waste  - Step 2</v>
       </c>
       <c r="G82" s="296" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H82" s="296" t="str">
@@ -9597,7 +9609,7 @@
         <v>BIOINDF</v>
       </c>
       <c r="I82" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J82" s="296" t="str">
@@ -9616,7 +9628,7 @@
         <v>327</v>
       </c>
       <c r="E83" s="296" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>MINBIOINDF_S3</v>
       </c>
       <c r="F83" s="294" t="str">
@@ -9624,7 +9636,7 @@
         <v>Domestic Potential of Industrial Food Waste  - Step 3</v>
       </c>
       <c r="G83" s="296" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Domestic Potential</v>
       </c>
       <c r="H83" s="296" t="str">
@@ -9632,7 +9644,7 @@
         <v>BIOINDF</v>
       </c>
       <c r="I83" s="296" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>MIN</v>
       </c>
       <c r="J83" s="296" t="str">
@@ -9651,31 +9663,28 @@
         <v>328</v>
       </c>
       <c r="E84" s="296" t="str">
-        <f t="shared" ref="E84:E85" si="20">I84&amp;H84&amp;J84</f>
-        <v>IMPELC_UK</v>
+        <f t="shared" ref="E84:E85" si="19">I84&amp;H84&amp;J84</f>
+        <v>MINCYC</v>
       </c>
       <c r="F84" s="294" t="str">
-        <f t="shared" ref="F84:F85" si="21">G84 &amp; " of " &amp; VLOOKUP(H84,$B$13:$C$90,2,FALSE) &amp; IF(J84&lt;&gt;0,IF(VLOOKUP(J84,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J84,$I$4:$J$10,2,FALSE),""),"")</f>
-        <v>Import of Electricity - UK</v>
+        <f t="shared" si="18"/>
+        <v>Domestic Potential of Cycling</v>
       </c>
       <c r="G84" s="296" t="str">
-        <f t="shared" ref="G84:G85" si="22">VLOOKUP(I84,$E$4:$F$9,2,FALSE)</f>
-        <v>Import</v>
+        <f t="shared" ref="G84:G85" si="20">VLOOKUP(I84,$E$4:$F$9,2,FALSE)</f>
+        <v>Domestic Potential</v>
       </c>
       <c r="H84" s="296" t="str">
-        <f>$B$43</f>
-        <v>ELC</v>
+        <f>$B$90</f>
+        <v>CYC</v>
       </c>
       <c r="I84" s="296" t="str">
-        <f>$E$5</f>
-        <v>IMP</v>
-      </c>
-      <c r="J84" s="296" t="str">
-        <f>$I$4</f>
-        <v>_UK</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>MIN</v>
+      </c>
+      <c r="J84" s="296"/>
       <c r="K84" s="296" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L84" s="294"/>
     </row>
@@ -9687,31 +9696,28 @@
         <v>329</v>
       </c>
       <c r="E85" s="296" t="str">
+        <f t="shared" si="19"/>
+        <v>MINWLK</v>
+      </c>
+      <c r="F85" s="294" t="str">
+        <f t="shared" si="18"/>
+        <v>Domestic Potential of Walking</v>
+      </c>
+      <c r="G85" s="296" t="str">
         <f t="shared" si="20"/>
-        <v>EXPELC_UK</v>
-      </c>
-      <c r="F85" s="294" t="str">
-        <f t="shared" si="21"/>
-        <v>Export of Electricity - UK</v>
-      </c>
-      <c r="G85" s="296" t="str">
-        <f t="shared" si="22"/>
-        <v>Export</v>
+        <v>Domestic Potential</v>
       </c>
       <c r="H85" s="296" t="str">
-        <f>$B$43</f>
-        <v>ELC</v>
+        <f>$B$91</f>
+        <v>WLK</v>
       </c>
       <c r="I85" s="296" t="str">
-        <f>$E$6</f>
-        <v>EXP</v>
-      </c>
-      <c r="J85" s="296" t="str">
-        <f>$I$4</f>
-        <v>_UK</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>MIN</v>
+      </c>
+      <c r="J85" s="296"/>
       <c r="K85" s="296" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="L85" s="294"/>
     </row>
@@ -9723,27 +9729,31 @@
         <v>330</v>
       </c>
       <c r="E86" s="296" t="str">
-        <f t="shared" ref="E86" si="23">I86&amp;H86&amp;J86</f>
-        <v>BDNBIOWOO</v>
+        <f t="shared" ref="E86:E87" si="21">I86&amp;H86&amp;J86</f>
+        <v>IMPELC_UK</v>
       </c>
       <c r="F86" s="294" t="str">
-        <f>G86 &amp; " of " &amp; VLOOKUP(H86,$B$13:$C$90,2,FALSE) &amp; IF(J86&lt;&gt;0,IF(VLOOKUP(J86,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J86,$I$4:$J$10,2,FALSE),""),"")</f>
-        <v xml:space="preserve">Blending of Biomass - generic </v>
+        <f>G86 &amp; " of " &amp; VLOOKUP(H86,$B$13:$C$91,2,FALSE) &amp; IF(J86&lt;&gt;0,IF(VLOOKUP(J86,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J86,$I$4:$J$10,2,FALSE),""),"")</f>
+        <v>Import of Electricity - UK</v>
       </c>
       <c r="G86" s="296" t="str">
-        <f>VLOOKUP(I86,$E$4:$F$9,2,FALSE)</f>
-        <v>Blending</v>
+        <f t="shared" ref="G86:G87" si="22">VLOOKUP(I86,$E$4:$F$9,2,FALSE)</f>
+        <v>Import</v>
       </c>
       <c r="H86" s="296" t="str">
-        <f>B76</f>
-        <v>BIOWOO</v>
+        <f>$B$43</f>
+        <v>ELC</v>
       </c>
       <c r="I86" s="296" t="str">
-        <f>$E$9</f>
-        <v>BDN</v>
+        <f>$E$5</f>
+        <v>IMP</v>
+      </c>
+      <c r="J86" s="296" t="str">
+        <f>$I$4</f>
+        <v>_UK</v>
       </c>
       <c r="K86" s="296" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="2:12">
@@ -9754,31 +9764,31 @@
         <v>331</v>
       </c>
       <c r="E87" s="296" t="str">
-        <f>LEFT(B4,1)&amp;I87&amp;H87&amp;J87</f>
-        <v>SREFOILCRD_Whitegate</v>
+        <f t="shared" si="21"/>
+        <v>EXPELC_UK</v>
       </c>
       <c r="F87" s="294" t="str">
-        <f>G87 &amp; " of " &amp; VLOOKUP(H87,$B$13:$C$90,2,FALSE) &amp; IF(J87&lt;&gt;0,IF(VLOOKUP(J87,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J87,$I$4:$J$10,2,FALSE),""),"")</f>
-        <v>Refinery of Crude Oil  - Whitegate</v>
+        <f t="shared" ref="F87:F89" si="23">G87 &amp; " of " &amp; VLOOKUP(H87,$B$13:$C$90,2,FALSE) &amp; IF(J87&lt;&gt;0,IF(VLOOKUP(J87,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J87,$I$4:$J$10,2,FALSE),""),"")</f>
+        <v>Export of Electricity - UK</v>
       </c>
       <c r="G87" s="296" t="str">
-        <f>VLOOKUP(I87,$E$4:$F$9,2,FALSE)</f>
-        <v>Refinery</v>
-      </c>
-      <c r="H87" t="str">
-        <f>B51</f>
-        <v>OILCRD</v>
+        <f t="shared" si="22"/>
+        <v>Export</v>
+      </c>
+      <c r="H87" s="296" t="str">
+        <f>$B$43</f>
+        <v>ELC</v>
       </c>
       <c r="I87" s="296" t="str">
-        <f>$E$7</f>
-        <v>REF</v>
-      </c>
-      <c r="J87" t="str">
-        <f>I6</f>
-        <v>_Whitegate</v>
+        <f>$E$6</f>
+        <v>EXP</v>
+      </c>
+      <c r="J87" s="296" t="str">
+        <f>$I$4</f>
+        <v>_UK</v>
       </c>
       <c r="K87" s="296" t="s">
-        <v>186</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="2:12">
@@ -9789,26 +9799,25 @@
         <v>332</v>
       </c>
       <c r="E88" s="296" t="str">
-        <f>I88&amp;$B$4&amp;H88&amp;J88</f>
-        <v>FT-SUPNGA</v>
+        <f t="shared" ref="E88" si="24">I88&amp;H88&amp;J88</f>
+        <v>BDNBIOWOO</v>
       </c>
       <c r="F88" s="294" t="str">
-        <f>G88 &amp; " - " &amp; VLOOKUP(H88,$B$13:$C$90,2,FALSE) &amp; IF(J88&lt;&gt;0,IF(VLOOKUP(J88,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J88,$I$4:$J$10,2,FALSE),""),"") &amp; " (" &amp; $B$4 &amp; ")"</f>
-        <v>Fuel Tech - Natural Gas (SUP)</v>
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">Blending of Biomass - generic </v>
       </c>
       <c r="G88" s="296" t="str">
-        <f t="shared" ref="G88" si="24">VLOOKUP(I88,$E$4:$F$9,2,FALSE)</f>
-        <v>Fuel Tech</v>
-      </c>
-      <c r="H88" s="294" t="str">
-        <f>B20</f>
-        <v>NGA</v>
+        <f>VLOOKUP(I88,$E$4:$F$9,2,FALSE)</f>
+        <v>Blending</v>
+      </c>
+      <c r="H88" s="296" t="str">
+        <f>B76</f>
+        <v>BIOWOO</v>
       </c>
       <c r="I88" s="296" t="str">
-        <f>$E$8</f>
-        <v>FT-</v>
-      </c>
-      <c r="J88" s="294"/>
+        <f>$E$9</f>
+        <v>BDN</v>
+      </c>
       <c r="K88" s="296" t="s">
         <v>186</v>
       </c>
@@ -9821,51 +9830,58 @@
         <v>443</v>
       </c>
       <c r="E89" s="296" t="str">
-        <f t="shared" ref="E89:E92" si="25">I89&amp;$B$4&amp;H89&amp;J89</f>
-        <v>FT-SUPCOA</v>
+        <f>LEFT(B4,1)&amp;I89&amp;H89&amp;J89</f>
+        <v>SREFOILCRD_Whitegate</v>
       </c>
       <c r="F89" s="294" t="str">
-        <f t="shared" ref="F89:F92" si="26">G89 &amp; " - " &amp; VLOOKUP(H89,$B$13:$C$90,2,FALSE) &amp; IF(J89&lt;&gt;0,IF(VLOOKUP(J89,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J89,$I$4:$J$10,2,FALSE),""),"") &amp; " (" &amp; $B$4 &amp; ")"</f>
-        <v>Fuel Tech - Coal (SUP)</v>
+        <f t="shared" si="23"/>
+        <v>Refinery of Crude Oil  - Whitegate</v>
       </c>
       <c r="G89" s="296" t="str">
-        <f t="shared" ref="G89:G92" si="27">VLOOKUP(I89,$E$4:$F$9,2,FALSE)</f>
-        <v>Fuel Tech</v>
-      </c>
-      <c r="H89" s="294" t="str">
-        <f>B13</f>
-        <v>COA</v>
+        <f>VLOOKUP(I89,$E$4:$F$9,2,FALSE)</f>
+        <v>Refinery</v>
+      </c>
+      <c r="H89" t="str">
+        <f>B51</f>
+        <v>OILCRD</v>
       </c>
       <c r="I89" s="296" t="str">
-        <f t="shared" ref="I89:I92" si="28">$E$8</f>
-        <v>FT-</v>
-      </c>
-      <c r="J89" s="294"/>
+        <f>$E$7</f>
+        <v>REF</v>
+      </c>
+      <c r="J89" t="str">
+        <f>I6</f>
+        <v>_Whitegate</v>
+      </c>
       <c r="K89" s="296" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="90" spans="2:12">
-      <c r="B90" s="314"/>
-      <c r="C90" s="296"/>
+      <c r="B90" s="314" t="s">
+        <v>510</v>
+      </c>
+      <c r="C90" s="296" t="s">
+        <v>512</v>
+      </c>
       <c r="E90" s="296" t="str">
-        <f t="shared" si="25"/>
-        <v>FT-SUPWAS</v>
+        <f>I90&amp;$B$4&amp;H90&amp;J90</f>
+        <v>FT-SUPNGA</v>
       </c>
       <c r="F90" s="294" t="str">
-        <f t="shared" si="26"/>
-        <v>Fuel Tech - Waste (SUP)</v>
+        <f>G90 &amp; " - " &amp; VLOOKUP(H90,$B$13:$C$91,2,FALSE) &amp; IF(J90&lt;&gt;0,IF(VLOOKUP(J90,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J90,$I$4:$J$10,2,FALSE),""),"") &amp; " (" &amp; $B$4 &amp; ")"</f>
+        <v>Fuel Tech - Natural Gas (SUP)</v>
       </c>
       <c r="G90" s="296" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="G90" si="25">VLOOKUP(I90,$E$4:$F$9,2,FALSE)</f>
         <v>Fuel Tech</v>
       </c>
       <c r="H90" s="294" t="str">
-        <f>B45</f>
-        <v>WAS</v>
+        <f>B20</f>
+        <v>NGA</v>
       </c>
       <c r="I90" s="296" t="str">
-        <f t="shared" si="28"/>
+        <f>$E$8</f>
         <v>FT-</v>
       </c>
       <c r="J90" s="294"/>
@@ -9874,24 +9890,30 @@
       </c>
     </row>
     <row r="91" spans="2:12">
+      <c r="B91" s="313" t="s">
+        <v>511</v>
+      </c>
+      <c r="C91" s="296" t="s">
+        <v>513</v>
+      </c>
       <c r="E91" s="296" t="str">
-        <f t="shared" si="25"/>
-        <v>FT-SUPBIO</v>
+        <f t="shared" ref="E91:E94" si="26">I91&amp;$B$4&amp;H91&amp;J91</f>
+        <v>FT-SUPCOA</v>
       </c>
       <c r="F91" s="294" t="str">
-        <f t="shared" si="26"/>
-        <v>Fuel Tech - Biomass (SUP)</v>
+        <f t="shared" ref="F91:F94" si="27">G91 &amp; " - " &amp; VLOOKUP(H91,$B$13:$C$91,2,FALSE) &amp; IF(J91&lt;&gt;0,IF(VLOOKUP(J91,$I$4:$J$10,2,FALSE)&lt;&gt;""," - " &amp; VLOOKUP(J91,$I$4:$J$10,2,FALSE),""),"") &amp; " (" &amp; $B$4 &amp; ")"</f>
+        <v>Fuel Tech - Coal (SUP)</v>
       </c>
       <c r="G91" s="296" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="G91:G94" si="28">VLOOKUP(I91,$E$4:$F$9,2,FALSE)</f>
         <v>Fuel Tech</v>
       </c>
       <c r="H91" s="294" t="str">
-        <f>B21</f>
-        <v>BIO</v>
+        <f>B13</f>
+        <v>COA</v>
       </c>
       <c r="I91" s="296" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="I91:I94" si="29">$E$8</f>
         <v>FT-</v>
       </c>
       <c r="J91" s="294"/>
@@ -9900,28 +9922,82 @@
       </c>
     </row>
     <row r="92" spans="2:12">
+      <c r="B92" s="313"/>
+      <c r="C92" s="296"/>
       <c r="E92" s="296" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
+        <v>FT-SUPWAS</v>
+      </c>
+      <c r="F92" s="294" t="str">
+        <f t="shared" si="27"/>
+        <v>Fuel Tech - Waste (SUP)</v>
+      </c>
+      <c r="G92" s="296" t="str">
+        <f t="shared" si="28"/>
+        <v>Fuel Tech</v>
+      </c>
+      <c r="H92" s="294" t="str">
+        <f>B45</f>
+        <v>WAS</v>
+      </c>
+      <c r="I92" s="296" t="str">
+        <f t="shared" si="29"/>
+        <v>FT-</v>
+      </c>
+      <c r="J92" s="294"/>
+      <c r="K92" s="296" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12">
+      <c r="E93" s="296" t="str">
+        <f t="shared" si="26"/>
+        <v>FT-SUPBIO</v>
+      </c>
+      <c r="F93" s="294" t="str">
+        <f t="shared" si="27"/>
+        <v>Fuel Tech - Biomass (SUP)</v>
+      </c>
+      <c r="G93" s="296" t="str">
+        <f t="shared" si="28"/>
+        <v>Fuel Tech</v>
+      </c>
+      <c r="H93" s="294" t="str">
+        <f>B21</f>
+        <v>BIO</v>
+      </c>
+      <c r="I93" s="296" t="str">
+        <f t="shared" si="29"/>
+        <v>FT-</v>
+      </c>
+      <c r="J93" s="294"/>
+      <c r="K93" s="296" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12">
+      <c r="E94" s="296" t="str">
+        <f t="shared" si="26"/>
         <v>FT-SUPELC</v>
       </c>
-      <c r="F92" s="294" t="str">
-        <f t="shared" si="26"/>
+      <c r="F94" s="294" t="str">
+        <f t="shared" si="27"/>
         <v>Fuel Tech - Electricity (SUP)</v>
       </c>
-      <c r="G92" s="296" t="str">
-        <f t="shared" si="27"/>
+      <c r="G94" s="296" t="str">
+        <f t="shared" si="28"/>
         <v>Fuel Tech</v>
       </c>
-      <c r="H92" s="294" t="str">
+      <c r="H94" s="294" t="str">
         <f>B43</f>
         <v>ELC</v>
       </c>
-      <c r="I92" s="296" t="str">
-        <f t="shared" si="28"/>
+      <c r="I94" s="296" t="str">
+        <f t="shared" si="29"/>
         <v>FT-</v>
       </c>
-      <c r="J92" s="294"/>
-      <c r="K92" s="296" t="s">
+      <c r="J94" s="294"/>
+      <c r="K94" s="296" t="s">
         <v>186</v>
       </c>
     </row>
@@ -10056,7 +10132,7 @@
         <v>Import of Electricity - UK</v>
       </c>
       <c r="E5" s="42" t="str">
-        <f>Commodities!C54</f>
+        <f>Commodities!C56</f>
         <v>ELCC</v>
       </c>
       <c r="F5" s="193">
@@ -10105,7 +10181,7 @@
         <v>Export of Electricity - UK</v>
       </c>
       <c r="D6" s="49" t="str">
-        <f>Commodities!C54</f>
+        <f>Commodities!C56</f>
         <v>ELCC</v>
       </c>
       <c r="E6" s="49"/>
@@ -10152,20 +10228,20 @@
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="57"/>
-      <c r="F7" s="508" t="s">
+      <c r="F7" s="514" t="s">
         <v>195</v>
       </c>
-      <c r="G7" s="508"/>
-      <c r="H7" s="508"/>
-      <c r="I7" s="508"/>
-      <c r="J7" s="508"/>
+      <c r="G7" s="514"/>
+      <c r="H7" s="514"/>
+      <c r="I7" s="514"/>
+      <c r="J7" s="514"/>
       <c r="K7" s="491" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="508" t="s">
+      <c r="L7" s="514" t="s">
         <v>286</v>
       </c>
-      <c r="M7" s="508"/>
+      <c r="M7" s="514"/>
       <c r="N7" s="57"/>
     </row>
     <row r="9" spans="2:19">
@@ -10826,15 +10902,15 @@
         <v>16</v>
       </c>
       <c r="C5" s="289" t="str">
-        <f>Commodities!C50</f>
+        <f>Commodities!C52</f>
         <v>SUPNGA</v>
       </c>
       <c r="D5" s="289" t="str">
-        <f>Commodities!C49</f>
+        <f>Commodities!C51</f>
         <v>SUPCOA</v>
       </c>
       <c r="E5" s="289" t="str">
-        <f>Commodities!C53</f>
+        <f>Commodities!C55</f>
         <v>SUPWAS</v>
       </c>
       <c r="F5" s="289" t="s">
@@ -10843,7 +10919,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="276" t="str">
-        <f>Commodities!C64</f>
+        <f>Commodities!C66</f>
         <v>SUPCO2N</v>
       </c>
       <c r="C6" s="148">
@@ -10861,7 +10937,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="276" t="str">
-        <f>Commodities!C60</f>
+        <f>Commodities!C62</f>
         <v>SUPCH4N</v>
       </c>
       <c r="C7" s="148"/>
@@ -10870,7 +10946,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="276" t="str">
-        <f>Commodities!C63</f>
+        <f>Commodities!C65</f>
         <v>SUPSO2N</v>
       </c>
       <c r="C8" s="148"/>
@@ -10879,7 +10955,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="276" t="str">
-        <f>Commodities!C67</f>
+        <f>Commodities!C69</f>
         <v>SUPNOXN</v>
       </c>
       <c r="C9" s="148"/>
@@ -10888,13 +10964,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="275" t="str">
-        <f>Commodities!C68</f>
+        <f>Commodities!C70</f>
         <v>SUPPM10</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="275" t="str">
-        <f>Commodities!C69</f>
+        <f>Commodities!C71</f>
         <v>SUPPM25</v>
       </c>
     </row>
@@ -10943,10 +11019,10 @@
       <c r="J1" s="117" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="512" t="s">
+      <c r="P1" s="518" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="512"/>
+      <c r="Q1" s="518"/>
     </row>
     <row r="2" spans="1:22">
       <c r="H2" s="142"/>
@@ -14063,7 +14139,7 @@
     <col min="40" max="16384" width="9.140625" style="242"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="86.25" thickBot="1">
+    <row r="1" spans="1:39" ht="87" thickBot="1">
       <c r="A1" s="336" t="s">
         <v>501</v>
       </c>
@@ -16223,10 +16299,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:L94"/>
+  <dimension ref="B2:L96"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17174,53 +17250,53 @@
       <c r="B49" s="312" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B13</f>
-        <v>SUPCOA</v>
-      </c>
-      <c r="D49" s="309" t="str">
-        <f>CONVENTIONS!C13 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Coal (SUP)</v>
-      </c>
-      <c r="E49" s="303" t="s">
+      <c r="C49" s="318" t="str">
+        <f>CONVENTIONS!B90</f>
+        <v>CYC</v>
+      </c>
+      <c r="D49" s="318" t="str">
+        <f>CONVENTIONS!C90</f>
+        <v>Cycling</v>
+      </c>
+      <c r="E49" s="312" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="303"/>
-      <c r="G49" s="303"/>
-      <c r="H49" s="303"/>
-      <c r="I49" s="303"/>
+      <c r="F49" s="312"/>
+      <c r="G49" s="312"/>
+      <c r="H49" s="312"/>
+      <c r="I49" s="312"/>
     </row>
     <row r="50" spans="2:12">
       <c r="B50" s="312" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B20</f>
-        <v>SUPNGA</v>
-      </c>
-      <c r="D50" s="309" t="str">
-        <f>CONVENTIONS!C20 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Natural Gas (SUP)</v>
-      </c>
-      <c r="E50" s="303" t="s">
+      <c r="C50" s="318" t="str">
+        <f>CONVENTIONS!B91</f>
+        <v>WLK</v>
+      </c>
+      <c r="D50" s="318" t="str">
+        <f>CONVENTIONS!C91</f>
+        <v>Walking</v>
+      </c>
+      <c r="E50" s="312" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="303"/>
-      <c r="G50" s="303"/>
-      <c r="H50" s="303"/>
-      <c r="I50" s="303"/>
+      <c r="F50" s="312"/>
+      <c r="G50" s="312"/>
+      <c r="H50" s="312"/>
+      <c r="I50" s="312"/>
     </row>
     <row r="51" spans="2:12">
       <c r="B51" s="312" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B21</f>
-        <v>SUPBIO</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B13</f>
+        <v>SUPCOA</v>
       </c>
       <c r="D51" s="309" t="str">
-        <f>CONVENTIONS!C21 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Biomass (SUP)</v>
+        <f>CONVENTIONS!C13 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Coal (SUP)</v>
       </c>
       <c r="E51" s="303" t="s">
         <v>10</v>
@@ -17235,12 +17311,12 @@
         <v>23</v>
       </c>
       <c r="C52" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B43</f>
-        <v>SUPELC</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B20</f>
+        <v>SUPNGA</v>
       </c>
       <c r="D52" s="309" t="str">
-        <f>CONVENTIONS!C43 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Electricity (SUP)</v>
+        <f>CONVENTIONS!C20 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Natural Gas (SUP)</v>
       </c>
       <c r="E52" s="303" t="s">
         <v>10</v>
@@ -17255,12 +17331,12 @@
         <v>23</v>
       </c>
       <c r="C53" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B45</f>
-        <v>SUPWAS</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B21</f>
+        <v>SUPBIO</v>
       </c>
       <c r="D53" s="309" t="str">
-        <f>CONVENTIONS!C45 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Waste (SUP)</v>
+        <f>CONVENTIONS!C21 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Biomass (SUP)</v>
       </c>
       <c r="E53" s="303" t="s">
         <v>10</v>
@@ -17275,12 +17351,12 @@
         <v>23</v>
       </c>
       <c r="C54" s="309" t="str">
-        <f>CONVENTIONS!$B$43&amp;CONVENTIONS!P4</f>
-        <v>ELCC</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B43</f>
+        <v>SUPELC</v>
       </c>
       <c r="D54" s="309" t="str">
-        <f>CONVENTIONS!$C$43 &amp;  " - " &amp; CONVENTIONS!Q4</f>
-        <v>Electricity - centralised</v>
+        <f>CONVENTIONS!C43 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Electricity (SUP)</v>
       </c>
       <c r="E54" s="303" t="s">
         <v>10</v>
@@ -17295,20 +17371,18 @@
         <v>23</v>
       </c>
       <c r="C55" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M4&amp;CONVENTIONS!P4</f>
-        <v>SUPH2GC</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!B45</f>
+        <v>SUPWAS</v>
       </c>
       <c r="D55" s="309" t="str">
-        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N4 &amp; " - " &amp; CONVENTIONS!Q4&amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Hydrogen gaseous - centralised (SUP)</v>
+        <f>CONVENTIONS!C45 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Waste (SUP)</v>
       </c>
       <c r="E55" s="303" t="s">
         <v>10</v>
       </c>
       <c r="F55" s="303"/>
-      <c r="G55" s="303" t="s">
-        <v>73</v>
-      </c>
+      <c r="G55" s="303"/>
       <c r="H55" s="303"/>
       <c r="I55" s="303"/>
     </row>
@@ -17317,20 +17391,18 @@
         <v>23</v>
       </c>
       <c r="C56" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M5&amp;CONVENTIONS!P4</f>
-        <v>SUPH2LC</v>
+        <f>CONVENTIONS!$B$43&amp;CONVENTIONS!P4</f>
+        <v>ELCC</v>
       </c>
       <c r="D56" s="309" t="str">
-        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N5 &amp; " - " &amp; CONVENTIONS!Q4&amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Hydrogen liquid - centralised (SUP)</v>
+        <f>CONVENTIONS!$C$43 &amp;  " - " &amp; CONVENTIONS!Q4</f>
+        <v>Electricity - centralised</v>
       </c>
       <c r="E56" s="303" t="s">
         <v>10</v>
       </c>
       <c r="F56" s="303"/>
-      <c r="G56" s="303" t="s">
-        <v>73</v>
-      </c>
+      <c r="G56" s="303"/>
       <c r="H56" s="303"/>
       <c r="I56" s="303"/>
     </row>
@@ -17339,12 +17411,12 @@
         <v>23</v>
       </c>
       <c r="C57" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M4&amp;CONVENTIONS!P5</f>
-        <v>SUPH2GD</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M4&amp;CONVENTIONS!P4</f>
+        <v>SUPH2GC</v>
       </c>
       <c r="D57" s="309" t="str">
-        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N4 &amp; " - " &amp; CONVENTIONS!Q5 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Hydrogen gaseous - decentralised (SUP)</v>
+        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N4 &amp; " - " &amp; CONVENTIONS!Q4&amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Hydrogen gaseous - centralised (SUP)</v>
       </c>
       <c r="E57" s="303" t="s">
         <v>10</v>
@@ -17361,12 +17433,12 @@
         <v>23</v>
       </c>
       <c r="C58" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M5&amp;CONVENTIONS!P5</f>
-        <v>SUPH2LD</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M5&amp;CONVENTIONS!P4</f>
+        <v>SUPH2LC</v>
       </c>
       <c r="D58" s="309" t="str">
-        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N5 &amp; " - " &amp; CONVENTIONS!Q5 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Hydrogen liquid - decentralised (SUP)</v>
+        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N5 &amp; " - " &amp; CONVENTIONS!Q4&amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Hydrogen liquid - centralised (SUP)</v>
       </c>
       <c r="E58" s="303" t="s">
         <v>10</v>
@@ -17379,68 +17451,72 @@
       <c r="I58" s="303"/>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="319" t="s">
-        <v>417</v>
-      </c>
-      <c r="C59" s="319"/>
-      <c r="D59" s="319"/>
-      <c r="E59" s="319"/>
-      <c r="F59" s="319"/>
-      <c r="G59" s="319"/>
-      <c r="H59" s="319"/>
-      <c r="I59" s="319"/>
+      <c r="B59" s="312" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="309" t="str">
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M4&amp;CONVENTIONS!P5</f>
+        <v>SUPH2GD</v>
+      </c>
+      <c r="D59" s="309" t="str">
+        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N4 &amp; " - " &amp; CONVENTIONS!Q5 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Hydrogen gaseous - decentralised (SUP)</v>
+      </c>
+      <c r="E59" s="303" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="303"/>
+      <c r="G59" s="303" t="s">
+        <v>73</v>
+      </c>
+      <c r="H59" s="303"/>
+      <c r="I59" s="303"/>
     </row>
     <row r="60" spans="2:12">
       <c r="B60" s="312" t="s">
-        <v>338</v>
+        <v>23</v>
       </c>
       <c r="C60" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M13</f>
-        <v>SUPCH4N</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!$B$89&amp;CONVENTIONS!M5&amp;CONVENTIONS!P5</f>
+        <v>SUPH2LD</v>
       </c>
       <c r="D60" s="309" t="str">
-        <f>CONVENTIONS!N13 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Methane - eNergy Emissions (SUP)</v>
+        <f>CONVENTIONS!$C$89 &amp; " " &amp; CONVENTIONS!N5 &amp; " - " &amp; CONVENTIONS!Q5 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Hydrogen liquid - decentralised (SUP)</v>
       </c>
       <c r="E60" s="303" t="s">
-        <v>339</v>
+        <v>10</v>
       </c>
       <c r="F60" s="303"/>
-      <c r="G60" s="303"/>
+      <c r="G60" s="303" t="s">
+        <v>73</v>
+      </c>
       <c r="H60" s="303"/>
       <c r="I60" s="303"/>
     </row>
     <row r="61" spans="2:12">
-      <c r="B61" s="312" t="s">
-        <v>338</v>
-      </c>
-      <c r="C61" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M14</f>
-        <v>SUPCH4P</v>
-      </c>
-      <c r="D61" s="309" t="str">
-        <f>CONVENTIONS!N14 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Methane Emissions - Process Emissions (SUP)</v>
-      </c>
-      <c r="E61" s="303" t="s">
-        <v>339</v>
-      </c>
-      <c r="F61" s="303"/>
-      <c r="G61" s="303"/>
-      <c r="H61" s="303"/>
-      <c r="I61" s="303"/>
+      <c r="B61" s="319" t="s">
+        <v>417</v>
+      </c>
+      <c r="C61" s="319"/>
+      <c r="D61" s="319"/>
+      <c r="E61" s="319"/>
+      <c r="F61" s="319"/>
+      <c r="G61" s="319"/>
+      <c r="H61" s="319"/>
+      <c r="I61" s="319"/>
     </row>
     <row r="62" spans="2:12">
       <c r="B62" s="312" t="s">
         <v>338</v>
       </c>
       <c r="C62" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M15</f>
-        <v>SUPN2ON</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M13</f>
+        <v>SUPCH4N</v>
       </c>
       <c r="D62" s="309" t="str">
-        <f>CONVENTIONS!N15 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>N2O Emissions - eNergy Emissions (SUP)</v>
+        <f>CONVENTIONS!N13 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Methane - eNergy Emissions (SUP)</v>
       </c>
       <c r="E62" s="303" t="s">
         <v>339</v>
@@ -17455,12 +17531,12 @@
         <v>338</v>
       </c>
       <c r="C63" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M16</f>
-        <v>SUPSO2N</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M14</f>
+        <v>SUPCH4P</v>
       </c>
       <c r="D63" s="309" t="str">
-        <f>CONVENTIONS!N16 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Sulfur dioxide - eNergy Emissions (SUP)</v>
+        <f>CONVENTIONS!N14 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Methane Emissions - Process Emissions (SUP)</v>
       </c>
       <c r="E63" s="303" t="s">
         <v>339</v>
@@ -17478,12 +17554,12 @@
         <v>338</v>
       </c>
       <c r="C64" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M17</f>
-        <v>SUPCO2N</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M15</f>
+        <v>SUPN2ON</v>
       </c>
       <c r="D64" s="309" t="str">
-        <f>CONVENTIONS!N17 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Carbon Dioxide - eNergy Emissions (SUP)</v>
+        <f>CONVENTIONS!N15 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>N2O Emissions - eNergy Emissions (SUP)</v>
       </c>
       <c r="E64" s="303" t="s">
         <v>339</v>
@@ -17501,12 +17577,12 @@
         <v>338</v>
       </c>
       <c r="C65" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M18</f>
-        <v>SUPCO2P</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M16</f>
+        <v>SUPSO2N</v>
       </c>
       <c r="D65" s="309" t="str">
-        <f>CONVENTIONS!N18 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Carbon Dioxide - Process Emissions (SUP)</v>
+        <f>CONVENTIONS!N16 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Sulfur dioxide - eNergy Emissions (SUP)</v>
       </c>
       <c r="E65" s="303" t="s">
         <v>339</v>
@@ -17524,12 +17600,12 @@
         <v>338</v>
       </c>
       <c r="C66" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M19</f>
-        <v>SUPCO2S</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M17</f>
+        <v>SUPCO2N</v>
       </c>
       <c r="D66" s="309" t="str">
-        <f>CONVENTIONS!N19 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Carbon Dioxide - Sequestered (SUP)</v>
+        <f>CONVENTIONS!N17 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Carbon Dioxide - eNergy Emissions (SUP)</v>
       </c>
       <c r="E66" s="303" t="s">
         <v>339</v>
@@ -17547,12 +17623,12 @@
         <v>338</v>
       </c>
       <c r="C67" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M20</f>
-        <v>SUPNOXN</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M18</f>
+        <v>SUPCO2P</v>
       </c>
       <c r="D67" s="309" t="str">
-        <f>CONVENTIONS!N20 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Nitrogen Oxide  - eNergy Emissions (SUP)</v>
+        <f>CONVENTIONS!N18 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Carbon Dioxide - Process Emissions (SUP)</v>
       </c>
       <c r="E67" s="303" t="s">
         <v>339</v>
@@ -17570,12 +17646,12 @@
         <v>338</v>
       </c>
       <c r="C68" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M21</f>
-        <v>SUPPM10</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M19</f>
+        <v>SUPCO2S</v>
       </c>
       <c r="D68" s="309" t="str">
-        <f>CONVENTIONS!N21 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Particulate Matter &lt;10 µm (SUP)</v>
+        <f>CONVENTIONS!N19 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Carbon Dioxide - Sequestered (SUP)</v>
       </c>
       <c r="E68" s="303" t="s">
         <v>339</v>
@@ -17590,12 +17666,12 @@
         <v>338</v>
       </c>
       <c r="C69" s="309" t="str">
-        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M22</f>
-        <v>SUPPM25</v>
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M20</f>
+        <v>SUPNOXN</v>
       </c>
       <c r="D69" s="309" t="str">
-        <f>CONVENTIONS!N22 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
-        <v>Particulate Matter &lt;2.5 µm (SUP)</v>
+        <f>CONVENTIONS!N20 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Nitrogen Oxide  - eNergy Emissions (SUP)</v>
       </c>
       <c r="E69" s="303" t="s">
         <v>339</v>
@@ -17605,25 +17681,45 @@
       <c r="H69" s="303"/>
       <c r="I69" s="303"/>
     </row>
+    <row r="70" spans="2:12">
+      <c r="B70" s="312" t="s">
+        <v>338</v>
+      </c>
+      <c r="C70" s="309" t="str">
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M21</f>
+        <v>SUPPM10</v>
+      </c>
+      <c r="D70" s="309" t="str">
+        <f>CONVENTIONS!N21 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Particulate Matter &lt;10 µm (SUP)</v>
+      </c>
+      <c r="E70" s="303" t="s">
+        <v>339</v>
+      </c>
+      <c r="F70" s="303"/>
+      <c r="G70" s="303"/>
+      <c r="H70" s="303"/>
+      <c r="I70" s="303"/>
+    </row>
     <row r="71" spans="2:12">
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
-    </row>
-    <row r="72" spans="2:12">
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
+      <c r="B71" s="312" t="s">
+        <v>338</v>
+      </c>
+      <c r="C71" s="309" t="str">
+        <f>CONVENTIONS!$B$4&amp;CONVENTIONS!M22</f>
+        <v>SUPPM25</v>
+      </c>
+      <c r="D71" s="309" t="str">
+        <f>CONVENTIONS!N22 &amp; " (" &amp; CONVENTIONS!$B$4 &amp; ")"</f>
+        <v>Particulate Matter &lt;2.5 µm (SUP)</v>
+      </c>
+      <c r="E71" s="303" t="s">
+        <v>339</v>
+      </c>
+      <c r="F71" s="303"/>
+      <c r="G71" s="303"/>
+      <c r="H71" s="303"/>
+      <c r="I71" s="303"/>
     </row>
     <row r="73" spans="2:12">
       <c r="B73"/>
@@ -17844,6 +17940,26 @@
       <c r="G94"/>
       <c r="H94"/>
       <c r="I94"/>
+    </row>
+    <row r="95" spans="2:9">
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+    </row>
+    <row r="96" spans="2:9">
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19819,15 +19935,15 @@
     </row>
     <row r="80" spans="2:9" s="294" customFormat="1">
       <c r="B80" s="309" t="str">
-        <f>CONVENTIONS!K84</f>
+        <f>CONVENTIONS!K86</f>
         <v>IMP</v>
       </c>
       <c r="C80" s="309" t="str">
-        <f>CONVENTIONS!E84</f>
+        <f>CONVENTIONS!E86</f>
         <v>IMPELC_UK</v>
       </c>
       <c r="D80" s="309" t="str">
-        <f>CONVENTIONS!F84</f>
+        <f>CONVENTIONS!F86</f>
         <v>Import of Electricity - UK</v>
       </c>
       <c r="E80" s="323" t="s">
@@ -19844,15 +19960,15 @@
     </row>
     <row r="81" spans="2:9" s="294" customFormat="1">
       <c r="B81" s="309" t="str">
-        <f>CONVENTIONS!K85</f>
+        <f>CONVENTIONS!K87</f>
         <v>EXP</v>
       </c>
       <c r="C81" s="309" t="str">
-        <f>CONVENTIONS!E85</f>
+        <f>CONVENTIONS!E87</f>
         <v>EXPELC_UK</v>
       </c>
       <c r="D81" s="309" t="str">
-        <f>CONVENTIONS!F85</f>
+        <f>CONVENTIONS!F87</f>
         <v>Export of Electricity - UK</v>
       </c>
       <c r="E81" s="323" t="s">
@@ -19869,15 +19985,15 @@
     </row>
     <row r="82" spans="2:9">
       <c r="B82" s="309" t="str">
-        <f>CONVENTIONS!K86</f>
+        <f>CONVENTIONS!K88</f>
         <v>PRE</v>
       </c>
       <c r="C82" s="309" t="str">
-        <f>CONVENTIONS!E86</f>
+        <f>CONVENTIONS!E88</f>
         <v>BDNBIOWOO</v>
       </c>
       <c r="D82" s="309" t="str">
-        <f>CONVENTIONS!F86</f>
+        <f>CONVENTIONS!F88</f>
         <v xml:space="preserve">Blending of Biomass - generic </v>
       </c>
       <c r="E82" s="323" t="s">
@@ -19892,15 +20008,15 @@
     </row>
     <row r="83" spans="2:9">
       <c r="B83" s="309" t="str">
-        <f>CONVENTIONS!K87</f>
+        <f>CONVENTIONS!K89</f>
         <v>PRE</v>
       </c>
       <c r="C83" s="309" t="str">
-        <f>CONVENTIONS!E87</f>
+        <f>CONVENTIONS!E89</f>
         <v>SREFOILCRD_Whitegate</v>
       </c>
       <c r="D83" s="309" t="str">
-        <f>CONVENTIONS!F87</f>
+        <f>CONVENTIONS!F89</f>
         <v>Refinery of Crude Oil  - Whitegate</v>
       </c>
       <c r="E83" s="323" t="s">
@@ -19930,15 +20046,15 @@
     </row>
     <row r="85" spans="2:9">
       <c r="B85" s="309" t="str">
-        <f>CONVENTIONS!K88</f>
+        <f>CONVENTIONS!K90</f>
         <v>PRE</v>
       </c>
       <c r="C85" s="309" t="str">
-        <f>CONVENTIONS!E88</f>
+        <f>CONVENTIONS!E90</f>
         <v>FT-SUPNGA</v>
       </c>
       <c r="D85" s="309" t="str">
-        <f>CONVENTIONS!F88</f>
+        <f>CONVENTIONS!F90</f>
         <v>Fuel Tech - Natural Gas (SUP)</v>
       </c>
       <c r="E85" s="284" t="s">
@@ -19955,15 +20071,15 @@
     </row>
     <row r="86" spans="2:9">
       <c r="B86" s="309" t="str">
-        <f>CONVENTIONS!K89</f>
+        <f>CONVENTIONS!K91</f>
         <v>PRE</v>
       </c>
       <c r="C86" s="309" t="str">
-        <f>CONVENTIONS!E89</f>
+        <f>CONVENTIONS!E91</f>
         <v>FT-SUPCOA</v>
       </c>
       <c r="D86" s="309" t="str">
-        <f>CONVENTIONS!F89</f>
+        <f>CONVENTIONS!F91</f>
         <v>Fuel Tech - Coal (SUP)</v>
       </c>
       <c r="E86" s="331" t="s">
@@ -19978,15 +20094,15 @@
     </row>
     <row r="87" spans="2:9">
       <c r="B87" s="309" t="str">
-        <f>CONVENTIONS!K90</f>
+        <f>CONVENTIONS!K92</f>
         <v>PRE</v>
       </c>
       <c r="C87" s="309" t="str">
-        <f>CONVENTIONS!E90</f>
+        <f>CONVENTIONS!E92</f>
         <v>FT-SUPWAS</v>
       </c>
       <c r="D87" s="309" t="str">
-        <f>CONVENTIONS!F90</f>
+        <f>CONVENTIONS!F92</f>
         <v>Fuel Tech - Waste (SUP)</v>
       </c>
       <c r="E87" s="331" t="s">
@@ -20001,15 +20117,15 @@
     </row>
     <row r="88" spans="2:9">
       <c r="B88" s="309" t="str">
-        <f>CONVENTIONS!K91</f>
+        <f>CONVENTIONS!K93</f>
         <v>PRE</v>
       </c>
       <c r="C88" s="309" t="str">
-        <f>CONVENTIONS!E91</f>
+        <f>CONVENTIONS!E93</f>
         <v>FT-SUPBIO</v>
       </c>
       <c r="D88" s="309" t="str">
-        <f>CONVENTIONS!F91</f>
+        <f>CONVENTIONS!F93</f>
         <v>Fuel Tech - Biomass (SUP)</v>
       </c>
       <c r="E88" s="331" t="s">
@@ -20024,15 +20140,15 @@
     </row>
     <row r="89" spans="2:9">
       <c r="B89" s="309" t="str">
-        <f>CONVENTIONS!K92</f>
+        <f>CONVENTIONS!K94</f>
         <v>PRE</v>
       </c>
       <c r="C89" s="309" t="str">
-        <f>CONVENTIONS!E92</f>
+        <f>CONVENTIONS!E94</f>
         <v>FT-SUPELC</v>
       </c>
       <c r="D89" s="309" t="str">
-        <f>CONVENTIONS!F92</f>
+        <f>CONVENTIONS!F94</f>
         <v>Fuel Tech - Electricity (SUP)</v>
       </c>
       <c r="E89" s="284" t="s">
@@ -20404,7 +20520,7 @@
         <v>GASNAT</v>
       </c>
       <c r="D6" s="275" t="str">
-        <f>Commodities!C50</f>
+        <f>Commodities!C52</f>
         <v>SUPNGA</v>
       </c>
       <c r="E6" s="47">
@@ -20429,7 +20545,7 @@
         <v>COAHAR</v>
       </c>
       <c r="D7" s="275" t="str">
-        <f>Commodities!C49</f>
+        <f>Commodities!C51</f>
         <v>SUPCOA</v>
       </c>
       <c r="E7" s="47">
@@ -20454,7 +20570,7 @@
         <v>MSWAS</v>
       </c>
       <c r="D8" s="275" t="str">
-        <f>Commodities!C53</f>
+        <f>Commodities!C55</f>
         <v>SUPWAS</v>
       </c>
       <c r="E8" s="47">
@@ -20479,7 +20595,7 @@
         <v>BIOWOO, BIOWPE, BIOWCH</v>
       </c>
       <c r="D9" s="275" t="str">
-        <f>Commodities!C51</f>
+        <f>Commodities!C53</f>
         <v>SUPBIO</v>
       </c>
       <c r="E9" s="47">
@@ -20503,7 +20619,7 @@
         <v>70</v>
       </c>
       <c r="D10" s="275" t="str">
-        <f>Commodities!C52</f>
+        <f>Commodities!C54</f>
         <v>SUPELC</v>
       </c>
       <c r="E10" s="47">
@@ -21329,24 +21445,24 @@
       <c r="E23" s="141"/>
       <c r="F23" s="141"/>
       <c r="G23" s="141"/>
-      <c r="H23" s="500" t="s">
+      <c r="H23" s="506" t="s">
         <v>89</v>
       </c>
-      <c r="I23" s="501"/>
-      <c r="J23" s="501"/>
-      <c r="K23" s="502"/>
-      <c r="L23" s="503" t="s">
+      <c r="I23" s="507"/>
+      <c r="J23" s="507"/>
+      <c r="K23" s="508"/>
+      <c r="L23" s="509" t="s">
         <v>90</v>
       </c>
-      <c r="M23" s="503"/>
-      <c r="N23" s="503"/>
-      <c r="O23" s="504"/>
-      <c r="P23" s="493" t="s">
+      <c r="M23" s="509"/>
+      <c r="N23" s="509"/>
+      <c r="O23" s="510"/>
+      <c r="P23" s="499" t="s">
         <v>91</v>
       </c>
-      <c r="Q23" s="493"/>
-      <c r="R23" s="493"/>
-      <c r="S23" s="494"/>
+      <c r="Q23" s="499"/>
+      <c r="R23" s="499"/>
+      <c r="S23" s="500"/>
       <c r="T23"/>
     </row>
     <row r="24" spans="2:20">
@@ -22596,15 +22712,15 @@
       <c r="E57"/>
       <c r="F57"/>
       <c r="G57"/>
-      <c r="H57" s="495" t="s">
+      <c r="H57" s="501" t="s">
         <v>85</v>
       </c>
-      <c r="I57" s="496"/>
+      <c r="I57" s="502"/>
       <c r="J57"/>
-      <c r="K57" s="495" t="s">
+      <c r="K57" s="501" t="s">
         <v>96</v>
       </c>
-      <c r="L57" s="496"/>
+      <c r="L57" s="502"/>
       <c r="M57"/>
       <c r="S57"/>
     </row>
@@ -22636,7 +22752,7 @@
       <c r="E59"/>
       <c r="F59"/>
       <c r="G59"/>
-      <c r="H59" s="497" t="s">
+      <c r="H59" s="503" t="s">
         <v>87</v>
       </c>
       <c r="I59" s="64">
@@ -22660,7 +22776,7 @@
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
-      <c r="H60" s="498"/>
+      <c r="H60" s="504"/>
       <c r="I60" s="65">
         <v>0.13700000000000001</v>
       </c>
@@ -22676,7 +22792,7 @@
       <c r="S60"/>
     </row>
     <row r="61" spans="2:19">
-      <c r="H61" s="499"/>
+      <c r="H61" s="505"/>
       <c r="I61" s="65">
         <v>41.868000000000002</v>
       </c>
@@ -22718,8 +22834,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B2:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -23517,7 +23633,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J25" s="505" t="s">
+      <c r="J25" s="511" t="s">
         <v>139</v>
       </c>
       <c r="M25" s="241" t="s">
@@ -23569,7 +23685,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J26" s="506"/>
+      <c r="J26" s="512"/>
       <c r="L26" s="237"/>
       <c r="M26" s="272"/>
       <c r="N26" s="267"/>
@@ -23609,7 +23725,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J27" s="506"/>
+      <c r="J27" s="512"/>
       <c r="L27" s="230"/>
       <c r="M27" s="239"/>
       <c r="N27" s="239"/>
@@ -23650,7 +23766,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J28" s="506"/>
+      <c r="J28" s="512"/>
       <c r="L28" s="178"/>
     </row>
     <row r="29" spans="2:17">
@@ -23686,7 +23802,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J29" s="506"/>
+      <c r="J29" s="512"/>
       <c r="L29" s="178"/>
     </row>
     <row r="30" spans="2:17">
@@ -23722,7 +23838,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J30" s="506"/>
+      <c r="J30" s="512"/>
       <c r="L30" s="178"/>
     </row>
     <row r="31" spans="2:17">
@@ -23758,7 +23874,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J31" s="506"/>
+      <c r="J31" s="512"/>
       <c r="L31" s="178"/>
     </row>
     <row r="32" spans="2:17">
@@ -23794,7 +23910,7 @@
         <f>SUM($O$25:$P$25)+$Q$25*(Imports_Fossil!O$31/Imports_Fossil!$D$31)</f>
         <v>6.0342803129016236</v>
       </c>
-      <c r="J32" s="507"/>
+      <c r="J32" s="513"/>
       <c r="L32" s="178"/>
     </row>
     <row r="33" spans="2:22">
@@ -23865,7 +23981,7 @@
       <c r="L36" s="43">
         <v>2050</v>
       </c>
-      <c r="M36" s="513">
+      <c r="M36" s="493">
         <v>0</v>
       </c>
       <c r="N36" s="180" t="s">
@@ -23965,7 +24081,7 @@
         <f t="shared" si="9"/>
         <v>2.4623085394510844</v>
       </c>
-      <c r="M38" s="514">
+      <c r="M38" s="494">
         <v>5</v>
       </c>
       <c r="N38" s="143" t="s">
@@ -24033,7 +24149,7 @@
         <f t="shared" si="10"/>
         <v>4.9246170789021688</v>
       </c>
-      <c r="M39" s="515">
+      <c r="M39" s="495">
         <v>5</v>
       </c>
       <c r="N39" s="144" t="s">
@@ -24098,7 +24214,7 @@
         <f t="shared" si="10"/>
         <v>9.8492341578043376</v>
       </c>
-      <c r="M40" s="515">
+      <c r="M40" s="495">
         <v>5</v>
       </c>
       <c r="N40" s="144" t="s">
@@ -24156,7 +24272,7 @@
       <c r="L41" s="128">
         <v>27.064417978971818</v>
       </c>
-      <c r="M41" s="516">
+      <c r="M41" s="496">
         <v>5</v>
       </c>
       <c r="N41" s="145" t="s">
@@ -24200,7 +24316,7 @@
         <f t="shared" si="11"/>
         <v>59.810866344000004</v>
       </c>
-      <c r="M42" s="517"/>
+      <c r="M42" s="497"/>
       <c r="N42" s="146" t="s">
         <v>103</v>
       </c>
@@ -24252,7 +24368,7 @@
         <f t="shared" si="12"/>
         <v>2.855752168393686</v>
       </c>
-      <c r="M43" s="514">
+      <c r="M43" s="494">
         <v>5</v>
       </c>
       <c r="N43" s="143" t="s">
@@ -24308,7 +24424,7 @@
         <f t="shared" si="13"/>
         <v>5.7115043367873719</v>
       </c>
-      <c r="M44" s="515">
+      <c r="M44" s="495">
         <v>5</v>
       </c>
       <c r="N44" s="144" t="s">
@@ -24361,7 +24477,7 @@
         <f t="shared" si="13"/>
         <v>11.423008673574744</v>
       </c>
-      <c r="M45" s="515">
+      <c r="M45" s="495">
         <v>5</v>
       </c>
       <c r="N45" s="144" t="s">
@@ -24414,7 +24530,7 @@
         <f t="shared" si="14"/>
         <v>82.768324715808077</v>
       </c>
-      <c r="M46" s="516">
+      <c r="M46" s="496">
         <v>5</v>
       </c>
       <c r="N46" s="145" t="s">
@@ -24458,7 +24574,7 @@
         <f t="shared" si="15"/>
         <v>102.75858989456388</v>
       </c>
-      <c r="M47" s="517"/>
+      <c r="M47" s="497"/>
       <c r="N47" s="146" t="s">
         <v>271</v>
       </c>
@@ -24510,7 +24626,7 @@
         <f t="shared" si="16"/>
         <v>0.89671505307741584</v>
       </c>
-      <c r="M48" s="514">
+      <c r="M48" s="494">
         <v>5</v>
       </c>
       <c r="N48" s="143" t="s">
@@ -24565,7 +24681,7 @@
         <f t="shared" si="17"/>
         <v>1.7934301061548317</v>
       </c>
-      <c r="M49" s="515">
+      <c r="M49" s="495">
         <v>5</v>
       </c>
       <c r="N49" s="144" t="s">
@@ -24618,7 +24734,7 @@
         <f t="shared" si="17"/>
         <v>3.5868602123096633</v>
       </c>
-      <c r="M50" s="515">
+      <c r="M50" s="495">
         <v>5</v>
       </c>
       <c r="N50" s="144" t="s">
@@ -24671,7 +24787,7 @@
         <f t="shared" si="18"/>
         <v>103.86945463245809</v>
       </c>
-      <c r="M51" s="516">
+      <c r="M51" s="496">
         <v>5</v>
       </c>
       <c r="N51" s="145" t="s">
@@ -24715,7 +24831,7 @@
         <f t="shared" si="19"/>
         <v>110.14646000400001</v>
       </c>
-      <c r="M52" s="517"/>
+      <c r="M52" s="497"/>
       <c r="N52" s="146" t="s">
         <v>103</v>
       </c>
@@ -24767,7 +24883,7 @@
         <f t="shared" si="20"/>
         <v>0.38430645131889257</v>
       </c>
-      <c r="M53" s="514">
+      <c r="M53" s="494">
         <v>5</v>
       </c>
       <c r="N53" s="143" t="s">
@@ -24823,7 +24939,7 @@
         <f t="shared" si="21"/>
         <v>0.76861290263778514</v>
       </c>
-      <c r="M54" s="515">
+      <c r="M54" s="495">
         <v>5</v>
       </c>
       <c r="N54" s="144" t="s">
@@ -24876,7 +24992,7 @@
         <f t="shared" si="21"/>
         <v>1.5372258052755703</v>
       </c>
-      <c r="M55" s="515">
+      <c r="M55" s="495">
         <v>5</v>
       </c>
       <c r="N55" s="144" t="s">
@@ -24929,7 +25045,7 @@
         <f t="shared" si="22"/>
         <v>34.025327552767749</v>
       </c>
-      <c r="M56" s="516">
+      <c r="M56" s="496">
         <v>5</v>
       </c>
       <c r="N56" s="145" t="s">
@@ -24973,7 +25089,7 @@
         <f>K57</f>
         <v>36.715472712</v>
       </c>
-      <c r="M57" s="518"/>
+      <c r="M57" s="498"/>
       <c r="N57" s="147" t="s">
         <v>103</v>
       </c>
@@ -25225,11 +25341,11 @@
       </c>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
-      <c r="E9" s="508" t="s">
+      <c r="E9" s="514" t="s">
         <v>289</v>
       </c>
-      <c r="F9" s="508"/>
-      <c r="G9" s="508"/>
+      <c r="F9" s="514"/>
+      <c r="G9" s="514"/>
       <c r="H9" s="490" t="s">
         <v>288</v>
       </c>
@@ -25594,7 +25710,7 @@
       <c r="E5" s="182">
         <v>10</v>
       </c>
-      <c r="F5" s="509" t="s">
+      <c r="F5" s="515" t="s">
         <v>177</v>
       </c>
       <c r="Q5" s="276"/>
@@ -25615,7 +25731,7 @@
       <c r="E6" s="182">
         <v>10</v>
       </c>
-      <c r="F6" s="510"/>
+      <c r="F6" s="516"/>
       <c r="Q6" s="276"/>
     </row>
     <row r="7" spans="2:17" ht="15">
@@ -25634,7 +25750,7 @@
       <c r="E7" s="182">
         <v>10</v>
       </c>
-      <c r="F7" s="510"/>
+      <c r="F7" s="516"/>
       <c r="Q7" s="276"/>
     </row>
     <row r="8" spans="2:17" ht="15">
@@ -25653,7 +25769,7 @@
       <c r="E8" s="182">
         <v>10</v>
       </c>
-      <c r="F8" s="510"/>
+      <c r="F8" s="516"/>
       <c r="Q8" s="276"/>
     </row>
     <row r="9" spans="2:17" ht="15">
@@ -25672,7 +25788,7 @@
       <c r="E9" s="182">
         <v>10</v>
       </c>
-      <c r="F9" s="510"/>
+      <c r="F9" s="516"/>
       <c r="Q9" s="276"/>
     </row>
     <row r="10" spans="2:17" ht="15">
@@ -25691,7 +25807,7 @@
       <c r="E10" s="182">
         <v>10</v>
       </c>
-      <c r="F10" s="510"/>
+      <c r="F10" s="516"/>
       <c r="Q10" s="276"/>
     </row>
     <row r="11" spans="2:17" ht="15">
@@ -25710,7 +25826,7 @@
       <c r="E11" s="182">
         <v>10</v>
       </c>
-      <c r="F11" s="510"/>
+      <c r="F11" s="516"/>
       <c r="Q11" s="276"/>
     </row>
     <row r="12" spans="2:17" ht="15">
@@ -25729,7 +25845,7 @@
       <c r="E12" s="182">
         <v>10</v>
       </c>
-      <c r="F12" s="510"/>
+      <c r="F12" s="516"/>
       <c r="Q12" s="276"/>
     </row>
     <row r="13" spans="2:17" ht="15">
@@ -25748,7 +25864,7 @@
       <c r="E13" s="182">
         <v>10</v>
       </c>
-      <c r="F13" s="510"/>
+      <c r="F13" s="516"/>
       <c r="Q13" s="276"/>
     </row>
     <row r="14" spans="2:17" ht="15">
@@ -25767,7 +25883,7 @@
       <c r="E14" s="128">
         <v>10</v>
       </c>
-      <c r="F14" s="510"/>
+      <c r="F14" s="516"/>
       <c r="Q14" s="276"/>
     </row>
     <row r="15" spans="2:17" ht="15">
@@ -25786,7 +25902,7 @@
       <c r="E15" s="182">
         <v>10</v>
       </c>
-      <c r="F15" s="510"/>
+      <c r="F15" s="516"/>
       <c r="Q15" s="276"/>
     </row>
     <row r="16" spans="2:17" ht="15">
@@ -25805,7 +25921,7 @@
       <c r="E16" s="182">
         <v>10</v>
       </c>
-      <c r="F16" s="510"/>
+      <c r="F16" s="516"/>
       <c r="Q16" s="276"/>
     </row>
     <row r="17" spans="2:17" ht="15">
@@ -25824,7 +25940,7 @@
       <c r="E17" s="182">
         <v>10</v>
       </c>
-      <c r="F17" s="510"/>
+      <c r="F17" s="516"/>
       <c r="Q17" s="276"/>
     </row>
     <row r="18" spans="2:17" ht="15">
@@ -25843,7 +25959,7 @@
       <c r="E18" s="182">
         <v>10</v>
       </c>
-      <c r="F18" s="510"/>
+      <c r="F18" s="516"/>
       <c r="Q18" s="276"/>
     </row>
     <row r="19" spans="2:17" ht="15">
@@ -25862,7 +25978,7 @@
       <c r="E19" s="182">
         <v>10</v>
       </c>
-      <c r="F19" s="510"/>
+      <c r="F19" s="516"/>
       <c r="Q19" s="276"/>
     </row>
     <row r="20" spans="2:17" ht="15">
@@ -25881,7 +25997,7 @@
       <c r="E20" s="182">
         <v>10</v>
       </c>
-      <c r="F20" s="510"/>
+      <c r="F20" s="516"/>
       <c r="Q20" s="276"/>
     </row>
     <row r="21" spans="2:17">
@@ -25900,7 +26016,7 @@
       <c r="E21" s="182">
         <v>10</v>
       </c>
-      <c r="F21" s="510"/>
+      <c r="F21" s="516"/>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="38" t="str">
@@ -25918,7 +26034,7 @@
       <c r="E22" s="182">
         <v>10</v>
       </c>
-      <c r="F22" s="510"/>
+      <c r="F22" s="516"/>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" s="38" t="str">
@@ -25936,7 +26052,7 @@
       <c r="E23" s="182">
         <v>10</v>
       </c>
-      <c r="F23" s="510"/>
+      <c r="F23" s="516"/>
     </row>
     <row r="24" spans="2:17">
       <c r="B24" s="122" t="str">
@@ -25954,7 +26070,7 @@
       <c r="E24" s="128">
         <v>10</v>
       </c>
-      <c r="F24" s="510"/>
+      <c r="F24" s="516"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="38" t="str">
@@ -25972,7 +26088,7 @@
       <c r="E25" s="182">
         <v>10</v>
       </c>
-      <c r="F25" s="510"/>
+      <c r="F25" s="516"/>
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="38" t="str">
@@ -25990,7 +26106,7 @@
       <c r="E26" s="182">
         <v>10</v>
       </c>
-      <c r="F26" s="510"/>
+      <c r="F26" s="516"/>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="38" t="str">
@@ -26008,7 +26124,7 @@
       <c r="E27" s="182">
         <v>10</v>
       </c>
-      <c r="F27" s="510"/>
+      <c r="F27" s="516"/>
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="38" t="str">
@@ -26026,7 +26142,7 @@
       <c r="E28" s="182">
         <v>10</v>
       </c>
-      <c r="F28" s="510"/>
+      <c r="F28" s="516"/>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="38" t="str">
@@ -26044,7 +26160,7 @@
       <c r="E29" s="182">
         <v>10</v>
       </c>
-      <c r="F29" s="510"/>
+      <c r="F29" s="516"/>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="38" t="str">
@@ -26062,7 +26178,7 @@
       <c r="E30" s="182">
         <v>10</v>
       </c>
-      <c r="F30" s="510"/>
+      <c r="F30" s="516"/>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="38" t="str">
@@ -26080,7 +26196,7 @@
       <c r="E31" s="182">
         <v>10</v>
       </c>
-      <c r="F31" s="510"/>
+      <c r="F31" s="516"/>
     </row>
     <row r="32" spans="2:17">
       <c r="B32" s="38" t="str">
@@ -26098,7 +26214,7 @@
       <c r="E32" s="182">
         <v>10</v>
       </c>
-      <c r="F32" s="510"/>
+      <c r="F32" s="516"/>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="38" t="str">
@@ -26116,7 +26232,7 @@
       <c r="E33" s="182">
         <v>10</v>
       </c>
-      <c r="F33" s="510"/>
+      <c r="F33" s="516"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="122" t="str">
@@ -26134,7 +26250,7 @@
       <c r="E34" s="128">
         <v>10</v>
       </c>
-      <c r="F34" s="511"/>
+      <c r="F34" s="517"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="38"/>
@@ -26239,7 +26355,7 @@
   <dimension ref="B1:AC18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Enable walking and cycling
</commit_message>
<xml_diff>
--- a/VT_IE_SUP.xlsx
+++ b/VT_IE_SUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7857BC-0B38-42E8-9738-327DE3ACCC7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775A9ED1-A716-473A-AF44-F8CC0268B826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONVENTIONS" sheetId="20" r:id="rId1"/>
@@ -790,7 +790,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="514">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -6858,8 +6858,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:T94"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10124,11 +10124,11 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="42" t="str">
-        <f>Processes!C80</f>
+        <f>Processes!C82</f>
         <v>IMPELC_UK</v>
       </c>
       <c r="C5" s="42" t="str">
-        <f>Processes!D80</f>
+        <f>Processes!D82</f>
         <v>Import of Electricity - UK</v>
       </c>
       <c r="E5" s="42" t="str">
@@ -10173,11 +10173,11 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="49" t="str">
-        <f>Processes!C81</f>
+        <f>Processes!C83</f>
         <v>EXPELC_UK</v>
       </c>
       <c r="C6" s="49" t="str">
-        <f>Processes!D81</f>
+        <f>Processes!D83</f>
         <v>Export of Electricity - UK</v>
       </c>
       <c r="D6" s="49" t="str">
@@ -14139,7 +14139,7 @@
     <col min="40" max="16384" width="9.140625" style="242"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="87" thickBot="1">
+    <row r="1" spans="1:39" ht="87.75" thickBot="1">
       <c r="A1" s="336" t="s">
         <v>501</v>
       </c>
@@ -16301,8 +16301,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A26" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17970,10 +17970,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABBFF4F-A0CF-43AC-AC4F-5B8E72D4ACA3}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:V89"/>
+  <dimension ref="B1:V91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19935,198 +19935,198 @@
     </row>
     <row r="80" spans="2:9" s="294" customFormat="1">
       <c r="B80" s="309" t="str">
+        <f>CONVENTIONS!K84</f>
+        <v>MIN</v>
+      </c>
+      <c r="C80" s="309" t="str">
+        <f>CONVENTIONS!E84</f>
+        <v>MINCYC</v>
+      </c>
+      <c r="D80" s="309" t="str">
+        <f>CONVENTIONS!F84</f>
+        <v>Domestic Potential of Cycling</v>
+      </c>
+      <c r="E80" s="323" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="296" t="s">
+        <v>425</v>
+      </c>
+      <c r="G80" s="296"/>
+      <c r="H80" s="296"/>
+      <c r="I80" s="296"/>
+    </row>
+    <row r="81" spans="2:9" s="294" customFormat="1">
+      <c r="B81" s="309" t="str">
+        <f>CONVENTIONS!K85</f>
+        <v>MIN</v>
+      </c>
+      <c r="C81" s="309" t="str">
+        <f>CONVENTIONS!E85</f>
+        <v>MINWLK</v>
+      </c>
+      <c r="D81" s="309" t="str">
+        <f>CONVENTIONS!F85</f>
+        <v>Domestic Potential of Walking</v>
+      </c>
+      <c r="E81" s="323" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="296" t="s">
+        <v>425</v>
+      </c>
+      <c r="G81" s="296"/>
+      <c r="H81" s="296"/>
+      <c r="I81" s="296"/>
+    </row>
+    <row r="82" spans="2:9" s="294" customFormat="1">
+      <c r="B82" s="309" t="str">
         <f>CONVENTIONS!K86</f>
         <v>IMP</v>
       </c>
-      <c r="C80" s="309" t="str">
+      <c r="C82" s="309" t="str">
         <f>CONVENTIONS!E86</f>
         <v>IMPELC_UK</v>
       </c>
-      <c r="D80" s="309" t="str">
+      <c r="D82" s="309" t="str">
         <f>CONVENTIONS!F86</f>
         <v>Import of Electricity - UK</v>
       </c>
-      <c r="E80" s="323" t="s">
+      <c r="E82" s="323" t="s">
         <v>10</v>
       </c>
-      <c r="F80" s="296" t="s">
+      <c r="F82" s="296" t="s">
         <v>425</v>
       </c>
-      <c r="G80" s="296" t="s">
+      <c r="G82" s="296" t="s">
         <v>65</v>
       </c>
-      <c r="H80" s="296"/>
-      <c r="I80" s="296"/>
-    </row>
-    <row r="81" spans="2:9" s="294" customFormat="1">
-      <c r="B81" s="309" t="str">
+      <c r="H82" s="296"/>
+      <c r="I82" s="296"/>
+    </row>
+    <row r="83" spans="2:9" s="294" customFormat="1">
+      <c r="B83" s="309" t="str">
         <f>CONVENTIONS!K87</f>
         <v>EXP</v>
       </c>
-      <c r="C81" s="309" t="str">
+      <c r="C83" s="309" t="str">
         <f>CONVENTIONS!E87</f>
         <v>EXPELC_UK</v>
       </c>
-      <c r="D81" s="309" t="str">
+      <c r="D83" s="309" t="str">
         <f>CONVENTIONS!F87</f>
         <v>Export of Electricity - UK</v>
       </c>
-      <c r="E81" s="323" t="s">
+      <c r="E83" s="323" t="s">
         <v>10</v>
       </c>
-      <c r="F81" s="296" t="s">
+      <c r="F83" s="296" t="s">
         <v>425</v>
       </c>
-      <c r="G81" s="296" t="s">
+      <c r="G83" s="296" t="s">
         <v>65</v>
       </c>
-      <c r="H81" s="296"/>
-      <c r="I81" s="296"/>
-    </row>
-    <row r="82" spans="2:9">
-      <c r="B82" s="309" t="str">
+      <c r="H83" s="296"/>
+      <c r="I83" s="296"/>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="B84" s="309" t="str">
         <f>CONVENTIONS!K88</f>
         <v>PRE</v>
       </c>
-      <c r="C82" s="309" t="str">
+      <c r="C84" s="309" t="str">
         <f>CONVENTIONS!E88</f>
         <v>BDNBIOWOO</v>
       </c>
-      <c r="D82" s="309" t="str">
+      <c r="D84" s="309" t="str">
         <f>CONVENTIONS!F88</f>
         <v xml:space="preserve">Blending of Biomass - generic </v>
       </c>
-      <c r="E82" s="323" t="s">
+      <c r="E84" s="323" t="s">
         <v>10</v>
       </c>
-      <c r="F82" s="296" t="s">
+      <c r="F84" s="296" t="s">
         <v>425</v>
       </c>
-      <c r="G82" s="296"/>
-      <c r="H82" s="328"/>
-      <c r="I82" s="317"/>
-    </row>
-    <row r="83" spans="2:9">
-      <c r="B83" s="309" t="str">
+      <c r="G84" s="296"/>
+      <c r="H84" s="328"/>
+      <c r="I84" s="317"/>
+    </row>
+    <row r="85" spans="2:9">
+      <c r="B85" s="309" t="str">
         <f>CONVENTIONS!K89</f>
         <v>PRE</v>
       </c>
-      <c r="C83" s="309" t="str">
+      <c r="C85" s="309" t="str">
         <f>CONVENTIONS!E89</f>
         <v>SREFOILCRD_Whitegate</v>
       </c>
-      <c r="D83" s="309" t="str">
+      <c r="D85" s="309" t="str">
         <f>CONVENTIONS!F89</f>
         <v>Refinery of Crude Oil  - Whitegate</v>
       </c>
-      <c r="E83" s="323" t="s">
+      <c r="E85" s="323" t="s">
         <v>10</v>
       </c>
-      <c r="F83" s="296" t="s">
+      <c r="F85" s="296" t="s">
         <v>425</v>
       </c>
-      <c r="G83" s="317"/>
-      <c r="H83" s="328" t="str">
+      <c r="G85" s="317"/>
+      <c r="H85" s="328" t="str">
         <f>Commodities!C11</f>
         <v>OILCRD</v>
       </c>
-      <c r="I83" s="317"/>
-    </row>
-    <row r="84" spans="2:9">
-      <c r="B84" s="302" t="s">
+      <c r="I85" s="317"/>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="B86" s="302" t="s">
         <v>424</v>
       </c>
-      <c r="C84" s="306"/>
-      <c r="D84" s="307"/>
-      <c r="E84" s="307"/>
-      <c r="F84" s="307"/>
-      <c r="G84" s="308"/>
-      <c r="H84" s="308"/>
-      <c r="I84" s="308"/>
-    </row>
-    <row r="85" spans="2:9">
-      <c r="B85" s="309" t="str">
+      <c r="C86" s="306"/>
+      <c r="D86" s="307"/>
+      <c r="E86" s="307"/>
+      <c r="F86" s="307"/>
+      <c r="G86" s="308"/>
+      <c r="H86" s="308"/>
+      <c r="I86" s="308"/>
+    </row>
+    <row r="87" spans="2:9">
+      <c r="B87" s="309" t="str">
         <f>CONVENTIONS!K90</f>
         <v>PRE</v>
       </c>
-      <c r="C85" s="309" t="str">
+      <c r="C87" s="309" t="str">
         <f>CONVENTIONS!E90</f>
         <v>FT-SUPNGA</v>
       </c>
-      <c r="D85" s="309" t="str">
+      <c r="D87" s="309" t="str">
         <f>CONVENTIONS!F90</f>
         <v>Fuel Tech - Natural Gas (SUP)</v>
       </c>
-      <c r="E85" s="284" t="s">
+      <c r="E87" s="284" t="s">
         <v>10</v>
       </c>
-      <c r="F85" s="296" t="s">
+      <c r="F87" s="296" t="s">
         <v>425</v>
       </c>
-      <c r="G85" s="317" t="s">
+      <c r="G87" s="317" t="s">
         <v>73</v>
       </c>
-      <c r="H85" s="328"/>
-      <c r="I85" s="317"/>
-    </row>
-    <row r="86" spans="2:9">
-      <c r="B86" s="309" t="str">
+      <c r="H87" s="328"/>
+      <c r="I87" s="317"/>
+    </row>
+    <row r="88" spans="2:9">
+      <c r="B88" s="309" t="str">
         <f>CONVENTIONS!K91</f>
         <v>PRE</v>
       </c>
-      <c r="C86" s="309" t="str">
+      <c r="C88" s="309" t="str">
         <f>CONVENTIONS!E91</f>
         <v>FT-SUPCOA</v>
       </c>
-      <c r="D86" s="309" t="str">
+      <c r="D88" s="309" t="str">
         <f>CONVENTIONS!F91</f>
         <v>Fuel Tech - Coal (SUP)</v>
-      </c>
-      <c r="E86" s="331" t="s">
-        <v>10</v>
-      </c>
-      <c r="F86" s="296" t="s">
-        <v>425</v>
-      </c>
-      <c r="G86" s="310"/>
-      <c r="H86" s="310"/>
-      <c r="I86" s="310"/>
-    </row>
-    <row r="87" spans="2:9">
-      <c r="B87" s="309" t="str">
-        <f>CONVENTIONS!K92</f>
-        <v>PRE</v>
-      </c>
-      <c r="C87" s="309" t="str">
-        <f>CONVENTIONS!E92</f>
-        <v>FT-SUPWAS</v>
-      </c>
-      <c r="D87" s="309" t="str">
-        <f>CONVENTIONS!F92</f>
-        <v>Fuel Tech - Waste (SUP)</v>
-      </c>
-      <c r="E87" s="331" t="s">
-        <v>10</v>
-      </c>
-      <c r="F87" s="296" t="s">
-        <v>425</v>
-      </c>
-      <c r="G87" s="310"/>
-      <c r="H87" s="310"/>
-      <c r="I87" s="310"/>
-    </row>
-    <row r="88" spans="2:9">
-      <c r="B88" s="309" t="str">
-        <f>CONVENTIONS!K93</f>
-        <v>PRE</v>
-      </c>
-      <c r="C88" s="309" t="str">
-        <f>CONVENTIONS!E93</f>
-        <v>FT-SUPBIO</v>
-      </c>
-      <c r="D88" s="309" t="str">
-        <f>CONVENTIONS!F93</f>
-        <v>Fuel Tech - Biomass (SUP)</v>
       </c>
       <c r="E88" s="331" t="s">
         <v>10</v>
@@ -20140,28 +20140,74 @@
     </row>
     <row r="89" spans="2:9">
       <c r="B89" s="309" t="str">
+        <f>CONVENTIONS!K92</f>
+        <v>PRE</v>
+      </c>
+      <c r="C89" s="309" t="str">
+        <f>CONVENTIONS!E92</f>
+        <v>FT-SUPWAS</v>
+      </c>
+      <c r="D89" s="309" t="str">
+        <f>CONVENTIONS!F92</f>
+        <v>Fuel Tech - Waste (SUP)</v>
+      </c>
+      <c r="E89" s="331" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" s="296" t="s">
+        <v>425</v>
+      </c>
+      <c r="G89" s="310"/>
+      <c r="H89" s="310"/>
+      <c r="I89" s="310"/>
+    </row>
+    <row r="90" spans="2:9">
+      <c r="B90" s="309" t="str">
+        <f>CONVENTIONS!K93</f>
+        <v>PRE</v>
+      </c>
+      <c r="C90" s="309" t="str">
+        <f>CONVENTIONS!E93</f>
+        <v>FT-SUPBIO</v>
+      </c>
+      <c r="D90" s="309" t="str">
+        <f>CONVENTIONS!F93</f>
+        <v>Fuel Tech - Biomass (SUP)</v>
+      </c>
+      <c r="E90" s="331" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="296" t="s">
+        <v>425</v>
+      </c>
+      <c r="G90" s="310"/>
+      <c r="H90" s="310"/>
+      <c r="I90" s="310"/>
+    </row>
+    <row r="91" spans="2:9">
+      <c r="B91" s="309" t="str">
         <f>CONVENTIONS!K94</f>
         <v>PRE</v>
       </c>
-      <c r="C89" s="309" t="str">
+      <c r="C91" s="309" t="str">
         <f>CONVENTIONS!E94</f>
         <v>FT-SUPELC</v>
       </c>
-      <c r="D89" s="309" t="str">
+      <c r="D91" s="309" t="str">
         <f>CONVENTIONS!F94</f>
         <v>Fuel Tech - Electricity (SUP)</v>
       </c>
-      <c r="E89" s="284" t="s">
+      <c r="E91" s="284" t="s">
         <v>10</v>
       </c>
-      <c r="F89" s="296" t="s">
+      <c r="F91" s="296" t="s">
         <v>425</v>
       </c>
-      <c r="G89" s="310" t="s">
+      <c r="G91" s="310" t="s">
         <v>65</v>
       </c>
-      <c r="H89" s="310"/>
-      <c r="I89" s="310"/>
+      <c r="H91" s="310"/>
+      <c r="I91" s="310"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20175,7 +20221,7 @@
   <dimension ref="B1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20512,7 +20558,7 @@
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="275" t="str">
-        <f>Processes!C85</f>
+        <f>Processes!C87</f>
         <v>FT-SUPNGA</v>
       </c>
       <c r="C6" s="275" t="str">
@@ -20537,7 +20583,7 @@
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="275" t="str">
-        <f>Processes!C86</f>
+        <f>Processes!C88</f>
         <v>FT-SUPCOA</v>
       </c>
       <c r="C7" s="275" t="str">
@@ -20562,7 +20608,7 @@
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="275" t="str">
-        <f>Processes!C87</f>
+        <f>Processes!C89</f>
         <v>FT-SUPWAS</v>
       </c>
       <c r="C8" s="275" t="str">
@@ -20587,7 +20633,7 @@
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="275" t="str">
-        <f>Processes!C88</f>
+        <f>Processes!C90</f>
         <v>FT-SUPBIO</v>
       </c>
       <c r="C9" s="275" t="str">
@@ -20612,7 +20658,7 @@
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="275" t="str">
-        <f>Processes!C89</f>
+        <f>Processes!C91</f>
         <v>FT-SUPELC</v>
       </c>
       <c r="C10" s="275" t="s">
@@ -25109,8 +25155,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:N23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -25602,9 +25648,18 @@
       <c r="N21" s="204"/>
     </row>
     <row r="22" spans="2:14">
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="B22" s="25" t="str">
+        <f>Processes!C80</f>
+        <v>MINCYC</v>
+      </c>
+      <c r="C22" s="25" t="str">
+        <f>Processes!D80</f>
+        <v>Domestic Potential of Cycling</v>
+      </c>
+      <c r="D22" s="25" t="str">
+        <f>Commodities!C49</f>
+        <v>CYC</v>
+      </c>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
@@ -25617,6 +25672,18 @@
       <c r="N22" s="204"/>
     </row>
     <row r="23" spans="2:14">
+      <c r="B23" s="25" t="str">
+        <f>Processes!C81</f>
+        <v>MINWLK</v>
+      </c>
+      <c r="C23" s="25" t="str">
+        <f>Processes!D81</f>
+        <v>Domestic Potential of Walking</v>
+      </c>
+      <c r="D23" s="25" t="str">
+        <f>Commodities!C50</f>
+        <v>WLK</v>
+      </c>
       <c r="N23" s="204"/>
     </row>
   </sheetData>
@@ -25634,8 +25701,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -26309,11 +26376,11 @@
     </row>
     <row r="40" spans="2:6">
       <c r="B40" s="38" t="str">
-        <f>Processes!C82</f>
+        <f>Processes!C84</f>
         <v>BDNBIOWOO</v>
       </c>
       <c r="C40" s="38" t="str">
-        <f>Processes!D82</f>
+        <f>Processes!D84</f>
         <v xml:space="preserve">Blending of Biomass - generic </v>
       </c>
       <c r="D40" s="38" t="str">
@@ -26485,11 +26552,11 @@
     </row>
     <row r="5" spans="2:25">
       <c r="B5" s="213" t="str">
-        <f>Processes!C83</f>
+        <f>Processes!C85</f>
         <v>SREFOILCRD_Whitegate</v>
       </c>
       <c r="C5" s="213" t="str">
-        <f>Processes!D83</f>
+        <f>Processes!D85</f>
         <v>Refinery of Crude Oil  - Whitegate</v>
       </c>
       <c r="D5" s="214" t="str">
@@ -26949,12 +27016,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -27100,6 +27161,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F399E6-2CA4-4BC3-AE7C-3570BA9F00A0}">
   <ds:schemaRefs>
@@ -27109,15 +27176,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1EBC224-6025-40B6-954C-A60FF473B45B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F32A5943-069C-47E6-B7B1-1C4E8CC11B6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27133,4 +27191,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1EBC224-6025-40B6-954C-A60FF473B45B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add a scenario allowing to cover biogas production in 2018; add info on coal prices in SUP VT
</commit_message>
<xml_diff>
--- a/VT_IE_SUP.xlsx
+++ b/VT_IE_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3CDBB4-4123-4AE6-951D-AE9203DF5C76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA7CACF-7F2F-4BDE-8CE6-EA36BC623440}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="22" r:id="rId1"/>
@@ -801,7 +801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="596">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -2666,6 +2666,27 @@
   </si>
   <si>
     <t>Other_Indexes</t>
+  </si>
+  <si>
+    <t>Coal prices</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/energyexplained/coal/prices-and-outlook.php</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>USD2019/short ton</t>
+  </si>
+  <si>
+    <t>Bituminous</t>
+  </si>
+  <si>
+    <t>lignite</t>
+  </si>
+  <si>
+    <t>anthracite</t>
   </si>
 </sst>
 </file>
@@ -6119,6 +6140,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="121" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="121" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6157,9 +6181,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="121" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7829,8 +7850,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -7917,7 +7938,7 @@
       <c r="F5" s="128">
         <v>10</v>
       </c>
-      <c r="G5" s="503" t="s">
+      <c r="G5" s="504" t="s">
         <v>150</v>
       </c>
       <c r="R5" s="220"/>
@@ -7942,7 +7963,7 @@
       <c r="F6" s="128">
         <v>10</v>
       </c>
-      <c r="G6" s="504"/>
+      <c r="G6" s="505"/>
       <c r="R6" s="220"/>
     </row>
     <row r="7" spans="2:18" ht="15">
@@ -7965,7 +7986,7 @@
       <c r="F7" s="128">
         <v>10</v>
       </c>
-      <c r="G7" s="504"/>
+      <c r="G7" s="505"/>
       <c r="R7" s="220"/>
     </row>
     <row r="8" spans="2:18" ht="15">
@@ -7988,7 +8009,7 @@
       <c r="F8" s="128">
         <v>10</v>
       </c>
-      <c r="G8" s="504"/>
+      <c r="G8" s="505"/>
       <c r="R8" s="220"/>
     </row>
     <row r="9" spans="2:18" ht="15">
@@ -8011,7 +8032,7 @@
       <c r="F9" s="128">
         <v>10</v>
       </c>
-      <c r="G9" s="504"/>
+      <c r="G9" s="505"/>
       <c r="R9" s="220"/>
     </row>
     <row r="10" spans="2:18" ht="15">
@@ -8034,7 +8055,7 @@
       <c r="F10" s="128">
         <v>10</v>
       </c>
-      <c r="G10" s="504"/>
+      <c r="G10" s="505"/>
       <c r="R10" s="220"/>
     </row>
     <row r="11" spans="2:18" ht="15">
@@ -8057,7 +8078,7 @@
       <c r="F11" s="128">
         <v>10</v>
       </c>
-      <c r="G11" s="504"/>
+      <c r="G11" s="505"/>
       <c r="R11" s="220"/>
     </row>
     <row r="12" spans="2:18" ht="15">
@@ -8080,7 +8101,7 @@
       <c r="F12" s="128">
         <v>10</v>
       </c>
-      <c r="G12" s="504"/>
+      <c r="G12" s="505"/>
       <c r="R12" s="220"/>
     </row>
     <row r="13" spans="2:18" ht="15">
@@ -8103,7 +8124,7 @@
       <c r="F13" s="128">
         <v>10</v>
       </c>
-      <c r="G13" s="504"/>
+      <c r="G13" s="505"/>
       <c r="R13" s="220"/>
     </row>
     <row r="14" spans="2:18" ht="15">
@@ -8126,7 +8147,7 @@
       <c r="F14" s="77">
         <v>10</v>
       </c>
-      <c r="G14" s="504"/>
+      <c r="G14" s="505"/>
       <c r="R14" s="220"/>
     </row>
     <row r="15" spans="2:18" ht="15">
@@ -8149,7 +8170,7 @@
       <c r="F15" s="128">
         <v>10</v>
       </c>
-      <c r="G15" s="504"/>
+      <c r="G15" s="505"/>
       <c r="R15" s="220"/>
     </row>
     <row r="16" spans="2:18" ht="15">
@@ -8172,7 +8193,7 @@
       <c r="F16" s="128">
         <v>10</v>
       </c>
-      <c r="G16" s="504"/>
+      <c r="G16" s="505"/>
       <c r="R16" s="220"/>
     </row>
     <row r="17" spans="2:18" ht="15">
@@ -8195,7 +8216,7 @@
       <c r="F17" s="128">
         <v>10</v>
       </c>
-      <c r="G17" s="504"/>
+      <c r="G17" s="505"/>
       <c r="R17" s="220"/>
     </row>
     <row r="18" spans="2:18" ht="15">
@@ -8218,7 +8239,7 @@
       <c r="F18" s="128">
         <v>10</v>
       </c>
-      <c r="G18" s="504"/>
+      <c r="G18" s="505"/>
       <c r="R18" s="220"/>
     </row>
     <row r="19" spans="2:18" ht="15">
@@ -8241,7 +8262,7 @@
       <c r="F19" s="128">
         <v>10</v>
       </c>
-      <c r="G19" s="504"/>
+      <c r="G19" s="505"/>
       <c r="R19" s="220"/>
     </row>
     <row r="20" spans="2:18" ht="15">
@@ -8264,7 +8285,7 @@
       <c r="F20" s="128">
         <v>10</v>
       </c>
-      <c r="G20" s="504"/>
+      <c r="G20" s="505"/>
       <c r="R20" s="220"/>
     </row>
     <row r="21" spans="2:18">
@@ -8287,7 +8308,7 @@
       <c r="F21" s="128">
         <v>10</v>
       </c>
-      <c r="G21" s="504"/>
+      <c r="G21" s="505"/>
     </row>
     <row r="22" spans="2:18">
       <c r="B22" s="33" t="str">
@@ -8309,7 +8330,7 @@
       <c r="F22" s="128">
         <v>10</v>
       </c>
-      <c r="G22" s="504"/>
+      <c r="G22" s="505"/>
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="33" t="str">
@@ -8331,7 +8352,7 @@
       <c r="F23" s="128">
         <v>10</v>
       </c>
-      <c r="G23" s="504"/>
+      <c r="G23" s="505"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="71" t="str">
@@ -8353,7 +8374,7 @@
       <c r="F24" s="77">
         <v>10</v>
       </c>
-      <c r="G24" s="504"/>
+      <c r="G24" s="505"/>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="33" t="str">
@@ -8375,7 +8396,7 @@
       <c r="F25" s="128">
         <v>10</v>
       </c>
-      <c r="G25" s="504"/>
+      <c r="G25" s="505"/>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="33" t="str">
@@ -8397,7 +8418,7 @@
       <c r="F26" s="128">
         <v>10</v>
       </c>
-      <c r="G26" s="504"/>
+      <c r="G26" s="505"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="33" t="str">
@@ -8419,7 +8440,7 @@
       <c r="F27" s="128">
         <v>10</v>
       </c>
-      <c r="G27" s="504"/>
+      <c r="G27" s="505"/>
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="33" t="str">
@@ -8441,7 +8462,7 @@
       <c r="F28" s="128">
         <v>10</v>
       </c>
-      <c r="G28" s="504"/>
+      <c r="G28" s="505"/>
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="33" t="str">
@@ -8463,7 +8484,7 @@
       <c r="F29" s="128">
         <v>10</v>
       </c>
-      <c r="G29" s="504"/>
+      <c r="G29" s="505"/>
     </row>
     <row r="30" spans="2:18">
       <c r="B30" s="33" t="str">
@@ -8485,7 +8506,7 @@
       <c r="F30" s="128">
         <v>10</v>
       </c>
-      <c r="G30" s="504"/>
+      <c r="G30" s="505"/>
     </row>
     <row r="31" spans="2:18">
       <c r="B31" s="33" t="str">
@@ -8507,7 +8528,7 @@
       <c r="F31" s="128">
         <v>10</v>
       </c>
-      <c r="G31" s="504"/>
+      <c r="G31" s="505"/>
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="33" t="str">
@@ -8529,7 +8550,7 @@
       <c r="F32" s="128">
         <v>10</v>
       </c>
-      <c r="G32" s="504"/>
+      <c r="G32" s="505"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="33" t="str">
@@ -8551,7 +8572,7 @@
       <c r="F33" s="128">
         <v>10</v>
       </c>
-      <c r="G33" s="504"/>
+      <c r="G33" s="505"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="71" t="str">
@@ -8573,7 +8594,7 @@
       <c r="F34" s="77">
         <v>10</v>
       </c>
-      <c r="G34" s="505"/>
+      <c r="G34" s="506"/>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="33"/>
@@ -8691,7 +8712,7 @@
   <dimension ref="B1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9696,20 +9717,20 @@
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="G7" s="502" t="s">
+      <c r="G7" s="503" t="s">
         <v>167</v>
       </c>
-      <c r="H7" s="502"/>
-      <c r="I7" s="502"/>
-      <c r="J7" s="502"/>
-      <c r="K7" s="502"/>
+      <c r="H7" s="503"/>
+      <c r="I7" s="503"/>
+      <c r="J7" s="503"/>
+      <c r="K7" s="503"/>
       <c r="L7" s="275" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="502" t="s">
+      <c r="M7" s="503" t="s">
         <v>236</v>
       </c>
-      <c r="N7" s="502"/>
+      <c r="N7" s="503"/>
       <c r="O7" s="52"/>
     </row>
     <row r="9" spans="2:20">
@@ -10458,10 +10479,10 @@
   </sheetPr>
   <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="D3" sqref="D3"/>
-      <selection pane="topRight" activeCell="G13" sqref="G13"/>
+      <selection pane="topRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10487,10 +10508,10 @@
       <c r="J1" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="506" t="s">
+      <c r="P1" s="507" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="506"/>
+      <c r="Q1" s="507"/>
     </row>
     <row r="2" spans="1:22">
       <c r="H2" s="88"/>
@@ -13562,7 +13583,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -13687,7 +13708,7 @@
       <selection activeCell="A65" sqref="A65:XFD65"/>
       <selection pane="topRight" activeCell="A65" sqref="A65:XFD65"/>
       <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="AE43" sqref="AE43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -16296,16 +16317,10 @@
       </c>
     </row>
     <row r="39" spans="14:16">
-      <c r="P39" s="443">
-        <f>('EB2018'!P$20-'EB2018'!P$25)/(SUM('EB2018'!$O$20:$Z$20)-SUM('EB2018'!$O$25:$Z$25))</f>
-        <v>0.20874581836826736</v>
-      </c>
+      <c r="P39" s="443"/>
     </row>
     <row r="40" spans="14:16">
-      <c r="N40" s="442">
-        <f>(SUM('EB2018'!O20:Z20)-SUM('EB2018'!O25:Z25))/'EB2018'!M14</f>
-        <v>0.9923342574100722</v>
-      </c>
+      <c r="N40" s="442"/>
     </row>
   </sheetData>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.59055118110236227" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.19685039370078741"/>
@@ -16324,7 +16339,7 @@
   <dimension ref="B2:T97"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19571,8 +19586,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:L97"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -21282,7 +21297,7 @@
   <dimension ref="B1:W94"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24480,8 +24495,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24507,15 +24522,15 @@
     <col min="26" max="16384" width="9.140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="18.75">
+    <row r="1" spans="2:20" ht="18.75">
       <c r="B1" s="11" t="s">
         <v>567</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="2:18" s="219" customFormat="1"/>
-    <row r="3" spans="2:18" ht="18.75">
+    <row r="2" spans="2:20" s="219" customFormat="1"/>
+    <row r="3" spans="2:20" ht="18.75">
       <c r="G3" s="479" t="s">
         <v>586</v>
       </c>
@@ -24531,7 +24546,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="2:18">
+    <row r="4" spans="2:20">
       <c r="C4" s="17" t="s">
         <v>536</v>
       </c>
@@ -24569,7 +24584,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="26.25" thickBot="1">
+    <row r="5" spans="2:20" ht="26.25" thickBot="1">
       <c r="C5" s="10" t="s">
         <v>538</v>
       </c>
@@ -24603,7 +24618,7 @@
       </c>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="2:18">
+    <row r="6" spans="2:20">
       <c r="C6" s="481" t="str">
         <f>Processes!C11</f>
         <v>IE,National</v>
@@ -24651,7 +24666,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="7" spans="2:18">
+    <row r="7" spans="2:20">
       <c r="C7" s="481" t="str">
         <f>Processes!C19</f>
         <v>IE,National</v>
@@ -24698,8 +24713,14 @@
       <c r="N7" s="218" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="8" spans="2:18">
+      <c r="R7" s="37" t="s">
+        <v>589</v>
+      </c>
+      <c r="T7" s="219" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
       <c r="C8" s="485" t="str">
         <f>Processes!C8</f>
         <v>IE,National</v>
@@ -24747,7 +24768,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="2:18">
+    <row r="9" spans="2:20">
       <c r="C9" s="481" t="str">
         <f>Processes!C7</f>
         <v>IE,National</v>
@@ -24768,34 +24789,40 @@
         <v>COABIT</v>
       </c>
       <c r="H9" s="483">
-        <f>H$8*$N$9</f>
+        <f t="shared" ref="H9:M9" si="0">H$8*$N$9</f>
         <v>1.7676490662378885</v>
       </c>
       <c r="I9" s="483">
-        <f>I$8*$N$9</f>
+        <f t="shared" si="0"/>
         <v>1.2363943607780541</v>
       </c>
       <c r="J9" s="483">
-        <f>J$8*$N$9</f>
+        <f t="shared" si="0"/>
         <v>1.3174694008290742</v>
       </c>
       <c r="K9" s="483">
-        <f>K$8*$N$9</f>
+        <f t="shared" si="0"/>
         <v>1.6215008010203991</v>
       </c>
       <c r="L9" s="483">
-        <f>L$8*$N$9</f>
+        <f t="shared" si="0"/>
         <v>1.7836508811224392</v>
       </c>
       <c r="M9" s="483">
-        <f>M$8*$N$9</f>
+        <f t="shared" si="0"/>
         <v>1.962015969234683</v>
       </c>
       <c r="N9" s="487">
         <v>0.95000000000000495</v>
       </c>
-    </row>
-    <row r="10" spans="2:18">
+      <c r="R9" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="S9" s="37" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
       <c r="C10" s="481" t="str">
         <f>Processes!C9</f>
         <v>IE,National</v>
@@ -24816,34 +24843,40 @@
         <v>COACOK</v>
       </c>
       <c r="H10" s="483">
-        <f>H$8*$N10</f>
+        <f t="shared" ref="H10:M11" si="1">H$8*$N10</f>
         <v>2.3630676990759136</v>
       </c>
       <c r="I10" s="483">
-        <f>I$8*$N10</f>
+        <f t="shared" si="1"/>
         <v>1.6528640401980297</v>
       </c>
       <c r="J10" s="483">
-        <f>J$8*$N10</f>
+        <f t="shared" si="1"/>
         <v>1.7612485674241301</v>
       </c>
       <c r="K10" s="483">
-        <f>K$8*$N10</f>
+        <f t="shared" si="1"/>
         <v>2.1676905445220065</v>
       </c>
       <c r="L10" s="483">
-        <f>L$8*$N10</f>
+        <f t="shared" si="1"/>
         <v>2.3844595989742072</v>
       </c>
       <c r="M10" s="483">
-        <f>M$8*$N10</f>
+        <f t="shared" si="1"/>
         <v>2.6229055588716279</v>
       </c>
       <c r="N10" s="488">
         <v>1.2700000000000062</v>
       </c>
-    </row>
-    <row r="11" spans="2:18">
+      <c r="R10" s="37" t="s">
+        <v>593</v>
+      </c>
+      <c r="S10" s="37">
+        <v>58.93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
       <c r="C11" s="481" t="str">
         <f>Processes!C10</f>
         <v>IE,National</v>
@@ -24864,34 +24897,40 @@
         <v>COALIG</v>
       </c>
       <c r="H11" s="483">
-        <f>H$8*$N11</f>
+        <f t="shared" si="1"/>
         <v>1.6291696463022047</v>
       </c>
       <c r="I11" s="483">
-        <f>I$8*$N11</f>
+        <f t="shared" si="1"/>
         <v>1.1395339730673333</v>
       </c>
       <c r="J11" s="483">
-        <f>J$8*$N11</f>
+        <f t="shared" si="1"/>
         <v>1.2142575122848633</v>
       </c>
       <c r="K11" s="483">
-        <f>K$8*$N11</f>
+        <f t="shared" si="1"/>
         <v>1.4944707843506013</v>
       </c>
       <c r="L11" s="483">
-        <f>L$8*$N11</f>
+        <f t="shared" si="1"/>
         <v>1.6439178627856614</v>
       </c>
       <c r="M11" s="483">
-        <f>M$8*$N11</f>
+        <f t="shared" si="1"/>
         <v>1.8083096490642274</v>
       </c>
       <c r="N11" s="488">
         <v>0.87557603686636576</v>
       </c>
-    </row>
-    <row r="12" spans="2:18">
+      <c r="R11" s="37" t="s">
+        <v>594</v>
+      </c>
+      <c r="S11" s="37">
+        <v>19.86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20">
       <c r="C12" s="481" t="str">
         <f>Processes!C20</f>
         <v>IE,National</v>
@@ -24912,34 +24951,40 @@
         <v>GASLNG</v>
       </c>
       <c r="H12" s="483">
-        <f>H$7*$N12</f>
+        <f t="shared" ref="H12:M12" si="2">H$7*$N12</f>
         <v>6.5078020231419309</v>
       </c>
       <c r="I12" s="483">
-        <f>I$7*$N12</f>
+        <f t="shared" si="2"/>
         <v>6.0522171624172225</v>
       </c>
       <c r="J12" s="483">
-        <f>J$7*$N12</f>
+        <f t="shared" si="2"/>
         <v>6.5942067590516009</v>
       </c>
       <c r="K12" s="483">
-        <f>K$7*$N12</f>
+        <f t="shared" si="2"/>
         <v>10.026807537735994</v>
       </c>
       <c r="L12" s="483">
-        <f>L$7*$N12</f>
+        <f t="shared" si="2"/>
         <v>11.743107927078192</v>
       </c>
       <c r="M12" s="483">
-        <f>M$7*$N12</f>
+        <f t="shared" si="2"/>
         <v>13.753189464145629</v>
       </c>
       <c r="N12" s="488">
         <v>1.0669585115925122</v>
       </c>
-    </row>
-    <row r="13" spans="2:18">
+      <c r="R12" s="37" t="s">
+        <v>595</v>
+      </c>
+      <c r="S12" s="37">
+        <v>102.22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
       <c r="C13" s="481" t="str">
         <f>Processes!C14</f>
         <v>IE,National</v>
@@ -24960,34 +25005,34 @@
         <v>OILDST</v>
       </c>
       <c r="H13" s="483">
-        <f>H$6*$N13</f>
+        <f t="shared" ref="H13:M18" si="3">H$6*$N13</f>
         <v>15.417783022591095</v>
       </c>
       <c r="I13" s="483">
-        <f>I$6*$N13</f>
+        <f t="shared" si="3"/>
         <v>15.068586863377233</v>
       </c>
       <c r="J13" s="483">
-        <f>J$6*$N13</f>
+        <f t="shared" si="3"/>
         <v>16.982058211107677</v>
       </c>
       <c r="K13" s="483">
-        <f>K$6*$N13</f>
+        <f t="shared" si="3"/>
         <v>18.177977803439202</v>
       </c>
       <c r="L13" s="483">
-        <f>L$6*$N13</f>
+        <f t="shared" si="3"/>
         <v>19.373897395770726</v>
       </c>
       <c r="M13" s="483">
-        <f>M$6*$N13</f>
+        <f t="shared" si="3"/>
         <v>20.330633069635947</v>
       </c>
       <c r="N13" s="488">
         <v>1.5294117647058842</v>
       </c>
     </row>
-    <row r="14" spans="2:18">
+    <row r="14" spans="2:20">
       <c r="C14" s="481" t="str">
         <f>Processes!C16</f>
         <v>IE,National</v>
@@ -25008,34 +25053,34 @@
         <v>OILGSL</v>
       </c>
       <c r="H14" s="483">
-        <f>H$6*$N14</f>
+        <f t="shared" si="3"/>
         <v>16.603766332021141</v>
       </c>
       <c r="I14" s="483">
-        <f>I$6*$N14</f>
+        <f t="shared" si="3"/>
         <v>16.227708929790829</v>
       </c>
       <c r="J14" s="483">
-        <f>J$6*$N14</f>
+        <f t="shared" si="3"/>
         <v>18.288370381192841</v>
       </c>
       <c r="K14" s="483">
-        <f>K$6*$N14</f>
+        <f t="shared" si="3"/>
         <v>19.576283788319095</v>
       </c>
       <c r="L14" s="483">
-        <f>L$6*$N14</f>
+        <f t="shared" si="3"/>
         <v>20.864197195445353</v>
       </c>
       <c r="M14" s="483">
-        <f>M$6*$N14</f>
+        <f t="shared" si="3"/>
         <v>21.894527921146356</v>
       </c>
       <c r="N14" s="488">
         <v>1.6470588235294101</v>
       </c>
     </row>
-    <row r="15" spans="2:18">
+    <row r="15" spans="2:20">
       <c r="C15" s="481" t="str">
         <f>Processes!C13</f>
         <v>IE,National</v>
@@ -25056,34 +25101,34 @@
         <v>OILHFO</v>
       </c>
       <c r="H15" s="483">
-        <f>H$6*$N15</f>
+        <f t="shared" si="3"/>
         <v>8.165495085426107</v>
       </c>
       <c r="I15" s="483">
-        <f>I$6*$N15</f>
+        <f t="shared" si="3"/>
         <v>7.9805554272578423</v>
       </c>
       <c r="J15" s="483">
-        <f>J$6*$N15</f>
+        <f t="shared" si="3"/>
         <v>8.9939592910366173</v>
       </c>
       <c r="K15" s="483">
-        <f>K$6*$N15</f>
+        <f t="shared" si="3"/>
         <v>9.6273367058983492</v>
       </c>
       <c r="L15" s="483">
-        <f>L$6*$N15</f>
+        <f t="shared" si="3"/>
         <v>10.260714120760083</v>
       </c>
       <c r="M15" s="483">
-        <f>M$6*$N15</f>
+        <f t="shared" si="3"/>
         <v>10.76741605264947</v>
       </c>
       <c r="N15" s="488">
         <v>0.80999999999999872</v>
       </c>
     </row>
-    <row r="16" spans="2:18">
+    <row r="16" spans="2:20">
       <c r="C16" s="481" t="str">
         <f>Processes!C12</f>
         <v>IE,National</v>
@@ -25104,27 +25149,27 @@
         <v>OILKER</v>
       </c>
       <c r="H16" s="483">
-        <f>H$6*$N16</f>
+        <f t="shared" si="3"/>
         <v>16.603766332021141</v>
       </c>
       <c r="I16" s="483">
-        <f>I$6*$N16</f>
+        <f t="shared" si="3"/>
         <v>16.227708929790829</v>
       </c>
       <c r="J16" s="483">
-        <f>J$6*$N16</f>
+        <f t="shared" si="3"/>
         <v>18.288370381192841</v>
       </c>
       <c r="K16" s="483">
-        <f>K$6*$N16</f>
+        <f t="shared" si="3"/>
         <v>19.576283788319095</v>
       </c>
       <c r="L16" s="483">
-        <f>L$6*$N16</f>
+        <f t="shared" si="3"/>
         <v>20.864197195445353</v>
       </c>
       <c r="M16" s="483">
-        <f>M$6*$N16</f>
+        <f t="shared" si="3"/>
         <v>21.894527921146356</v>
       </c>
       <c r="N16" s="488">
@@ -25152,27 +25197,27 @@
         <v>OILLPG</v>
       </c>
       <c r="H17" s="484">
-        <f>H$6*$N17</f>
+        <f t="shared" si="3"/>
         <v>13.045816403730882</v>
       </c>
       <c r="I17" s="484">
-        <f>I$6*$N17</f>
+        <f t="shared" si="3"/>
         <v>12.750342730549923</v>
       </c>
       <c r="J17" s="484">
-        <f>J$6*$N17</f>
+        <f t="shared" si="3"/>
         <v>14.369433870937215</v>
       </c>
       <c r="K17" s="484">
-        <f>K$6*$N17</f>
+        <f t="shared" si="3"/>
         <v>15.381365833679272</v>
       </c>
       <c r="L17" s="484">
-        <f>L$6*$N17</f>
+        <f t="shared" si="3"/>
         <v>16.393297796421329</v>
       </c>
       <c r="M17" s="484">
-        <f>M$6*$N17</f>
+        <f t="shared" si="3"/>
         <v>17.202843366614974</v>
       </c>
       <c r="N17" s="488">
@@ -25200,27 +25245,27 @@
         <v>OILCOK</v>
       </c>
       <c r="H18" s="483">
-        <f>H$6*$N18</f>
+        <f t="shared" si="3"/>
         <v>16.603766332021141</v>
       </c>
       <c r="I18" s="483">
-        <f>I$6*$N18</f>
+        <f t="shared" si="3"/>
         <v>16.227708929790829</v>
       </c>
       <c r="J18" s="483">
-        <f>J$6*$N18</f>
+        <f t="shared" si="3"/>
         <v>18.288370381192841</v>
       </c>
       <c r="K18" s="483">
-        <f>K$6*$N18</f>
+        <f t="shared" si="3"/>
         <v>19.576283788319095</v>
       </c>
       <c r="L18" s="483">
-        <f>L$6*$N18</f>
+        <f t="shared" si="3"/>
         <v>20.864197195445353</v>
       </c>
       <c r="M18" s="483">
-        <f>M$6*$N18</f>
+        <f t="shared" si="3"/>
         <v>21.894527921146356</v>
       </c>
       <c r="N18" s="489">
@@ -25240,7 +25285,7 @@
         <f>Processes!E21</f>
         <v>Import of Uranium</v>
       </c>
-      <c r="F19" s="507" t="s">
+      <c r="F19" s="494" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="490" t="str">
@@ -25268,7 +25313,7 @@
         <f>Processes!E18</f>
         <v>Import of Oil for Non-Energy uses</v>
       </c>
-      <c r="F20" s="507" t="s">
+      <c r="F20" s="494" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="493" t="str">
@@ -25276,27 +25321,27 @@
         <v>OILNEU</v>
       </c>
       <c r="H20" s="491">
-        <f t="shared" ref="H20" si="0">H6</f>
+        <f t="shared" ref="H20" si="4">H6</f>
         <v>10.080858130155704</v>
       </c>
       <c r="I20" s="491">
-        <f t="shared" ref="I20:M20" si="1">I6</f>
+        <f t="shared" ref="I20:M20" si="5">I6</f>
         <v>9.8525375645158704</v>
       </c>
       <c r="J20" s="491">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>11.103653445724236</v>
       </c>
       <c r="K20" s="491">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>11.885600871479463</v>
       </c>
       <c r="L20" s="491">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>12.66754829723469</v>
       </c>
       <c r="M20" s="491">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13.293106237838872</v>
       </c>
       <c r="N20" s="493"/>
@@ -25367,20 +25412,20 @@
       <c r="D24" s="468"/>
       <c r="E24" s="468"/>
       <c r="F24" s="469"/>
-      <c r="G24" s="494" t="s">
+      <c r="G24" s="495" t="s">
         <v>550</v>
       </c>
-      <c r="H24" s="494"/>
-      <c r="I24" s="494"/>
-      <c r="J24" s="495"/>
-      <c r="K24" s="496" t="s">
+      <c r="H24" s="495"/>
+      <c r="I24" s="495"/>
+      <c r="J24" s="496"/>
+      <c r="K24" s="497" t="s">
         <v>551</v>
       </c>
-      <c r="L24" s="497"/>
-      <c r="M24" s="498" t="s">
+      <c r="L24" s="498"/>
+      <c r="M24" s="499" t="s">
         <v>552</v>
       </c>
-      <c r="N24" s="497"/>
+      <c r="N24" s="498"/>
       <c r="S24"/>
     </row>
     <row r="25" spans="3:21">
@@ -25583,39 +25628,39 @@
         <v>2010</v>
       </c>
       <c r="F31" s="480">
-        <f t="shared" ref="F31:N31" si="2">F25</f>
+        <f t="shared" ref="F31:N31" si="6">F25</f>
         <v>2019</v>
       </c>
       <c r="G31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2025</v>
       </c>
       <c r="H31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2030</v>
       </c>
       <c r="I31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2035</v>
       </c>
       <c r="J31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2040</v>
       </c>
       <c r="K31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2025</v>
       </c>
       <c r="L31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2040</v>
       </c>
       <c r="M31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2025</v>
       </c>
       <c r="N31" s="480">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2040</v>
       </c>
       <c r="O31" s="58"/>
@@ -25795,39 +25840,39 @@
         <v>2010</v>
       </c>
       <c r="F36" s="480">
-        <f t="shared" ref="F36:N36" si="3">F25</f>
+        <f t="shared" ref="F36:N36" si="7">F25</f>
         <v>2019</v>
       </c>
       <c r="G36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2025</v>
       </c>
       <c r="H36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2030</v>
       </c>
       <c r="I36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2035</v>
       </c>
       <c r="J36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2040</v>
       </c>
       <c r="K36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2025</v>
       </c>
       <c r="L36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2040</v>
       </c>
       <c r="M36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2025</v>
       </c>
       <c r="N36" s="480">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2040</v>
       </c>
       <c r="O36" s="59"/>
@@ -26023,20 +26068,20 @@
       <c r="D42" s="468"/>
       <c r="E42" s="468"/>
       <c r="F42" s="469"/>
-      <c r="G42" s="494" t="s">
+      <c r="G42" s="495" t="s">
         <v>550</v>
       </c>
-      <c r="H42" s="494"/>
-      <c r="I42" s="494"/>
-      <c r="J42" s="495"/>
-      <c r="K42" s="496" t="s">
+      <c r="H42" s="495"/>
+      <c r="I42" s="495"/>
+      <c r="J42" s="496"/>
+      <c r="K42" s="497" t="s">
         <v>551</v>
       </c>
-      <c r="L42" s="497"/>
-      <c r="M42" s="498" t="s">
+      <c r="L42" s="498"/>
+      <c r="M42" s="499" t="s">
         <v>584</v>
       </c>
-      <c r="N42" s="497"/>
+      <c r="N42" s="498"/>
       <c r="O42"/>
     </row>
     <row r="43" spans="3:20">
@@ -26247,39 +26292,39 @@
         <v>2010</v>
       </c>
       <c r="F49" s="480">
-        <f t="shared" ref="F49:N49" si="4">F43</f>
+        <f t="shared" ref="F49:N49" si="8">F43</f>
         <v>2018</v>
       </c>
       <c r="G49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="H49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2030</v>
       </c>
       <c r="I49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2035</v>
       </c>
       <c r="J49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2040</v>
       </c>
       <c r="K49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="L49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2040</v>
       </c>
       <c r="M49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="N49" s="480">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2040</v>
       </c>
       <c r="O49"/>
@@ -26469,39 +26514,39 @@
         <v>2010</v>
       </c>
       <c r="F54" s="480">
-        <f t="shared" ref="F54:N54" si="5">F43</f>
+        <f t="shared" ref="F54:N54" si="9">F43</f>
         <v>2018</v>
       </c>
       <c r="G54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="H54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2030</v>
       </c>
       <c r="I54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2035</v>
       </c>
       <c r="J54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2040</v>
       </c>
       <c r="K54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="L54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2040</v>
       </c>
       <c r="M54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="N54" s="480">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2040</v>
       </c>
       <c r="O54"/>
@@ -26855,7 +26900,7 @@
   <dimension ref="B2:W58"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -27774,7 +27819,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K26" s="499" t="s">
+      <c r="K26" s="500" t="s">
         <v>122</v>
       </c>
       <c r="N26" s="187" t="s">
@@ -27830,7 +27875,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K27" s="500"/>
+      <c r="K27" s="501"/>
       <c r="M27" s="183"/>
       <c r="N27" s="216"/>
       <c r="O27" s="212"/>
@@ -27874,7 +27919,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K28" s="500"/>
+      <c r="K28" s="501"/>
       <c r="M28" s="176"/>
       <c r="N28" s="185"/>
       <c r="O28" s="185"/>
@@ -27919,7 +27964,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K29" s="500"/>
+      <c r="K29" s="501"/>
       <c r="M29" s="124"/>
     </row>
     <row r="30" spans="2:18">
@@ -27959,7 +28004,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K30" s="500"/>
+      <c r="K30" s="501"/>
       <c r="M30" s="124"/>
     </row>
     <row r="31" spans="2:18">
@@ -27999,7 +28044,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K31" s="500"/>
+      <c r="K31" s="501"/>
       <c r="M31" s="124"/>
     </row>
     <row r="32" spans="2:18">
@@ -28039,7 +28084,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K32" s="500"/>
+      <c r="K32" s="501"/>
       <c r="M32" s="124"/>
     </row>
     <row r="33" spans="2:23">
@@ -28079,7 +28124,7 @@
         <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K33" s="501"/>
+      <c r="K33" s="502"/>
       <c r="M33" s="124"/>
     </row>
     <row r="34" spans="2:23">
@@ -29354,7 +29399,7 @@
   <dimension ref="B2:O24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -29610,11 +29655,11 @@
       <c r="C9" s="52"/>
       <c r="D9" s="52"/>
       <c r="E9" s="52"/>
-      <c r="F9" s="502" t="s">
+      <c r="F9" s="503" t="s">
         <v>239</v>
       </c>
-      <c r="G9" s="502"/>
-      <c r="H9" s="502"/>
+      <c r="G9" s="503"/>
+      <c r="H9" s="503"/>
       <c r="I9" s="274" t="s">
         <v>238</v>
       </c>
@@ -29977,9 +30022,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30129,26 +30177,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1EBC224-6025-40B6-954C-A60FF473B45B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F399E6-2CA4-4BC3-AE7C-3570BA9F00A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30172,9 +30209,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F399E6-2CA4-4BC3-AE7C-3570BA9F00A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1EBC224-6025-40B6-954C-A60FF473B45B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update currency unit for biojet kerosene import
</commit_message>
<xml_diff>
--- a/VT_IE_SUP.xlsx
+++ b/VT_IE_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8149A3BC-04D7-461D-B0CA-68560E127D3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F3D9E-8AA2-4950-9189-F7996A8BE915}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="22" r:id="rId1"/>
@@ -801,7 +801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="595">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -2678,6 +2678,12 @@
   </si>
   <si>
     <t>anthracite</t>
+  </si>
+  <si>
+    <t>assumed 60% higher than kerosene</t>
+  </si>
+  <si>
+    <t>Import/Export</t>
   </si>
 </sst>
 </file>
@@ -4821,7 +4827,7 @@
     <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="507">
+  <cellXfs count="508">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6130,6 +6136,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="121" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7926,7 +7935,7 @@
       <c r="F5" s="128">
         <v>10</v>
       </c>
-      <c r="G5" s="503" t="s">
+      <c r="G5" s="504" t="s">
         <v>150</v>
       </c>
       <c r="R5" s="220"/>
@@ -7951,7 +7960,7 @@
       <c r="F6" s="128">
         <v>10</v>
       </c>
-      <c r="G6" s="504"/>
+      <c r="G6" s="505"/>
       <c r="R6" s="220"/>
     </row>
     <row r="7" spans="2:18" ht="15">
@@ -7974,7 +7983,7 @@
       <c r="F7" s="128">
         <v>10</v>
       </c>
-      <c r="G7" s="504"/>
+      <c r="G7" s="505"/>
       <c r="R7" s="220"/>
     </row>
     <row r="8" spans="2:18" ht="15">
@@ -7997,7 +8006,7 @@
       <c r="F8" s="128">
         <v>10</v>
       </c>
-      <c r="G8" s="504"/>
+      <c r="G8" s="505"/>
       <c r="R8" s="220"/>
     </row>
     <row r="9" spans="2:18" ht="15">
@@ -8020,7 +8029,7 @@
       <c r="F9" s="128">
         <v>10</v>
       </c>
-      <c r="G9" s="504"/>
+      <c r="G9" s="505"/>
       <c r="R9" s="220"/>
     </row>
     <row r="10" spans="2:18" ht="15">
@@ -8043,7 +8052,7 @@
       <c r="F10" s="128">
         <v>10</v>
       </c>
-      <c r="G10" s="504"/>
+      <c r="G10" s="505"/>
       <c r="R10" s="220"/>
     </row>
     <row r="11" spans="2:18" ht="15">
@@ -8066,7 +8075,7 @@
       <c r="F11" s="128">
         <v>10</v>
       </c>
-      <c r="G11" s="504"/>
+      <c r="G11" s="505"/>
       <c r="R11" s="220"/>
     </row>
     <row r="12" spans="2:18" ht="15">
@@ -8089,7 +8098,7 @@
       <c r="F12" s="128">
         <v>10</v>
       </c>
-      <c r="G12" s="504"/>
+      <c r="G12" s="505"/>
       <c r="R12" s="220"/>
     </row>
     <row r="13" spans="2:18" ht="15">
@@ -8112,7 +8121,7 @@
       <c r="F13" s="128">
         <v>10</v>
       </c>
-      <c r="G13" s="504"/>
+      <c r="G13" s="505"/>
       <c r="R13" s="220"/>
     </row>
     <row r="14" spans="2:18" ht="15">
@@ -8135,7 +8144,7 @@
       <c r="F14" s="77">
         <v>10</v>
       </c>
-      <c r="G14" s="504"/>
+      <c r="G14" s="505"/>
       <c r="R14" s="220"/>
     </row>
     <row r="15" spans="2:18" ht="15">
@@ -8158,7 +8167,7 @@
       <c r="F15" s="128">
         <v>10</v>
       </c>
-      <c r="G15" s="504"/>
+      <c r="G15" s="505"/>
       <c r="R15" s="220"/>
     </row>
     <row r="16" spans="2:18" ht="15">
@@ -8181,7 +8190,7 @@
       <c r="F16" s="128">
         <v>10</v>
       </c>
-      <c r="G16" s="504"/>
+      <c r="G16" s="505"/>
       <c r="R16" s="220"/>
     </row>
     <row r="17" spans="2:18" ht="15">
@@ -8204,7 +8213,7 @@
       <c r="F17" s="128">
         <v>10</v>
       </c>
-      <c r="G17" s="504"/>
+      <c r="G17" s="505"/>
       <c r="R17" s="220"/>
     </row>
     <row r="18" spans="2:18" ht="15">
@@ -8227,7 +8236,7 @@
       <c r="F18" s="128">
         <v>10</v>
       </c>
-      <c r="G18" s="504"/>
+      <c r="G18" s="505"/>
       <c r="R18" s="220"/>
     </row>
     <row r="19" spans="2:18" ht="15">
@@ -8250,7 +8259,7 @@
       <c r="F19" s="128">
         <v>10</v>
       </c>
-      <c r="G19" s="504"/>
+      <c r="G19" s="505"/>
       <c r="R19" s="220"/>
     </row>
     <row r="20" spans="2:18" ht="15">
@@ -8273,7 +8282,7 @@
       <c r="F20" s="128">
         <v>10</v>
       </c>
-      <c r="G20" s="504"/>
+      <c r="G20" s="505"/>
       <c r="R20" s="220"/>
     </row>
     <row r="21" spans="2:18">
@@ -8296,7 +8305,7 @@
       <c r="F21" s="128">
         <v>10</v>
       </c>
-      <c r="G21" s="504"/>
+      <c r="G21" s="505"/>
     </row>
     <row r="22" spans="2:18">
       <c r="B22" s="33" t="str">
@@ -8318,7 +8327,7 @@
       <c r="F22" s="128">
         <v>10</v>
       </c>
-      <c r="G22" s="504"/>
+      <c r="G22" s="505"/>
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="33" t="str">
@@ -8340,7 +8349,7 @@
       <c r="F23" s="128">
         <v>10</v>
       </c>
-      <c r="G23" s="504"/>
+      <c r="G23" s="505"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="71" t="str">
@@ -8362,7 +8371,7 @@
       <c r="F24" s="77">
         <v>10</v>
       </c>
-      <c r="G24" s="504"/>
+      <c r="G24" s="505"/>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="33" t="str">
@@ -8384,7 +8393,7 @@
       <c r="F25" s="128">
         <v>10</v>
       </c>
-      <c r="G25" s="504"/>
+      <c r="G25" s="505"/>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="33" t="str">
@@ -8406,7 +8415,7 @@
       <c r="F26" s="128">
         <v>10</v>
       </c>
-      <c r="G26" s="504"/>
+      <c r="G26" s="505"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="33" t="str">
@@ -8428,7 +8437,7 @@
       <c r="F27" s="128">
         <v>10</v>
       </c>
-      <c r="G27" s="504"/>
+      <c r="G27" s="505"/>
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="33" t="str">
@@ -8450,7 +8459,7 @@
       <c r="F28" s="128">
         <v>10</v>
       </c>
-      <c r="G28" s="504"/>
+      <c r="G28" s="505"/>
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="33" t="str">
@@ -8472,7 +8481,7 @@
       <c r="F29" s="128">
         <v>10</v>
       </c>
-      <c r="G29" s="504"/>
+      <c r="G29" s="505"/>
     </row>
     <row r="30" spans="2:18">
       <c r="B30" s="33" t="str">
@@ -8494,7 +8503,7 @@
       <c r="F30" s="128">
         <v>10</v>
       </c>
-      <c r="G30" s="504"/>
+      <c r="G30" s="505"/>
     </row>
     <row r="31" spans="2:18">
       <c r="B31" s="33" t="str">
@@ -8516,7 +8525,7 @@
       <c r="F31" s="128">
         <v>10</v>
       </c>
-      <c r="G31" s="504"/>
+      <c r="G31" s="505"/>
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="33" t="str">
@@ -8538,7 +8547,7 @@
       <c r="F32" s="128">
         <v>10</v>
       </c>
-      <c r="G32" s="504"/>
+      <c r="G32" s="505"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="33" t="str">
@@ -8560,7 +8569,7 @@
       <c r="F33" s="128">
         <v>10</v>
       </c>
-      <c r="G33" s="504"/>
+      <c r="G33" s="505"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="71" t="str">
@@ -8582,7 +8591,7 @@
       <c r="F34" s="77">
         <v>10</v>
       </c>
-      <c r="G34" s="505"/>
+      <c r="G34" s="506"/>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="33"/>
@@ -9668,20 +9677,20 @@
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="G7" s="502" t="s">
+      <c r="G7" s="503" t="s">
         <v>167</v>
       </c>
-      <c r="H7" s="502"/>
-      <c r="I7" s="502"/>
-      <c r="J7" s="502"/>
-      <c r="K7" s="502"/>
+      <c r="H7" s="503"/>
+      <c r="I7" s="503"/>
+      <c r="J7" s="503"/>
+      <c r="K7" s="503"/>
       <c r="L7" s="274" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="502" t="s">
+      <c r="M7" s="503" t="s">
         <v>236</v>
       </c>
-      <c r="N7" s="502"/>
+      <c r="N7" s="503"/>
       <c r="O7" s="52"/>
     </row>
     <row r="9" spans="2:20">
@@ -10459,10 +10468,10 @@
       <c r="J1" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="506" t="s">
+      <c r="P1" s="507" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="506"/>
+      <c r="Q1" s="507"/>
     </row>
     <row r="2" spans="1:22">
       <c r="H2" s="88"/>
@@ -21218,7 +21227,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:W93"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
@@ -25307,20 +25316,20 @@
       <c r="D24" s="467"/>
       <c r="E24" s="467"/>
       <c r="F24" s="468"/>
-      <c r="G24" s="494" t="s">
+      <c r="G24" s="495" t="s">
         <v>547</v>
       </c>
-      <c r="H24" s="494"/>
-      <c r="I24" s="494"/>
-      <c r="J24" s="495"/>
-      <c r="K24" s="496" t="s">
+      <c r="H24" s="495"/>
+      <c r="I24" s="495"/>
+      <c r="J24" s="496"/>
+      <c r="K24" s="497" t="s">
         <v>548</v>
       </c>
-      <c r="L24" s="497"/>
-      <c r="M24" s="498" t="s">
+      <c r="L24" s="498"/>
+      <c r="M24" s="499" t="s">
         <v>549</v>
       </c>
-      <c r="N24" s="497"/>
+      <c r="N24" s="498"/>
       <c r="S24"/>
     </row>
     <row r="25" spans="3:21">
@@ -25963,20 +25972,20 @@
       <c r="D42" s="467"/>
       <c r="E42" s="467"/>
       <c r="F42" s="468"/>
-      <c r="G42" s="494" t="s">
+      <c r="G42" s="495" t="s">
         <v>547</v>
       </c>
-      <c r="H42" s="494"/>
-      <c r="I42" s="494"/>
-      <c r="J42" s="495"/>
-      <c r="K42" s="496" t="s">
+      <c r="H42" s="495"/>
+      <c r="I42" s="495"/>
+      <c r="J42" s="496"/>
+      <c r="K42" s="497" t="s">
         <v>548</v>
       </c>
-      <c r="L42" s="497"/>
-      <c r="M42" s="498" t="s">
+      <c r="L42" s="498"/>
+      <c r="M42" s="499" t="s">
         <v>581</v>
       </c>
-      <c r="N42" s="497"/>
+      <c r="N42" s="498"/>
       <c r="O42"/>
     </row>
     <row r="43" spans="3:20">
@@ -26792,10 +26801,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B2:W58"/>
+  <dimension ref="B2:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -26840,7 +26849,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>3</v>
+        <v>565</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>40</v>
@@ -27529,765 +27538,656 @@
       <c r="L20" s="65"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="288" t="str">
-        <f>Processes!C31</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C21" s="288" t="str">
-        <f>Processes!D31</f>
-        <v>IMPBIOJKR_S1</v>
-      </c>
-      <c r="D21" s="288" t="str">
-        <f>Processes!E31</f>
-        <v>Import of Bio Jet Kerosene - Step 1</v>
-      </c>
-      <c r="E21" s="288" t="str">
-        <f>Commodities!C36</f>
-        <v>BIOJKR</v>
-      </c>
-      <c r="F21" s="289">
-        <f>Imports_Fossil!H18*1.6</f>
-        <v>26.566026131233826</v>
-      </c>
-      <c r="G21" s="289">
-        <f>Imports_Fossil!I16*1.6</f>
-        <v>25.964334287665327</v>
-      </c>
-      <c r="H21" s="289">
-        <f>Imports_Fossil!J16*1.6</f>
-        <v>29.261392609908548</v>
-      </c>
-      <c r="I21" s="289">
-        <f>Imports_Fossil!K16*1.6</f>
-        <v>31.322054061310553</v>
-      </c>
-      <c r="J21" s="289">
-        <f>Imports_Fossil!L16*1.6</f>
-        <v>33.382715512712565</v>
-      </c>
-      <c r="K21" s="289">
-        <f>Imports_Fossil!M16*1.6</f>
-        <v>35.031244673834173</v>
-      </c>
-      <c r="L21" s="289"/>
-    </row>
-    <row r="22" spans="2:18">
-      <c r="B22" s="124"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="124"/>
-      <c r="H22" s="124"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="35"/>
+    </row>
+    <row r="22" spans="2:18" ht="18.75">
+      <c r="B22" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="F22" s="13" t="str">
+        <f>Imports_Fossil!G3</f>
+        <v>~FI_T: IRE_PRICE</v>
+      </c>
+      <c r="G22" s="125"/>
+      <c r="H22" s="125"/>
       <c r="I22" s="124"/>
       <c r="J22" s="124"/>
       <c r="K22" s="124"/>
       <c r="L22" s="124"/>
       <c r="M22" s="124"/>
     </row>
-    <row r="23" spans="2:18" ht="26.25">
-      <c r="B23" s="11" t="s">
+    <row r="23" spans="2:18" ht="30.75" customHeight="1">
+      <c r="B23" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>585</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="38" t="str">
+        <f>Imports_Fossil!H4</f>
+        <v>2018~EUR18</v>
+      </c>
+      <c r="H23" s="38" t="str">
+        <f>Imports_Fossil!I4</f>
+        <v>2019~EUR19</v>
+      </c>
+      <c r="I23" s="38" t="str">
+        <f>Imports_Fossil!J4</f>
+        <v>2025~EUR19</v>
+      </c>
+      <c r="J23" s="38" t="str">
+        <f>Imports_Fossil!K4</f>
+        <v>2030~EUR19</v>
+      </c>
+      <c r="K23" s="38" t="str">
+        <f>Imports_Fossil!L4</f>
+        <v>2035~EUR19</v>
+      </c>
+      <c r="L23" s="38" t="str">
+        <f>Imports_Fossil!M4</f>
+        <v>2040~EUR19</v>
+      </c>
+      <c r="M23" s="126" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="26.25" thickBot="1">
+      <c r="B24" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M24" s="127"/>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="288" t="str">
+        <f>Processes!C31</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C25" s="288" t="str">
+        <f>Processes!D31</f>
+        <v>IMPBIOJKR_S1</v>
+      </c>
+      <c r="D25" s="288" t="str">
+        <f>Processes!E31</f>
+        <v>Import of Bio Jet Kerosene - Step 1</v>
+      </c>
+      <c r="E25" s="288" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="288" t="str">
+        <f>Commodities!C36</f>
+        <v>BIOJKR</v>
+      </c>
+      <c r="G25" s="289">
+        <f>Imports_Fossil!H18*1.6</f>
+        <v>26.566026131233826</v>
+      </c>
+      <c r="H25" s="289">
+        <f>Imports_Fossil!I16*1.6</f>
+        <v>25.964334287665327</v>
+      </c>
+      <c r="I25" s="289">
+        <f>Imports_Fossil!J16*1.6</f>
+        <v>29.261392609908548</v>
+      </c>
+      <c r="J25" s="289">
+        <f>Imports_Fossil!K16*1.6</f>
+        <v>31.322054061310553</v>
+      </c>
+      <c r="K25" s="289">
+        <f>Imports_Fossil!L16*1.6</f>
+        <v>33.382715512712565</v>
+      </c>
+      <c r="L25" s="289">
+        <f>Imports_Fossil!M16*1.6</f>
+        <v>35.031244673834173</v>
+      </c>
+      <c r="M25" s="494" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18">
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+    </row>
+    <row r="27" spans="2:18" ht="26.25">
+      <c r="B27" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="13" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="68"/>
-      <c r="G23" s="124"/>
-      <c r="H23" s="124"/>
-      <c r="I23" s="124"/>
-      <c r="J23" s="124"/>
-      <c r="K23" s="124"/>
-      <c r="L23" s="124"/>
-      <c r="N23" s="179" t="s">
+      <c r="F27" s="68"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="124"/>
+      <c r="K27" s="124"/>
+      <c r="L27" s="124"/>
+      <c r="N27" s="179" t="s">
         <v>161</v>
       </c>
-      <c r="O23" s="177"/>
-      <c r="P23" s="177"/>
-      <c r="Q23" s="177"/>
-      <c r="R23" s="177"/>
-    </row>
-    <row r="24" spans="2:18">
-      <c r="B24" s="17" t="s">
+      <c r="O27" s="177"/>
+      <c r="P27" s="177"/>
+      <c r="Q27" s="177"/>
+      <c r="R27" s="177"/>
+    </row>
+    <row r="28" spans="2:18">
+      <c r="B28" s="17" t="s">
         <v>533</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="D28" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F28" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G28" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="H28" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I28" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J28" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="K24" s="126" t="s">
+      <c r="K28" s="126" t="s">
         <v>71</v>
       </c>
-      <c r="N24" s="219" t="s">
+      <c r="N28" s="219" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B25" s="10" t="s">
+    <row r="29" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B29" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="127"/>
-      <c r="N25" s="178"/>
-      <c r="O25" s="178"/>
-      <c r="P25" s="217" t="s">
+      <c r="K29" s="127"/>
+      <c r="N29" s="178"/>
+      <c r="O29" s="178"/>
+      <c r="P29" s="217" t="s">
         <v>163</v>
       </c>
-      <c r="Q25" s="217"/>
-      <c r="R25" s="217" t="s">
+      <c r="Q29" s="217"/>
+      <c r="R29" s="217" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B26" s="69" t="str">
-        <f t="shared" ref="B26" si="0">B13</f>
+    <row r="30" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B30" s="69" t="str">
+        <f t="shared" ref="B30" si="0">B13</f>
         <v>IE,National</v>
       </c>
-      <c r="C26" s="69" t="str">
-        <f t="shared" ref="C26:D26" si="1">C13</f>
+      <c r="C30" s="69" t="str">
+        <f t="shared" ref="C30:D30" si="1">C13</f>
         <v>IMPBIOWPE_S1</v>
       </c>
-      <c r="D26" s="69" t="str">
+      <c r="D30" s="69" t="str">
         <f t="shared" si="1"/>
         <v>Import of Wood Pellets  - Step 1</v>
       </c>
-      <c r="E26" s="34" t="str">
+      <c r="E30" s="34" t="str">
         <f>Commodities!$C$41</f>
         <v>BIOWPE</v>
       </c>
-      <c r="F26" s="129">
-        <f t="shared" ref="F26:F33" si="2">SUM($P$26:$R$26)</f>
+      <c r="F30" s="129">
+        <f t="shared" ref="F30:F37" si="2">SUM($P$30:$R$30)</f>
         <v>4.8499999999999996</v>
       </c>
-      <c r="G26" s="129">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+      <c r="G30" s="129">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
         <v>4.3203296703296701</v>
       </c>
-      <c r="H26" s="129">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+      <c r="H30" s="129">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
         <v>4.4527472527472529</v>
       </c>
-      <c r="I26" s="129">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+      <c r="I30" s="129">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
         <v>4.5851648351648358</v>
       </c>
-      <c r="J26" s="129">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+      <c r="J30" s="129">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K26" s="499" t="s">
+      <c r="K30" s="500" t="s">
         <v>122</v>
       </c>
-      <c r="N26" s="187" t="s">
+      <c r="N30" s="187" t="s">
         <v>165</v>
       </c>
-      <c r="O26" s="215" t="s">
+      <c r="O30" s="215" t="s">
         <v>166</v>
       </c>
-      <c r="P26" s="207">
+      <c r="P30" s="207">
         <v>0.53</v>
       </c>
-      <c r="Q26" s="207">
+      <c r="Q30" s="207">
         <v>1.91</v>
       </c>
-      <c r="R26" s="207">
+      <c r="R30" s="207">
         <v>2.41</v>
       </c>
     </row>
-    <row r="27" spans="2:18">
-      <c r="B27" s="33" t="str">
-        <f t="shared" ref="B27" si="3">B14</f>
+    <row r="31" spans="2:18">
+      <c r="B31" s="33" t="str">
+        <f t="shared" ref="B31" si="3">B14</f>
         <v>IE,National</v>
       </c>
-      <c r="C27" s="33" t="str">
-        <f t="shared" ref="C27:D27" si="4">C14</f>
+      <c r="C31" s="33" t="str">
+        <f t="shared" ref="C31:D31" si="4">C14</f>
         <v>IMPBIOWPE_S2</v>
       </c>
-      <c r="D27" s="33" t="str">
+      <c r="D31" s="33" t="str">
         <f t="shared" si="4"/>
         <v>Import of Wood Pellets  - Step 2</v>
       </c>
-      <c r="E27" s="34" t="str">
+      <c r="E31" s="34" t="str">
         <f>Commodities!$C$41</f>
         <v>BIOWPE</v>
-      </c>
-      <c r="F27" s="181">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="G27" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
-        <v>4.3203296703296701</v>
-      </c>
-      <c r="H27" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
-        <v>4.4527472527472529</v>
-      </c>
-      <c r="I27" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
-        <v>4.5851648351648358</v>
-      </c>
-      <c r="J27" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
-        <v>4.6910989010989006</v>
-      </c>
-      <c r="K27" s="500"/>
-      <c r="M27" s="183"/>
-      <c r="N27" s="216"/>
-      <c r="O27" s="212"/>
-      <c r="P27" s="212"/>
-      <c r="Q27" s="212"/>
-    </row>
-    <row r="28" spans="2:18">
-      <c r="B28" s="33" t="str">
-        <f t="shared" ref="B28" si="5">B15</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C28" s="33" t="str">
-        <f t="shared" ref="C28:D28" si="6">C15</f>
-        <v>IMPBIOWPE_S3</v>
-      </c>
-      <c r="D28" s="33" t="str">
-        <f t="shared" si="6"/>
-        <v>Import of Wood Pellets  - Step 3</v>
-      </c>
-      <c r="E28" s="34" t="str">
-        <f>Commodities!$C$41</f>
-        <v>BIOWPE</v>
-      </c>
-      <c r="F28" s="181">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="G28" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
-        <v>4.3203296703296701</v>
-      </c>
-      <c r="H28" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
-        <v>4.4527472527472529</v>
-      </c>
-      <c r="I28" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
-        <v>4.5851648351648358</v>
-      </c>
-      <c r="J28" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
-        <v>4.6910989010989006</v>
-      </c>
-      <c r="K28" s="500"/>
-      <c r="M28" s="176"/>
-      <c r="N28" s="185"/>
-      <c r="O28" s="185"/>
-      <c r="P28" s="185"/>
-      <c r="Q28" s="185"/>
-      <c r="R28" s="185"/>
-    </row>
-    <row r="29" spans="2:18">
-      <c r="B29" s="71" t="str">
-        <f t="shared" ref="B29" si="7">B16</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C29" s="71" t="str">
-        <f t="shared" ref="C29:D29" si="8">C16</f>
-        <v>IMPBIOWPE_S4</v>
-      </c>
-      <c r="D29" s="71" t="str">
-        <f t="shared" si="8"/>
-        <v>Import of Wood Pellets  - Step 4</v>
-      </c>
-      <c r="E29" s="65" t="str">
-        <f>Commodities!$C$41</f>
-        <v>BIOWPE</v>
-      </c>
-      <c r="F29" s="182">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="G29" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
-        <v>4.3203296703296701</v>
-      </c>
-      <c r="H29" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
-        <v>4.4527472527472529</v>
-      </c>
-      <c r="I29" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
-        <v>4.5851648351648358</v>
-      </c>
-      <c r="J29" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
-        <v>4.6910989010989006</v>
-      </c>
-      <c r="K29" s="500"/>
-      <c r="M29" s="124"/>
-    </row>
-    <row r="30" spans="2:18">
-      <c r="B30" s="130" t="str">
-        <f t="shared" ref="B30" si="9">B17</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C30" s="130" t="str">
-        <f t="shared" ref="C30:D30" si="10">C17</f>
-        <v>IMPBIOWCH_S1</v>
-      </c>
-      <c r="D30" s="130" t="str">
-        <f t="shared" si="10"/>
-        <v>Import of Wood Chip  - Step 1</v>
-      </c>
-      <c r="E30" s="34" t="str">
-        <f>Commodities!$C$42</f>
-        <v>BIOWCH</v>
-      </c>
-      <c r="F30" s="131">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="G30" s="131">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
-        <v>4.3203296703296701</v>
-      </c>
-      <c r="H30" s="131">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
-        <v>4.4527472527472529</v>
-      </c>
-      <c r="I30" s="131">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
-        <v>4.5851648351648358</v>
-      </c>
-      <c r="J30" s="131">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
-        <v>4.6910989010989006</v>
-      </c>
-      <c r="K30" s="500"/>
-      <c r="M30" s="124"/>
-    </row>
-    <row r="31" spans="2:18">
-      <c r="B31" s="33" t="str">
-        <f t="shared" ref="B31" si="11">B18</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C31" s="33" t="str">
-        <f t="shared" ref="C31:D31" si="12">C18</f>
-        <v>IMPBIOWCH_S2</v>
-      </c>
-      <c r="D31" s="33" t="str">
-        <f t="shared" si="12"/>
-        <v>Import of Wood Chip  - Step 2</v>
-      </c>
-      <c r="E31" s="34" t="str">
-        <f>Commodities!$C$42</f>
-        <v>BIOWCH</v>
       </c>
       <c r="F31" s="181">
         <f t="shared" si="2"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="G31" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
         <v>4.3203296703296701</v>
       </c>
       <c r="H31" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
         <v>4.4527472527472529</v>
       </c>
       <c r="I31" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
         <v>4.5851648351648358</v>
       </c>
       <c r="J31" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K31" s="500"/>
-      <c r="M31" s="124"/>
+      <c r="K31" s="501"/>
+      <c r="M31" s="183"/>
+      <c r="N31" s="216"/>
+      <c r="O31" s="212"/>
+      <c r="P31" s="212"/>
+      <c r="Q31" s="212"/>
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="33" t="str">
-        <f t="shared" ref="B32" si="13">B19</f>
+        <f t="shared" ref="B32" si="5">B15</f>
         <v>IE,National</v>
       </c>
       <c r="C32" s="33" t="str">
-        <f t="shared" ref="C32:D32" si="14">C19</f>
-        <v>IMPBIOWCH_S3</v>
+        <f t="shared" ref="C32:D32" si="6">C15</f>
+        <v>IMPBIOWPE_S3</v>
       </c>
       <c r="D32" s="33" t="str">
-        <f t="shared" si="14"/>
-        <v>Import of Wood Chip  - Step 3</v>
+        <f t="shared" si="6"/>
+        <v>Import of Wood Pellets  - Step 3</v>
       </c>
       <c r="E32" s="34" t="str">
-        <f>Commodities!$C$42</f>
-        <v>BIOWCH</v>
+        <f>Commodities!$C$41</f>
+        <v>BIOWPE</v>
       </c>
       <c r="F32" s="181">
         <f t="shared" si="2"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="G32" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
         <v>4.3203296703296701</v>
       </c>
       <c r="H32" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
         <v>4.4527472527472529</v>
       </c>
       <c r="I32" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
         <v>4.5851648351648358</v>
       </c>
       <c r="J32" s="181">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
-      <c r="K32" s="500"/>
-      <c r="M32" s="124"/>
+      <c r="K32" s="501"/>
+      <c r="M32" s="176"/>
+      <c r="N32" s="185"/>
+      <c r="O32" s="185"/>
+      <c r="P32" s="185"/>
+      <c r="Q32" s="185"/>
+      <c r="R32" s="185"/>
     </row>
     <row r="33" spans="2:23">
       <c r="B33" s="71" t="str">
-        <f t="shared" ref="B33" si="15">B20</f>
+        <f t="shared" ref="B33" si="7">B16</f>
         <v>IE,National</v>
       </c>
       <c r="C33" s="71" t="str">
-        <f t="shared" ref="C33:D33" si="16">C20</f>
-        <v>IMPBIOWCH_S4</v>
+        <f t="shared" ref="C33:D33" si="8">C16</f>
+        <v>IMPBIOWPE_S4</v>
       </c>
       <c r="D33" s="71" t="str">
-        <f t="shared" si="16"/>
-        <v>Import of Wood Chip  - Step 4</v>
+        <f t="shared" si="8"/>
+        <v>Import of Wood Pellets  - Step 4</v>
       </c>
       <c r="E33" s="65" t="str">
-        <f>Commodities!$C$42</f>
-        <v>BIOWCH</v>
+        <f>Commodities!$C$41</f>
+        <v>BIOWPE</v>
       </c>
       <c r="F33" s="182">
         <f t="shared" si="2"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="G33" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
         <v>4.3203296703296701</v>
       </c>
       <c r="H33" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
         <v>4.4527472527472529</v>
       </c>
       <c r="I33" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
         <v>4.5851648351648358</v>
       </c>
       <c r="J33" s="182">
-        <f>SUM($P$26:$Q$26)+$R$26*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
         <v>4.6910989010989006</v>
       </c>
       <c r="K33" s="501"/>
       <c r="M33" s="124"/>
     </row>
     <row r="34" spans="2:23">
-      <c r="B34" s="124"/>
-      <c r="C34" s="124"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="124"/>
-      <c r="I34" s="124"/>
-      <c r="J34" s="124"/>
-      <c r="K34" s="124"/>
-      <c r="L34" s="124"/>
+      <c r="B34" s="130" t="str">
+        <f t="shared" ref="B34" si="9">B17</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C34" s="130" t="str">
+        <f t="shared" ref="C34:D34" si="10">C17</f>
+        <v>IMPBIOWCH_S1</v>
+      </c>
+      <c r="D34" s="130" t="str">
+        <f t="shared" si="10"/>
+        <v>Import of Wood Chip  - Step 1</v>
+      </c>
+      <c r="E34" s="34" t="str">
+        <f>Commodities!$C$42</f>
+        <v>BIOWCH</v>
+      </c>
+      <c r="F34" s="131">
+        <f t="shared" si="2"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G34" s="131">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <v>4.3203296703296701</v>
+      </c>
+      <c r="H34" s="131">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <v>4.4527472527472529</v>
+      </c>
+      <c r="I34" s="131">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <v>4.5851648351648358</v>
+      </c>
+      <c r="J34" s="131">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <v>4.6910989010989006</v>
+      </c>
+      <c r="K34" s="501"/>
       <c r="M34" s="124"/>
     </row>
     <row r="35" spans="2:23">
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="186"/>
-    </row>
-    <row r="36" spans="2:23" ht="18.75">
-      <c r="B36" s="11" t="s">
+      <c r="B35" s="33" t="str">
+        <f t="shared" ref="B35" si="11">B18</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C35" s="33" t="str">
+        <f t="shared" ref="C35:D35" si="12">C18</f>
+        <v>IMPBIOWCH_S2</v>
+      </c>
+      <c r="D35" s="33" t="str">
+        <f t="shared" si="12"/>
+        <v>Import of Wood Chip  - Step 2</v>
+      </c>
+      <c r="E35" s="34" t="str">
+        <f>Commodities!$C$42</f>
+        <v>BIOWCH</v>
+      </c>
+      <c r="F35" s="181">
+        <f t="shared" si="2"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G35" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <v>4.3203296703296701</v>
+      </c>
+      <c r="H35" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <v>4.4527472527472529</v>
+      </c>
+      <c r="I35" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <v>4.5851648351648358</v>
+      </c>
+      <c r="J35" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <v>4.6910989010989006</v>
+      </c>
+      <c r="K35" s="501"/>
+      <c r="M35" s="124"/>
+    </row>
+    <row r="36" spans="2:23">
+      <c r="B36" s="33" t="str">
+        <f t="shared" ref="B36" si="13">B19</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C36" s="33" t="str">
+        <f t="shared" ref="C36:D36" si="14">C19</f>
+        <v>IMPBIOWCH_S3</v>
+      </c>
+      <c r="D36" s="33" t="str">
+        <f t="shared" si="14"/>
+        <v>Import of Wood Chip  - Step 3</v>
+      </c>
+      <c r="E36" s="34" t="str">
+        <f>Commodities!$C$42</f>
+        <v>BIOWCH</v>
+      </c>
+      <c r="F36" s="181">
+        <f t="shared" si="2"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G36" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <v>4.3203296703296701</v>
+      </c>
+      <c r="H36" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <v>4.4527472527472529</v>
+      </c>
+      <c r="I36" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <v>4.5851648351648358</v>
+      </c>
+      <c r="J36" s="181">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <v>4.6910989010989006</v>
+      </c>
+      <c r="K36" s="501"/>
+      <c r="M36" s="124"/>
+    </row>
+    <row r="37" spans="2:23">
+      <c r="B37" s="71" t="str">
+        <f t="shared" ref="B37" si="15">B20</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C37" s="71" t="str">
+        <f t="shared" ref="C37:D37" si="16">C20</f>
+        <v>IMPBIOWCH_S4</v>
+      </c>
+      <c r="D37" s="71" t="str">
+        <f t="shared" si="16"/>
+        <v>Import of Wood Chip  - Step 4</v>
+      </c>
+      <c r="E37" s="65" t="str">
+        <f>Commodities!$C$42</f>
+        <v>BIOWCH</v>
+      </c>
+      <c r="F37" s="182">
+        <f t="shared" si="2"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G37" s="182">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!G$37/Imports_Fossil!$E$37)</f>
+        <v>4.3203296703296701</v>
+      </c>
+      <c r="H37" s="182">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!H$37/Imports_Fossil!$E$37)</f>
+        <v>4.4527472527472529</v>
+      </c>
+      <c r="I37" s="182">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!I$37/Imports_Fossil!$E$37)</f>
+        <v>4.5851648351648358</v>
+      </c>
+      <c r="J37" s="182">
+        <f>SUM($P$30:$Q$30)+$R$30*(Imports_Fossil!J$37/Imports_Fossil!$E$37)</f>
+        <v>4.6910989010989006</v>
+      </c>
+      <c r="K37" s="502"/>
+      <c r="M37" s="124"/>
+    </row>
+    <row r="38" spans="2:23">
+      <c r="B38" s="124"/>
+      <c r="C38" s="124"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="124"/>
+      <c r="J38" s="124"/>
+      <c r="K38" s="124"/>
+      <c r="L38" s="124"/>
+      <c r="M38" s="124"/>
+    </row>
+    <row r="39" spans="2:23">
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="186"/>
+    </row>
+    <row r="40" spans="2:23" ht="18.75">
+      <c r="B40" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="13" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="186"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-    </row>
-    <row r="37" spans="2:23">
-      <c r="B37" s="17" t="s">
-        <v>533</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="38">
-        <v>2018</v>
-      </c>
-      <c r="G37" s="38">
-        <v>2020</v>
-      </c>
-      <c r="H37" s="38">
-        <v>2025</v>
-      </c>
-      <c r="I37" s="38">
-        <v>2030</v>
-      </c>
-      <c r="J37" s="38">
-        <v>2035</v>
-      </c>
-      <c r="K37" s="38">
-        <v>2040</v>
-      </c>
-      <c r="L37" s="38">
-        <v>2045</v>
-      </c>
-      <c r="M37" s="38">
-        <v>2050</v>
-      </c>
-      <c r="N37" s="276">
-        <v>0</v>
-      </c>
-      <c r="O37" s="126" t="s">
-        <v>71</v>
-      </c>
-      <c r="P37" s="38"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-    </row>
-    <row r="38" spans="2:23" ht="15.75" thickBot="1">
-      <c r="B38" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-    </row>
-    <row r="39" spans="2:23">
-      <c r="B39" s="69" t="str">
-        <f>Imports_Bio!B5</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C39" s="69" t="str">
-        <f>Imports_Bio!C5</f>
-        <v>IMPBIOETH1G_S1</v>
-      </c>
-      <c r="D39" s="69" t="str">
-        <f>Imports_Bio!D5</f>
-        <v>Import of Ethanol 1st generation  - Step 1</v>
-      </c>
-      <c r="E39" s="70" t="str">
-        <f>Commodities!$C$30</f>
-        <v>BIOETH1G</v>
-      </c>
-      <c r="F39" s="209">
-        <f>'EB2018'!AJ3*Conversions!$C$2</f>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="G39" s="78">
-        <f>F39</f>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="H39" s="78">
-        <f t="shared" ref="H39:M39" si="17">G39</f>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="I39" s="78">
-        <f t="shared" si="17"/>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="J39" s="78">
-        <f t="shared" si="17"/>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="K39" s="78">
-        <f t="shared" si="17"/>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="L39" s="78">
-        <f t="shared" si="17"/>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="M39" s="78">
-        <f t="shared" si="17"/>
-        <v>0.95668374631852515</v>
-      </c>
-      <c r="N39" s="277">
-        <v>5</v>
-      </c>
-      <c r="O39" s="89" t="s">
-        <v>471</v>
-      </c>
-      <c r="P39" s="78"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-    </row>
-    <row r="40" spans="2:23">
-      <c r="B40" s="33" t="str">
-        <f>Imports_Bio!B6</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C40" s="33" t="str">
-        <f>Imports_Bio!C6</f>
-        <v>IMPBIOETH1G_S2</v>
-      </c>
-      <c r="D40" s="33" t="str">
-        <f>Imports_Bio!D6</f>
-        <v>Import of Ethanol 1st generation  - Step 2</v>
-      </c>
-      <c r="E40" s="35" t="str">
-        <f>Commodities!$C$30</f>
-        <v>BIOETH1G</v>
-      </c>
-      <c r="F40" s="211">
-        <v>0</v>
-      </c>
-      <c r="G40" s="76">
-        <f>G39*2</f>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="H40" s="76">
-        <f t="shared" ref="H40:M41" si="18">H39*2</f>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="I40" s="76">
-        <f t="shared" si="18"/>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="J40" s="76">
-        <f t="shared" si="18"/>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="K40" s="76">
-        <f t="shared" si="18"/>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="L40" s="76">
-        <f t="shared" si="18"/>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="M40" s="76">
-        <f t="shared" si="18"/>
-        <v>1.9133674926370503</v>
-      </c>
-      <c r="N40" s="278">
-        <v>5</v>
-      </c>
-      <c r="O40" s="90" t="s">
-        <v>231</v>
-      </c>
-      <c r="P40" s="76"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="186"/>
       <c r="R40"/>
       <c r="S40"/>
       <c r="T40"/>
@@ -28296,60 +28196,49 @@
       <c r="W40"/>
     </row>
     <row r="41" spans="2:23">
-      <c r="B41" s="33" t="str">
-        <f>Imports_Bio!B7</f>
-        <v>IE,National</v>
-      </c>
-      <c r="C41" s="33" t="str">
-        <f>Imports_Bio!C7</f>
-        <v>IMPBIOETH1G_S3</v>
-      </c>
-      <c r="D41" s="33" t="str">
-        <f>Imports_Bio!D7</f>
-        <v>Import of Ethanol 1st generation  - Step 3</v>
-      </c>
-      <c r="E41" s="35" t="str">
-        <f>Commodities!$C$30</f>
-        <v>BIOETH1G</v>
-      </c>
-      <c r="F41" s="211">
+      <c r="B41" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="38">
+        <v>2018</v>
+      </c>
+      <c r="G41" s="38">
+        <v>2020</v>
+      </c>
+      <c r="H41" s="38">
+        <v>2025</v>
+      </c>
+      <c r="I41" s="38">
+        <v>2030</v>
+      </c>
+      <c r="J41" s="38">
+        <v>2035</v>
+      </c>
+      <c r="K41" s="38">
+        <v>2040</v>
+      </c>
+      <c r="L41" s="38">
+        <v>2045</v>
+      </c>
+      <c r="M41" s="38">
+        <v>2050</v>
+      </c>
+      <c r="N41" s="276">
         <v>0</v>
       </c>
-      <c r="G41" s="76">
-        <f>G40*2</f>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="H41" s="76">
-        <f t="shared" si="18"/>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="I41" s="76">
-        <f t="shared" si="18"/>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="J41" s="76">
-        <f t="shared" si="18"/>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="K41" s="76">
-        <f t="shared" si="18"/>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="L41" s="76">
-        <f t="shared" si="18"/>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="M41" s="76">
-        <f t="shared" si="18"/>
-        <v>3.8267349852741006</v>
-      </c>
-      <c r="N41" s="278">
-        <v>5</v>
-      </c>
-      <c r="O41" s="90" t="s">
-        <v>232</v>
-      </c>
-      <c r="P41" s="76"/>
+      <c r="O41" s="126" t="s">
+        <v>71</v>
+      </c>
+      <c r="P41" s="38"/>
       <c r="R41"/>
       <c r="S41"/>
       <c r="T41"/>
@@ -28357,54 +28246,48 @@
       <c r="V41"/>
       <c r="W41"/>
     </row>
-    <row r="42" spans="2:23">
-      <c r="B42" s="71" t="str">
-        <f>"*"&amp;Imports_Bio!B8</f>
-        <v>*IE,National</v>
-      </c>
-      <c r="C42" s="71" t="str">
-        <f>"*"&amp;Imports_Bio!C8</f>
-        <v>*IMPBIOETH1G_S4</v>
-      </c>
-      <c r="D42" s="71" t="str">
-        <f>Imports_Bio!D8</f>
-        <v>Import of Ethanol 1st generation  - Step 4</v>
-      </c>
-      <c r="E42" s="65" t="str">
-        <f>Commodities!$C$30</f>
-        <v>BIOETH1G</v>
-      </c>
-      <c r="F42" s="213">
-        <v>0</v>
-      </c>
-      <c r="G42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="H42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="I42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="J42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="K42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="L42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="M42" s="77">
-        <v>27.064417978971818</v>
-      </c>
-      <c r="N42" s="279">
-        <v>5</v>
-      </c>
-      <c r="O42" s="91" t="s">
-        <v>233</v>
-      </c>
-      <c r="P42" s="77"/>
+    <row r="42" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B42" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N42" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
       <c r="R42"/>
       <c r="S42"/>
       <c r="T42"/>
@@ -28412,47 +28295,62 @@
       <c r="V42"/>
       <c r="W42"/>
     </row>
-    <row r="43" spans="2:23" ht="15.75" thickBot="1">
-      <c r="B43" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79">
-        <f>H43</f>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="H43" s="79">
-        <f>I43</f>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="I43" s="79">
-        <f>'SEAI-AEA_BioData'!G54*Conversions!$C$2/1000</f>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="J43" s="79">
-        <f>I43</f>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="K43" s="79">
-        <f t="shared" ref="K43:M43" si="19">J43</f>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="L43" s="79">
-        <f t="shared" si="19"/>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="M43" s="79">
-        <f t="shared" si="19"/>
-        <v>59.810866344000004</v>
-      </c>
-      <c r="N43" s="280"/>
-      <c r="O43" s="92" t="s">
-        <v>86</v>
-      </c>
-      <c r="P43" s="79"/>
+    <row r="43" spans="2:23">
+      <c r="B43" s="69" t="str">
+        <f>Imports_Bio!B5</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C43" s="69" t="str">
+        <f>Imports_Bio!C5</f>
+        <v>IMPBIOETH1G_S1</v>
+      </c>
+      <c r="D43" s="69" t="str">
+        <f>Imports_Bio!D5</f>
+        <v>Import of Ethanol 1st generation  - Step 1</v>
+      </c>
+      <c r="E43" s="70" t="str">
+        <f>Commodities!$C$30</f>
+        <v>BIOETH1G</v>
+      </c>
+      <c r="F43" s="209">
+        <f>'EB2018'!AJ3*Conversions!$C$2</f>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="G43" s="78">
+        <f>F43</f>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="H43" s="78">
+        <f t="shared" ref="H43:M43" si="17">G43</f>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="I43" s="78">
+        <f t="shared" si="17"/>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="J43" s="78">
+        <f t="shared" si="17"/>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="K43" s="78">
+        <f t="shared" si="17"/>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="L43" s="78">
+        <f t="shared" si="17"/>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="M43" s="78">
+        <f t="shared" si="17"/>
+        <v>0.95668374631852515</v>
+      </c>
+      <c r="N43" s="277">
+        <v>5</v>
+      </c>
+      <c r="O43" s="89" t="s">
+        <v>471</v>
+      </c>
+      <c r="P43" s="78"/>
       <c r="R43"/>
       <c r="S43"/>
       <c r="T43"/>
@@ -28461,61 +28359,60 @@
       <c r="W43"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="69" t="str">
-        <f>Imports_Bio!B9</f>
+      <c r="B44" s="33" t="str">
+        <f>Imports_Bio!B6</f>
         <v>IE,National</v>
       </c>
-      <c r="C44" s="69" t="str">
-        <f>Imports_Bio!C9</f>
-        <v>IMPBIODST1G_S1</v>
-      </c>
-      <c r="D44" s="69" t="str">
-        <f>Imports_Bio!D9</f>
-        <v>Import of Biodiesel 1st generation  - Step 1</v>
-      </c>
-      <c r="E44" s="70" t="str">
-        <f>Commodities!$C$32</f>
-        <v>BIODST1G</v>
-      </c>
-      <c r="F44" s="209">
-        <f>'EB2018'!AI3*Conversions!$C$2</f>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="G44" s="78">
-        <f>F44</f>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="H44" s="78">
-        <f t="shared" ref="H44:M44" si="20">G44</f>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="I44" s="78">
-        <f t="shared" si="20"/>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="J44" s="78">
-        <f t="shared" si="20"/>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="K44" s="78">
-        <f t="shared" si="20"/>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="L44" s="78">
-        <f t="shared" si="20"/>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="M44" s="78">
-        <f t="shared" si="20"/>
-        <v>4.3613769615262452</v>
-      </c>
-      <c r="N44" s="277">
+      <c r="C44" s="33" t="str">
+        <f>Imports_Bio!C6</f>
+        <v>IMPBIOETH1G_S2</v>
+      </c>
+      <c r="D44" s="33" t="str">
+        <f>Imports_Bio!D6</f>
+        <v>Import of Ethanol 1st generation  - Step 2</v>
+      </c>
+      <c r="E44" s="35" t="str">
+        <f>Commodities!$C$30</f>
+        <v>BIOETH1G</v>
+      </c>
+      <c r="F44" s="211">
+        <v>0</v>
+      </c>
+      <c r="G44" s="76">
+        <f>G43*2</f>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="H44" s="76">
+        <f t="shared" ref="H44:M45" si="18">H43*2</f>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="I44" s="76">
+        <f t="shared" si="18"/>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="J44" s="76">
+        <f t="shared" si="18"/>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="K44" s="76">
+        <f t="shared" si="18"/>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="L44" s="76">
+        <f t="shared" si="18"/>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="M44" s="76">
+        <f t="shared" si="18"/>
+        <v>1.9133674926370503</v>
+      </c>
+      <c r="N44" s="278">
         <v>5</v>
       </c>
-      <c r="O44" s="89" t="s">
-        <v>471</v>
-      </c>
-      <c r="P44" s="78"/>
+      <c r="O44" s="90" t="s">
+        <v>231</v>
+      </c>
+      <c r="P44" s="76"/>
       <c r="R44"/>
       <c r="S44"/>
       <c r="T44"/>
@@ -28525,770 +28422,998 @@
     </row>
     <row r="45" spans="2:23">
       <c r="B45" s="33" t="str">
+        <f>Imports_Bio!B7</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C45" s="33" t="str">
+        <f>Imports_Bio!C7</f>
+        <v>IMPBIOETH1G_S3</v>
+      </c>
+      <c r="D45" s="33" t="str">
+        <f>Imports_Bio!D7</f>
+        <v>Import of Ethanol 1st generation  - Step 3</v>
+      </c>
+      <c r="E45" s="35" t="str">
+        <f>Commodities!$C$30</f>
+        <v>BIOETH1G</v>
+      </c>
+      <c r="F45" s="211">
+        <v>0</v>
+      </c>
+      <c r="G45" s="76">
+        <f>G44*2</f>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="H45" s="76">
+        <f t="shared" si="18"/>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="I45" s="76">
+        <f t="shared" si="18"/>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="J45" s="76">
+        <f t="shared" si="18"/>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="K45" s="76">
+        <f t="shared" si="18"/>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="L45" s="76">
+        <f t="shared" si="18"/>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="M45" s="76">
+        <f t="shared" si="18"/>
+        <v>3.8267349852741006</v>
+      </c>
+      <c r="N45" s="278">
+        <v>5</v>
+      </c>
+      <c r="O45" s="90" t="s">
+        <v>232</v>
+      </c>
+      <c r="P45" s="76"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+    </row>
+    <row r="46" spans="2:23">
+      <c r="B46" s="71" t="str">
+        <f>"*"&amp;Imports_Bio!B8</f>
+        <v>*IE,National</v>
+      </c>
+      <c r="C46" s="71" t="str">
+        <f>"*"&amp;Imports_Bio!C8</f>
+        <v>*IMPBIOETH1G_S4</v>
+      </c>
+      <c r="D46" s="71" t="str">
+        <f>Imports_Bio!D8</f>
+        <v>Import of Ethanol 1st generation  - Step 4</v>
+      </c>
+      <c r="E46" s="65" t="str">
+        <f>Commodities!$C$30</f>
+        <v>BIOETH1G</v>
+      </c>
+      <c r="F46" s="213">
+        <v>0</v>
+      </c>
+      <c r="G46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="H46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="I46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="J46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="K46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="L46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="M46" s="77">
+        <v>27.064417978971818</v>
+      </c>
+      <c r="N46" s="279">
+        <v>5</v>
+      </c>
+      <c r="O46" s="91" t="s">
+        <v>233</v>
+      </c>
+      <c r="P46" s="77"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+    </row>
+    <row r="47" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B47" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="79">
+        <f>H47</f>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="H47" s="79">
+        <f>I47</f>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="I47" s="79">
+        <f>'SEAI-AEA_BioData'!G54*Conversions!$C$2/1000</f>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="J47" s="79">
+        <f>I47</f>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="K47" s="79">
+        <f t="shared" ref="K47:M47" si="19">J47</f>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="L47" s="79">
+        <f t="shared" si="19"/>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="M47" s="79">
+        <f t="shared" si="19"/>
+        <v>59.810866344000004</v>
+      </c>
+      <c r="N47" s="280"/>
+      <c r="O47" s="92" t="s">
+        <v>86</v>
+      </c>
+      <c r="P47" s="79"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+    </row>
+    <row r="48" spans="2:23">
+      <c r="B48" s="69" t="str">
+        <f>Imports_Bio!B9</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C48" s="69" t="str">
+        <f>Imports_Bio!C9</f>
+        <v>IMPBIODST1G_S1</v>
+      </c>
+      <c r="D48" s="69" t="str">
+        <f>Imports_Bio!D9</f>
+        <v>Import of Biodiesel 1st generation  - Step 1</v>
+      </c>
+      <c r="E48" s="70" t="str">
+        <f>Commodities!$C$32</f>
+        <v>BIODST1G</v>
+      </c>
+      <c r="F48" s="209">
+        <f>'EB2018'!AI3*Conversions!$C$2</f>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="G48" s="78">
+        <f>F48</f>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="H48" s="78">
+        <f t="shared" ref="H48:M48" si="20">G48</f>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="I48" s="78">
+        <f t="shared" si="20"/>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="J48" s="78">
+        <f t="shared" si="20"/>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="K48" s="78">
+        <f t="shared" si="20"/>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="L48" s="78">
+        <f t="shared" si="20"/>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="M48" s="78">
+        <f t="shared" si="20"/>
+        <v>4.3613769615262452</v>
+      </c>
+      <c r="N48" s="277">
+        <v>5</v>
+      </c>
+      <c r="O48" s="89" t="s">
+        <v>471</v>
+      </c>
+      <c r="P48" s="78"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+    </row>
+    <row r="49" spans="2:18">
+      <c r="B49" s="33" t="str">
         <f>Imports_Bio!B10</f>
         <v>IE,National</v>
       </c>
-      <c r="C45" s="33" t="str">
+      <c r="C49" s="33" t="str">
         <f>Imports_Bio!C10</f>
         <v>IMPBIODST1G_S2</v>
       </c>
-      <c r="D45" s="33" t="str">
+      <c r="D49" s="33" t="str">
         <f>Imports_Bio!D10</f>
         <v>Import of Biodiesel 1st generation  - Step 2</v>
       </c>
-      <c r="E45" s="35" t="str">
+      <c r="E49" s="35" t="str">
         <f>Commodities!$C$32</f>
         <v>BIODST1G</v>
       </c>
-      <c r="F45" s="211">
+      <c r="F49" s="211">
         <v>0</v>
       </c>
-      <c r="G45" s="76">
-        <f>G44*2</f>
+      <c r="G49" s="76">
+        <f>G48*2</f>
         <v>8.7227539230524904</v>
       </c>
-      <c r="H45" s="76">
-        <f t="shared" ref="H45:M46" si="21">H44*2</f>
+      <c r="H49" s="76">
+        <f t="shared" ref="H49:M50" si="21">H48*2</f>
         <v>8.7227539230524904</v>
       </c>
-      <c r="I45" s="76">
+      <c r="I49" s="76">
         <f t="shared" si="21"/>
         <v>8.7227539230524904</v>
       </c>
-      <c r="J45" s="76">
+      <c r="J49" s="76">
         <f t="shared" si="21"/>
         <v>8.7227539230524904</v>
       </c>
-      <c r="K45" s="76">
+      <c r="K49" s="76">
         <f t="shared" si="21"/>
         <v>8.7227539230524904</v>
       </c>
-      <c r="L45" s="76">
+      <c r="L49" s="76">
         <f t="shared" si="21"/>
         <v>8.7227539230524904</v>
       </c>
-      <c r="M45" s="76">
+      <c r="M49" s="76">
         <f t="shared" si="21"/>
         <v>8.7227539230524904</v>
       </c>
-      <c r="N45" s="278">
+      <c r="N49" s="278">
         <v>5</v>
       </c>
-      <c r="O45" s="90" t="s">
+      <c r="O49" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="P45" s="76"/>
-      <c r="R45" s="42"/>
-    </row>
-    <row r="46" spans="2:23">
-      <c r="B46" s="33" t="str">
+      <c r="P49" s="76"/>
+      <c r="R49" s="42"/>
+    </row>
+    <row r="50" spans="2:18">
+      <c r="B50" s="33" t="str">
         <f>Imports_Bio!B11</f>
         <v>IE,National</v>
       </c>
-      <c r="C46" s="33" t="str">
+      <c r="C50" s="33" t="str">
         <f>Imports_Bio!C11</f>
         <v>IMPBIODST1G_S3</v>
       </c>
-      <c r="D46" s="33" t="str">
+      <c r="D50" s="33" t="str">
         <f>Imports_Bio!D11</f>
         <v>Import of Biodiesel 1st generation  - Step 3</v>
       </c>
-      <c r="E46" s="35" t="str">
+      <c r="E50" s="35" t="str">
         <f>Commodities!$C$32</f>
         <v>BIODST1G</v>
       </c>
-      <c r="F46" s="211">
+      <c r="F50" s="211">
         <v>0</v>
       </c>
-      <c r="G46" s="76">
-        <f>G45*2</f>
+      <c r="G50" s="76">
+        <f>G49*2</f>
         <v>17.445507846104981</v>
       </c>
-      <c r="H46" s="76">
+      <c r="H50" s="76">
         <f t="shared" si="21"/>
         <v>17.445507846104981</v>
       </c>
-      <c r="I46" s="76">
+      <c r="I50" s="76">
         <f t="shared" si="21"/>
         <v>17.445507846104981</v>
       </c>
-      <c r="J46" s="76">
+      <c r="J50" s="76">
         <f t="shared" si="21"/>
         <v>17.445507846104981</v>
       </c>
-      <c r="K46" s="76">
+      <c r="K50" s="76">
         <f t="shared" si="21"/>
         <v>17.445507846104981</v>
       </c>
-      <c r="L46" s="76">
+      <c r="L50" s="76">
         <f t="shared" si="21"/>
         <v>17.445507846104981</v>
       </c>
-      <c r="M46" s="76">
+      <c r="M50" s="76">
         <f t="shared" si="21"/>
         <v>17.445507846104981</v>
       </c>
-      <c r="N46" s="278">
+      <c r="N50" s="278">
         <v>5</v>
       </c>
-      <c r="O46" s="90" t="s">
+      <c r="O50" s="90" t="s">
         <v>232</v>
       </c>
-      <c r="P46" s="76"/>
-      <c r="R46" s="42"/>
-    </row>
-    <row r="47" spans="2:23">
-      <c r="B47" s="71" t="str">
+      <c r="P50" s="76"/>
+      <c r="R50" s="42"/>
+    </row>
+    <row r="51" spans="2:18">
+      <c r="B51" s="71" t="str">
         <f>"*"&amp;Imports_Bio!B12</f>
         <v>*IE,National</v>
       </c>
-      <c r="C47" s="71" t="str">
+      <c r="C51" s="71" t="str">
         <f>"*"&amp;Imports_Bio!C12</f>
         <v>*IMPBIODST1G_S4</v>
       </c>
-      <c r="D47" s="71" t="str">
+      <c r="D51" s="71" t="str">
         <f>Imports_Bio!D12</f>
         <v>Import of Biodiesel 1st generation  - Step 4</v>
       </c>
-      <c r="E47" s="65" t="str">
+      <c r="E51" s="65" t="str">
         <f>Commodities!$C$32</f>
         <v>BIODST1G</v>
       </c>
-      <c r="F47" s="213">
+      <c r="F51" s="213">
         <v>0</v>
       </c>
-      <c r="G47" s="77">
-        <f>G48-SUM(G44:G46)</f>
+      <c r="G51" s="77">
+        <f>G52-SUM(G48:G50)</f>
         <v>72.228951163880168</v>
       </c>
-      <c r="H47" s="77">
-        <f t="shared" ref="H47:M47" si="22">H48-SUM(H44:H46)</f>
+      <c r="H51" s="77">
+        <f t="shared" ref="H51:M51" si="22">H52-SUM(H48:H50)</f>
         <v>72.228951163880168</v>
       </c>
-      <c r="I47" s="77">
+      <c r="I51" s="77">
         <f t="shared" si="22"/>
         <v>72.228951163880168</v>
       </c>
-      <c r="J47" s="77">
+      <c r="J51" s="77">
         <f t="shared" si="22"/>
         <v>72.228951163880168</v>
       </c>
-      <c r="K47" s="77">
+      <c r="K51" s="77">
         <f t="shared" si="22"/>
         <v>72.228951163880168</v>
       </c>
-      <c r="L47" s="77">
+      <c r="L51" s="77">
         <f t="shared" si="22"/>
         <v>72.228951163880168</v>
       </c>
-      <c r="M47" s="77">
+      <c r="M51" s="77">
         <f t="shared" si="22"/>
         <v>72.228951163880168</v>
       </c>
-      <c r="N47" s="279">
+      <c r="N51" s="279">
         <v>5</v>
       </c>
-      <c r="O47" s="91" t="s">
+      <c r="O51" s="91" t="s">
         <v>233</v>
       </c>
-      <c r="P47" s="77"/>
-      <c r="R47" s="42"/>
-    </row>
-    <row r="48" spans="2:23" ht="15.75" thickBot="1">
-      <c r="B48" s="72" t="s">
+      <c r="P51" s="77"/>
+      <c r="R51" s="42"/>
+    </row>
+    <row r="52" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B52" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="72"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="79">
-        <f>H48</f>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="79">
+        <f>H52</f>
         <v>102.75858989456388</v>
       </c>
-      <c r="H48" s="79">
-        <f>I48</f>
+      <c r="H52" s="79">
+        <f>I52</f>
         <v>102.75858989456388</v>
       </c>
-      <c r="I48" s="79">
+      <c r="I52" s="79">
         <f>2727.05194883825*Conversions!$C$2*0.9</f>
         <v>102.75858989456388</v>
       </c>
-      <c r="J48" s="79">
-        <f>I48</f>
+      <c r="J52" s="79">
+        <f>I52</f>
         <v>102.75858989456388</v>
       </c>
-      <c r="K48" s="79">
-        <f t="shared" ref="K48:M48" si="23">J48</f>
+      <c r="K52" s="79">
+        <f t="shared" ref="K52:M52" si="23">J52</f>
         <v>102.75858989456388</v>
       </c>
-      <c r="L48" s="79">
+      <c r="L52" s="79">
         <f t="shared" si="23"/>
         <v>102.75858989456388</v>
       </c>
-      <c r="M48" s="79">
+      <c r="M52" s="79">
         <f t="shared" si="23"/>
         <v>102.75858989456388</v>
       </c>
-      <c r="N48" s="280"/>
-      <c r="O48" s="92" t="s">
+      <c r="N52" s="280"/>
+      <c r="O52" s="92" t="s">
         <v>230</v>
       </c>
-      <c r="P48" s="79"/>
-      <c r="R48" s="42"/>
-    </row>
-    <row r="49" spans="2:18">
-      <c r="B49" s="69" t="str">
+      <c r="P52" s="79"/>
+      <c r="R52" s="42"/>
+    </row>
+    <row r="53" spans="2:18">
+      <c r="B53" s="69" t="str">
         <f>Imports_Bio!B13</f>
         <v>IE,National</v>
       </c>
-      <c r="C49" s="69" t="str">
+      <c r="C53" s="69" t="str">
         <f>Imports_Bio!C13</f>
         <v>IMPBIOWPE_S1</v>
       </c>
-      <c r="D49" s="69" t="str">
+      <c r="D53" s="69" t="str">
         <f>Imports_Bio!D13</f>
         <v>Import of Wood Pellets  - Step 1</v>
       </c>
-      <c r="E49" s="34" t="str">
+      <c r="E53" s="34" t="str">
         <f>Commodities!$C$41</f>
         <v>BIOWPE</v>
       </c>
-      <c r="F49" s="209">
-        <f>'EB2018'!AE3*Conversions!$C$2*Imports_Bio!$R$49</f>
+      <c r="F53" s="209">
+        <f>'EB2018'!AE3*Conversions!$C$2*Imports_Bio!$R$53</f>
         <v>0.67902889168989577</v>
       </c>
-      <c r="G49" s="78">
-        <f>MAX(F49:F49)</f>
+      <c r="G53" s="78">
+        <f>MAX(F53:F53)</f>
         <v>0.67902889168989577</v>
       </c>
-      <c r="H49" s="78">
-        <f>G49</f>
+      <c r="H53" s="78">
+        <f>G53</f>
         <v>0.67902889168989577</v>
       </c>
-      <c r="I49" s="78">
-        <f t="shared" ref="I49:M49" si="24">H49</f>
+      <c r="I53" s="78">
+        <f t="shared" ref="I53:M53" si="24">H53</f>
         <v>0.67902889168989577</v>
       </c>
-      <c r="J49" s="78">
+      <c r="J53" s="78">
         <f t="shared" si="24"/>
         <v>0.67902889168989577</v>
       </c>
-      <c r="K49" s="78">
+      <c r="K53" s="78">
         <f t="shared" si="24"/>
         <v>0.67902889168989577</v>
       </c>
-      <c r="L49" s="78">
+      <c r="L53" s="78">
         <f t="shared" si="24"/>
         <v>0.67902889168989577</v>
       </c>
-      <c r="M49" s="78">
+      <c r="M53" s="78">
         <f t="shared" si="24"/>
         <v>0.67902889168989577</v>
       </c>
-      <c r="N49" s="277">
+      <c r="N53" s="277">
         <v>5</v>
       </c>
-      <c r="O49" s="89" t="s">
+      <c r="O53" s="89" t="s">
         <v>234</v>
       </c>
-      <c r="P49" s="78"/>
-      <c r="R49" s="210">
+      <c r="P53" s="78"/>
+      <c r="R53" s="210">
         <v>0.7</v>
       </c>
     </row>
-    <row r="50" spans="2:18">
-      <c r="B50" s="33" t="str">
+    <row r="54" spans="2:18">
+      <c r="B54" s="33" t="str">
         <f>Imports_Bio!B14</f>
         <v>IE,National</v>
       </c>
-      <c r="C50" s="33" t="str">
+      <c r="C54" s="33" t="str">
         <f>Imports_Bio!C14</f>
         <v>IMPBIOWPE_S2</v>
       </c>
-      <c r="D50" s="33" t="str">
+      <c r="D54" s="33" t="str">
         <f>Imports_Bio!D14</f>
         <v>Import of Wood Pellets  - Step 2</v>
       </c>
-      <c r="E50" s="34" t="str">
+      <c r="E54" s="34" t="str">
         <f>Commodities!$C$41</f>
         <v>BIOWPE</v>
       </c>
-      <c r="F50" s="211">
+      <c r="F54" s="211">
         <v>0</v>
       </c>
-      <c r="G50" s="76">
-        <f>G49*2</f>
+      <c r="G54" s="76">
+        <f>G53*2</f>
         <v>1.3580577833797915</v>
       </c>
-      <c r="H50" s="76">
-        <f t="shared" ref="H50:M51" si="25">H49*2</f>
+      <c r="H54" s="76">
+        <f t="shared" ref="H54:M55" si="25">H53*2</f>
         <v>1.3580577833797915</v>
       </c>
-      <c r="I50" s="76">
+      <c r="I54" s="76">
         <f t="shared" si="25"/>
         <v>1.3580577833797915</v>
       </c>
-      <c r="J50" s="76">
+      <c r="J54" s="76">
         <f t="shared" si="25"/>
         <v>1.3580577833797915</v>
       </c>
-      <c r="K50" s="76">
+      <c r="K54" s="76">
         <f t="shared" si="25"/>
         <v>1.3580577833797915</v>
       </c>
-      <c r="L50" s="76">
+      <c r="L54" s="76">
         <f t="shared" si="25"/>
         <v>1.3580577833797915</v>
       </c>
-      <c r="M50" s="76">
+      <c r="M54" s="76">
         <f t="shared" si="25"/>
         <v>1.3580577833797915</v>
       </c>
-      <c r="N50" s="278">
+      <c r="N54" s="278">
         <v>5</v>
       </c>
-      <c r="O50" s="90" t="s">
+      <c r="O54" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="P50" s="76"/>
-      <c r="R50" s="42"/>
-    </row>
-    <row r="51" spans="2:18">
-      <c r="B51" s="33" t="str">
+      <c r="P54" s="76"/>
+      <c r="R54" s="42"/>
+    </row>
+    <row r="55" spans="2:18">
+      <c r="B55" s="33" t="str">
         <f>Imports_Bio!B15</f>
         <v>IE,National</v>
       </c>
-      <c r="C51" s="33" t="str">
+      <c r="C55" s="33" t="str">
         <f>Imports_Bio!C15</f>
         <v>IMPBIOWPE_S3</v>
       </c>
-      <c r="D51" s="33" t="str">
+      <c r="D55" s="33" t="str">
         <f>Imports_Bio!D15</f>
         <v>Import of Wood Pellets  - Step 3</v>
       </c>
-      <c r="E51" s="34" t="str">
+      <c r="E55" s="34" t="str">
         <f>Commodities!$C$41</f>
         <v>BIOWPE</v>
       </c>
-      <c r="F51" s="211">
+      <c r="F55" s="211">
         <v>0</v>
       </c>
-      <c r="G51" s="76">
-        <f>G50*2</f>
+      <c r="G55" s="76">
+        <f>G54*2</f>
         <v>2.7161155667595831</v>
       </c>
-      <c r="H51" s="76">
+      <c r="H55" s="76">
         <f t="shared" si="25"/>
         <v>2.7161155667595831</v>
       </c>
-      <c r="I51" s="76">
+      <c r="I55" s="76">
         <f t="shared" si="25"/>
         <v>2.7161155667595831</v>
       </c>
-      <c r="J51" s="76">
+      <c r="J55" s="76">
         <f t="shared" si="25"/>
         <v>2.7161155667595831</v>
       </c>
-      <c r="K51" s="76">
+      <c r="K55" s="76">
         <f t="shared" si="25"/>
         <v>2.7161155667595831</v>
       </c>
-      <c r="L51" s="76">
+      <c r="L55" s="76">
         <f t="shared" si="25"/>
         <v>2.7161155667595831</v>
       </c>
-      <c r="M51" s="76">
+      <c r="M55" s="76">
         <f t="shared" si="25"/>
         <v>2.7161155667595831</v>
       </c>
-      <c r="N51" s="278">
+      <c r="N55" s="278">
         <v>5</v>
       </c>
-      <c r="O51" s="90" t="s">
+      <c r="O55" s="90" t="s">
         <v>232</v>
       </c>
-      <c r="P51" s="76"/>
-      <c r="R51" s="42"/>
-    </row>
-    <row r="52" spans="2:18">
-      <c r="B52" s="71" t="str">
+      <c r="P55" s="76"/>
+      <c r="R55" s="42"/>
+    </row>
+    <row r="56" spans="2:18">
+      <c r="B56" s="71" t="str">
         <f>"*"&amp;Imports_Bio!B16</f>
         <v>*IE,National</v>
       </c>
-      <c r="C52" s="71" t="str">
+      <c r="C56" s="71" t="str">
         <f>"*"&amp;Imports_Bio!C16</f>
         <v>*IMPBIOWPE_S4</v>
       </c>
-      <c r="D52" s="71" t="str">
+      <c r="D56" s="71" t="str">
         <f>Imports_Bio!D16</f>
         <v>Import of Wood Pellets  - Step 4</v>
       </c>
-      <c r="E52" s="65" t="str">
+      <c r="E56" s="65" t="str">
         <f>Commodities!$C$41</f>
         <v>BIOWPE</v>
       </c>
-      <c r="F52" s="213">
+      <c r="F56" s="213">
         <v>0</v>
       </c>
-      <c r="G52" s="77">
-        <f>G53-SUM(G49:G51)</f>
+      <c r="G56" s="77">
+        <f>G57-SUM(G53:G55)</f>
         <v>105.39325776217073</v>
       </c>
-      <c r="H52" s="77">
-        <f t="shared" ref="H52:M52" si="26">H53-SUM(H49:H51)</f>
+      <c r="H56" s="77">
+        <f t="shared" ref="H56:M56" si="26">H57-SUM(H53:H55)</f>
         <v>105.39325776217073</v>
       </c>
-      <c r="I52" s="77">
+      <c r="I56" s="77">
         <f t="shared" si="26"/>
         <v>105.39325776217073</v>
       </c>
-      <c r="J52" s="77">
+      <c r="J56" s="77">
         <f t="shared" si="26"/>
         <v>105.39325776217073</v>
       </c>
-      <c r="K52" s="77">
+      <c r="K56" s="77">
         <f t="shared" si="26"/>
         <v>105.39325776217073</v>
       </c>
-      <c r="L52" s="77">
+      <c r="L56" s="77">
         <f t="shared" si="26"/>
         <v>105.39325776217073</v>
       </c>
-      <c r="M52" s="77">
+      <c r="M56" s="77">
         <f t="shared" si="26"/>
         <v>105.39325776217073</v>
       </c>
-      <c r="N52" s="279">
+      <c r="N56" s="279">
         <v>5</v>
       </c>
-      <c r="O52" s="91" t="s">
+      <c r="O56" s="91" t="s">
         <v>233</v>
       </c>
-      <c r="P52" s="77"/>
-      <c r="R52" s="42"/>
-    </row>
-    <row r="53" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B53" s="72" t="s">
+      <c r="P56" s="77"/>
+      <c r="R56" s="42"/>
+    </row>
+    <row r="57" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B57" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79">
-        <f>H53</f>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="79"/>
+      <c r="G57" s="79">
+        <f>H57</f>
         <v>110.14646000400001</v>
       </c>
-      <c r="H53" s="79">
-        <f>I53</f>
+      <c r="H57" s="79">
+        <f>I57</f>
         <v>110.14646000400001</v>
       </c>
-      <c r="I53" s="79">
+      <c r="I57" s="79">
         <f>'SEAI-AEA_BioData'!G52*Conversions!$C$2/1000</f>
         <v>110.14646000400001</v>
       </c>
-      <c r="J53" s="79">
-        <f>I53</f>
+      <c r="J57" s="79">
+        <f>I57</f>
         <v>110.14646000400001</v>
       </c>
-      <c r="K53" s="79">
-        <f t="shared" ref="K53:M53" si="27">J53</f>
+      <c r="K57" s="79">
+        <f t="shared" ref="K57:M57" si="27">J57</f>
         <v>110.14646000400001</v>
       </c>
-      <c r="L53" s="79">
+      <c r="L57" s="79">
         <f t="shared" si="27"/>
         <v>110.14646000400001</v>
       </c>
-      <c r="M53" s="79">
+      <c r="M57" s="79">
         <f t="shared" si="27"/>
         <v>110.14646000400001</v>
       </c>
-      <c r="N53" s="280"/>
-      <c r="O53" s="92" t="s">
+      <c r="N57" s="280"/>
+      <c r="O57" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="P53" s="79"/>
-      <c r="R53" s="42"/>
-    </row>
-    <row r="54" spans="2:18">
-      <c r="B54" s="69" t="str">
+      <c r="P57" s="79"/>
+      <c r="R57" s="42"/>
+    </row>
+    <row r="58" spans="2:18">
+      <c r="B58" s="69" t="str">
         <f>Imports_Bio!B17</f>
         <v>IE,National</v>
       </c>
-      <c r="C54" s="69" t="str">
+      <c r="C58" s="69" t="str">
         <f>Imports_Bio!C17</f>
         <v>IMPBIOWCH_S1</v>
       </c>
-      <c r="D54" s="69" t="str">
+      <c r="D58" s="69" t="str">
         <f>Imports_Bio!D17</f>
         <v>Import of Wood Chip  - Step 1</v>
       </c>
-      <c r="E54" s="70" t="str">
+      <c r="E58" s="70" t="str">
         <f>Commodities!$C$42</f>
         <v>BIOWCH</v>
       </c>
-      <c r="F54" s="209">
-        <f>'EB2018'!AE3*Conversions!$C$2*Imports_Bio!$R$54</f>
+      <c r="F58" s="209">
+        <f>'EB2018'!AE3*Conversions!$C$2*Imports_Bio!$R$58</f>
         <v>0.29101238215281255</v>
       </c>
-      <c r="G54" s="78">
-        <f>MAX(F54:F54)</f>
+      <c r="G58" s="78">
+        <f>MAX(F58:F58)</f>
         <v>0.29101238215281255</v>
       </c>
-      <c r="H54" s="78">
-        <f>G54</f>
+      <c r="H58" s="78">
+        <f>G58</f>
         <v>0.29101238215281255</v>
       </c>
-      <c r="I54" s="78">
-        <f t="shared" ref="I54:M54" si="28">H54</f>
+      <c r="I58" s="78">
+        <f t="shared" ref="I58:M58" si="28">H58</f>
         <v>0.29101238215281255</v>
       </c>
-      <c r="J54" s="78">
+      <c r="J58" s="78">
         <f t="shared" si="28"/>
         <v>0.29101238215281255</v>
       </c>
-      <c r="K54" s="78">
+      <c r="K58" s="78">
         <f t="shared" si="28"/>
         <v>0.29101238215281255</v>
       </c>
-      <c r="L54" s="78">
+      <c r="L58" s="78">
         <f t="shared" si="28"/>
         <v>0.29101238215281255</v>
       </c>
-      <c r="M54" s="78">
+      <c r="M58" s="78">
         <f t="shared" si="28"/>
         <v>0.29101238215281255</v>
       </c>
-      <c r="N54" s="277">
+      <c r="N58" s="277">
         <v>5</v>
       </c>
-      <c r="O54" s="89" t="s">
+      <c r="O58" s="89" t="s">
         <v>234</v>
       </c>
-      <c r="P54" s="78"/>
-      <c r="R54" s="208">
-        <f>1-R49</f>
+      <c r="P58" s="78"/>
+      <c r="R58" s="208">
+        <f>1-R53</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="55" spans="2:18">
-      <c r="B55" s="33" t="str">
+    <row r="59" spans="2:18">
+      <c r="B59" s="33" t="str">
         <f>Imports_Bio!B18</f>
         <v>IE,National</v>
       </c>
-      <c r="C55" s="33" t="str">
+      <c r="C59" s="33" t="str">
         <f>Imports_Bio!C18</f>
         <v>IMPBIOWCH_S2</v>
       </c>
-      <c r="D55" s="33" t="str">
+      <c r="D59" s="33" t="str">
         <f>Imports_Bio!D18</f>
         <v>Import of Wood Chip  - Step 2</v>
       </c>
-      <c r="E55" s="35" t="str">
+      <c r="E59" s="35" t="str">
         <f>Commodities!$C$42</f>
         <v>BIOWCH</v>
       </c>
-      <c r="F55" s="211">
+      <c r="F59" s="211">
         <v>0</v>
       </c>
-      <c r="G55" s="76">
-        <f>G54*2</f>
+      <c r="G59" s="76">
+        <f>G58*2</f>
         <v>0.58202476430562511</v>
       </c>
-      <c r="H55" s="76">
-        <f t="shared" ref="H55:M56" si="29">H54*2</f>
+      <c r="H59" s="76">
+        <f t="shared" ref="H59:M60" si="29">H58*2</f>
         <v>0.58202476430562511</v>
       </c>
-      <c r="I55" s="76">
+      <c r="I59" s="76">
         <f t="shared" si="29"/>
         <v>0.58202476430562511</v>
       </c>
-      <c r="J55" s="76">
+      <c r="J59" s="76">
         <f t="shared" si="29"/>
         <v>0.58202476430562511</v>
       </c>
-      <c r="K55" s="76">
+      <c r="K59" s="76">
         <f t="shared" si="29"/>
         <v>0.58202476430562511</v>
       </c>
-      <c r="L55" s="76">
+      <c r="L59" s="76">
         <f t="shared" si="29"/>
         <v>0.58202476430562511</v>
       </c>
-      <c r="M55" s="76">
+      <c r="M59" s="76">
         <f t="shared" si="29"/>
         <v>0.58202476430562511</v>
       </c>
-      <c r="N55" s="278">
+      <c r="N59" s="278">
         <v>5</v>
       </c>
-      <c r="O55" s="90" t="s">
+      <c r="O59" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="P55" s="76"/>
-      <c r="R55" s="42"/>
-    </row>
-    <row r="56" spans="2:18">
-      <c r="B56" s="33" t="str">
+      <c r="P59" s="76"/>
+      <c r="R59" s="42"/>
+    </row>
+    <row r="60" spans="2:18">
+      <c r="B60" s="33" t="str">
         <f>Imports_Bio!B19</f>
         <v>IE,National</v>
       </c>
-      <c r="C56" s="33" t="str">
+      <c r="C60" s="33" t="str">
         <f>Imports_Bio!C19</f>
         <v>IMPBIOWCH_S3</v>
       </c>
-      <c r="D56" s="33" t="str">
+      <c r="D60" s="33" t="str">
         <f>Imports_Bio!D19</f>
         <v>Import of Wood Chip  - Step 3</v>
       </c>
-      <c r="E56" s="35" t="str">
+      <c r="E60" s="35" t="str">
         <f>Commodities!$C$42</f>
         <v>BIOWCH</v>
       </c>
-      <c r="F56" s="211">
+      <c r="F60" s="211">
         <v>0</v>
       </c>
-      <c r="G56" s="76">
-        <f>G55*2</f>
+      <c r="G60" s="76">
+        <f>G59*2</f>
         <v>1.1640495286112502</v>
       </c>
-      <c r="H56" s="76">
+      <c r="H60" s="76">
         <f t="shared" si="29"/>
         <v>1.1640495286112502</v>
       </c>
-      <c r="I56" s="76">
+      <c r="I60" s="76">
         <f t="shared" si="29"/>
         <v>1.1640495286112502</v>
       </c>
-      <c r="J56" s="76">
+      <c r="J60" s="76">
         <f t="shared" si="29"/>
         <v>1.1640495286112502</v>
       </c>
-      <c r="K56" s="76">
+      <c r="K60" s="76">
         <f t="shared" si="29"/>
         <v>1.1640495286112502</v>
       </c>
-      <c r="L56" s="76">
+      <c r="L60" s="76">
         <f t="shared" si="29"/>
         <v>1.1640495286112502</v>
       </c>
-      <c r="M56" s="76">
+      <c r="M60" s="76">
         <f t="shared" si="29"/>
         <v>1.1640495286112502</v>
       </c>
-      <c r="N56" s="278">
+      <c r="N60" s="278">
         <v>5</v>
       </c>
-      <c r="O56" s="90" t="s">
+      <c r="O60" s="90" t="s">
         <v>232</v>
       </c>
-      <c r="P56" s="76"/>
-      <c r="R56" s="42"/>
-    </row>
-    <row r="57" spans="2:18">
-      <c r="B57" s="71" t="str">
+      <c r="P60" s="76"/>
+      <c r="R60" s="42"/>
+    </row>
+    <row r="61" spans="2:18">
+      <c r="B61" s="71" t="str">
         <f>"*"&amp;Imports_Bio!B20</f>
         <v>*IE,National</v>
       </c>
-      <c r="C57" s="71" t="str">
+      <c r="C61" s="71" t="str">
         <f>"*"&amp;Imports_Bio!C20</f>
         <v>*IMPBIOWCH_S4</v>
       </c>
-      <c r="D57" s="71" t="str">
+      <c r="D61" s="71" t="str">
         <f>Imports_Bio!D20</f>
         <v>Import of Wood Chip  - Step 4</v>
       </c>
-      <c r="E57" s="65" t="str">
+      <c r="E61" s="65" t="str">
         <f>Commodities!$C$42</f>
         <v>BIOWCH</v>
       </c>
-      <c r="F57" s="213">
+      <c r="F61" s="213">
         <v>0</v>
       </c>
-      <c r="G57" s="77">
-        <f>G58-SUM(G54:G56)</f>
+      <c r="G61" s="77">
+        <f>G62-SUM(G58:G60)</f>
         <v>34.678386036930313</v>
       </c>
-      <c r="H57" s="77">
-        <f t="shared" ref="H57:M57" si="30">H58-SUM(H54:H56)</f>
+      <c r="H61" s="77">
+        <f t="shared" ref="H61:M61" si="30">H62-SUM(H58:H60)</f>
         <v>34.678386036930313</v>
       </c>
-      <c r="I57" s="77">
+      <c r="I61" s="77">
         <f t="shared" si="30"/>
         <v>34.678386036930313</v>
       </c>
-      <c r="J57" s="77">
+      <c r="J61" s="77">
         <f t="shared" si="30"/>
         <v>34.678386036930313</v>
       </c>
-      <c r="K57" s="77">
+      <c r="K61" s="77">
         <f t="shared" si="30"/>
         <v>34.678386036930313</v>
       </c>
-      <c r="L57" s="77">
+      <c r="L61" s="77">
         <f t="shared" si="30"/>
         <v>34.678386036930313</v>
       </c>
-      <c r="M57" s="77">
+      <c r="M61" s="77">
         <f t="shared" si="30"/>
         <v>34.678386036930313</v>
       </c>
-      <c r="N57" s="279">
+      <c r="N61" s="279">
         <v>5</v>
       </c>
-      <c r="O57" s="91" t="s">
+      <c r="O61" s="91" t="s">
         <v>233</v>
       </c>
-      <c r="P57" s="77"/>
-      <c r="R57" s="42"/>
-    </row>
-    <row r="58" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B58" s="74" t="s">
+      <c r="P61" s="77"/>
+      <c r="R61" s="42"/>
+    </row>
+    <row r="62" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B62" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="80"/>
-      <c r="G58" s="80">
-        <f>H58</f>
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="75"/>
+      <c r="F62" s="80"/>
+      <c r="G62" s="80">
+        <f>H62</f>
         <v>36.715472712</v>
       </c>
-      <c r="H58" s="80">
-        <f>I58</f>
+      <c r="H62" s="80">
+        <f>I62</f>
         <v>36.715472712</v>
       </c>
-      <c r="I58" s="80">
+      <c r="I62" s="80">
         <f>'SEAI-AEA_BioData'!G50*Conversions!$C$2/1000</f>
         <v>36.715472712</v>
       </c>
-      <c r="J58" s="80">
-        <f>I58</f>
+      <c r="J62" s="80">
+        <f>I62</f>
         <v>36.715472712</v>
       </c>
-      <c r="K58" s="80">
-        <f>J58</f>
+      <c r="K62" s="80">
+        <f>J62</f>
         <v>36.715472712</v>
       </c>
-      <c r="L58" s="80">
-        <f>K58</f>
+      <c r="L62" s="80">
+        <f>K62</f>
         <v>36.715472712</v>
       </c>
-      <c r="M58" s="80">
-        <f>L58</f>
+      <c r="M62" s="80">
+        <f>L62</f>
         <v>36.715472712</v>
       </c>
-      <c r="N58" s="281"/>
-      <c r="O58" s="93" t="s">
+      <c r="N62" s="281"/>
+      <c r="O62" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="P58" s="80"/>
-      <c r="R58" s="42"/>
+      <c r="P62" s="80"/>
+      <c r="R62" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K26:K33"/>
+    <mergeCell ref="K30:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29556,11 +29681,11 @@
       <c r="C9" s="52"/>
       <c r="D9" s="52"/>
       <c r="E9" s="52"/>
-      <c r="F9" s="502" t="s">
+      <c r="F9" s="503" t="s">
         <v>239</v>
       </c>
-      <c r="G9" s="502"/>
-      <c r="H9" s="502"/>
+      <c r="G9" s="503"/>
+      <c r="H9" s="503"/>
       <c r="I9" s="273" t="s">
         <v>238</v>
       </c>

</xml_diff>